<commit_message>
Corrected Burn Down Chart... Part 2
</commit_message>
<xml_diff>
--- a/Burn Down Chart.xlsx
+++ b/Burn Down Chart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10780" windowHeight="15320" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25360" windowHeight="15320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 1" sheetId="1" r:id="rId1"/>
@@ -540,6 +540,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -552,7 +585,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -561,50 +594,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -779,23 +779,23 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="300392344"/>
-        <c:axId val="300395384"/>
+        <c:axId val="468494680"/>
+        <c:axId val="467886648"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="300392344"/>
+        <c:axId val="468494680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="300395384"/>
+        <c:crossAx val="467886648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="300395384"/>
+        <c:axId val="467886648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -803,7 +803,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="300392344"/>
+        <c:crossAx val="468494680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1180,22 +1180,22 @@
   <dimension ref="A1:AZ51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AZ21" sqref="AZ21"/>
+      <selection activeCell="X28" sqref="X28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.140625" defaultRowHeight="13"/>
   <sheetData>
     <row r="1" spans="1:16">
-      <c r="A1" s="17"/>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="A1" s="32"/>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -1510,82 +1510,82 @@
       <c r="P18" s="1"/>
     </row>
     <row r="19" spans="1:52" ht="14" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="19"/>
-      <c r="C19" s="19"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
-      <c r="L19" s="19"/>
-      <c r="M19" s="19" t="s">
+      <c r="B19" s="34"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
+      <c r="K19" s="34"/>
+      <c r="L19" s="34"/>
+      <c r="M19" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="N19" s="19"/>
-      <c r="O19" s="19"/>
-      <c r="P19" s="19"/>
-      <c r="Q19" s="28" t="s">
+      <c r="N19" s="34"/>
+      <c r="O19" s="34"/>
+      <c r="P19" s="34"/>
+      <c r="Q19" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="R19" s="29"/>
-      <c r="S19" s="29"/>
-      <c r="T19" s="29"/>
-      <c r="U19" s="29"/>
-      <c r="V19" s="29"/>
-      <c r="W19" s="29"/>
-      <c r="X19" s="29"/>
-      <c r="Y19" s="29"/>
-      <c r="Z19" s="29"/>
-      <c r="AA19" s="29"/>
-      <c r="AB19" s="29"/>
-      <c r="AC19" s="29"/>
-      <c r="AD19" s="29"/>
-      <c r="AE19" s="29"/>
-      <c r="AF19" s="29"/>
-      <c r="AG19" s="29"/>
-      <c r="AH19" s="29"/>
-      <c r="AI19" s="29"/>
-      <c r="AJ19" s="29"/>
-      <c r="AK19" s="29"/>
-      <c r="AL19" s="29"/>
-      <c r="AM19" s="29"/>
-      <c r="AN19" s="29"/>
-      <c r="AO19" s="29"/>
-      <c r="AP19" s="29"/>
-      <c r="AQ19" s="29"/>
-      <c r="AR19" s="29"/>
-      <c r="AS19" s="29"/>
-      <c r="AT19" s="29"/>
-      <c r="AU19" s="29"/>
-      <c r="AV19" s="29"/>
-      <c r="AW19" s="29"/>
-      <c r="AX19" s="29"/>
-      <c r="AY19" s="29"/>
-      <c r="AZ19" s="30"/>
+      <c r="R19" s="23"/>
+      <c r="S19" s="23"/>
+      <c r="T19" s="23"/>
+      <c r="U19" s="23"/>
+      <c r="V19" s="23"/>
+      <c r="W19" s="23"/>
+      <c r="X19" s="23"/>
+      <c r="Y19" s="23"/>
+      <c r="Z19" s="23"/>
+      <c r="AA19" s="23"/>
+      <c r="AB19" s="23"/>
+      <c r="AC19" s="23"/>
+      <c r="AD19" s="23"/>
+      <c r="AE19" s="23"/>
+      <c r="AF19" s="23"/>
+      <c r="AG19" s="23"/>
+      <c r="AH19" s="23"/>
+      <c r="AI19" s="23"/>
+      <c r="AJ19" s="23"/>
+      <c r="AK19" s="23"/>
+      <c r="AL19" s="23"/>
+      <c r="AM19" s="23"/>
+      <c r="AN19" s="23"/>
+      <c r="AO19" s="23"/>
+      <c r="AP19" s="23"/>
+      <c r="AQ19" s="23"/>
+      <c r="AR19" s="23"/>
+      <c r="AS19" s="23"/>
+      <c r="AT19" s="23"/>
+      <c r="AU19" s="23"/>
+      <c r="AV19" s="23"/>
+      <c r="AW19" s="23"/>
+      <c r="AX19" s="23"/>
+      <c r="AY19" s="23"/>
+      <c r="AZ19" s="24"/>
     </row>
     <row r="20" spans="1:52">
-      <c r="A20" s="23"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
-      <c r="L20" s="20"/>
-      <c r="M20" s="20"/>
-      <c r="N20" s="20"/>
-      <c r="O20" s="20"/>
-      <c r="P20" s="20"/>
+      <c r="A20" s="38"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="35"/>
+      <c r="I20" s="35"/>
+      <c r="J20" s="35"/>
+      <c r="K20" s="35"/>
+      <c r="L20" s="35"/>
+      <c r="M20" s="35"/>
+      <c r="N20" s="35"/>
+      <c r="O20" s="35"/>
+      <c r="P20" s="35"/>
       <c r="Q20" s="3">
         <v>0</v>
       </c>
@@ -1631,163 +1631,163 @@
       <c r="AE20" s="4">
         <v>14</v>
       </c>
-      <c r="AF20" s="36">
+      <c r="AF20" s="19">
         <v>15</v>
       </c>
-      <c r="AG20" s="36">
+      <c r="AG20" s="19">
         <v>16</v>
       </c>
-      <c r="AH20" s="36">
+      <c r="AH20" s="19">
         <v>17</v>
       </c>
-      <c r="AI20" s="36">
+      <c r="AI20" s="19">
         <v>18</v>
       </c>
-      <c r="AJ20" s="36">
+      <c r="AJ20" s="19">
         <v>19</v>
       </c>
-      <c r="AK20" s="36">
+      <c r="AK20" s="19">
         <v>20</v>
       </c>
-      <c r="AL20" s="36">
+      <c r="AL20" s="19">
         <v>21</v>
       </c>
-      <c r="AM20" s="36">
+      <c r="AM20" s="19">
         <v>22</v>
       </c>
-      <c r="AN20" s="36">
+      <c r="AN20" s="19">
         <v>23</v>
       </c>
-      <c r="AO20" s="36">
+      <c r="AO20" s="19">
         <v>24</v>
       </c>
-      <c r="AP20" s="36">
+      <c r="AP20" s="19">
         <v>25</v>
       </c>
-      <c r="AQ20" s="36">
+      <c r="AQ20" s="19">
         <v>26</v>
       </c>
-      <c r="AR20" s="36">
+      <c r="AR20" s="19">
         <v>27</v>
       </c>
-      <c r="AS20" s="36">
+      <c r="AS20" s="19">
         <v>28</v>
       </c>
-      <c r="AT20" s="36">
+      <c r="AT20" s="19">
         <v>29</v>
       </c>
-      <c r="AU20" s="36">
+      <c r="AU20" s="19">
         <v>30</v>
       </c>
-      <c r="AV20" s="36">
+      <c r="AV20" s="19">
         <v>31</v>
       </c>
-      <c r="AW20" s="36">
+      <c r="AW20" s="19">
         <v>32</v>
       </c>
-      <c r="AX20" s="36">
+      <c r="AX20" s="19">
         <v>33</v>
       </c>
-      <c r="AY20" s="36">
+      <c r="AY20" s="19">
         <v>34</v>
       </c>
-      <c r="AZ20" s="37">
+      <c r="AZ20" s="20">
         <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:52" ht="14" thickBot="1">
-      <c r="A21" s="32"/>
-      <c r="B21" s="33"/>
-      <c r="C21" s="33"/>
-      <c r="D21" s="33"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
-      <c r="I21" s="33"/>
-      <c r="J21" s="33"/>
-      <c r="K21" s="33"/>
-      <c r="L21" s="33"/>
-      <c r="M21" s="33"/>
-      <c r="N21" s="33"/>
-      <c r="O21" s="33"/>
-      <c r="P21" s="33"/>
-      <c r="Q21" s="34">
-        <f>SUM(Q22:Q51)</f>
+      <c r="A21" s="39"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="36"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="36"/>
+      <c r="H21" s="36"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="36"/>
+      <c r="K21" s="36"/>
+      <c r="L21" s="36"/>
+      <c r="M21" s="36"/>
+      <c r="N21" s="36"/>
+      <c r="O21" s="36"/>
+      <c r="P21" s="36"/>
+      <c r="Q21" s="17">
+        <f t="shared" ref="Q21:W21" si="0">SUM(Q22:Q51)</f>
         <v>54</v>
       </c>
-      <c r="R21" s="35">
-        <f>SUM(R22:R51)</f>
+      <c r="R21" s="18">
+        <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="S21" s="35">
-        <f>SUM(S22:S51)</f>
+      <c r="S21" s="18">
+        <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="T21" s="35">
-        <f>SUM(T22:T51)</f>
+      <c r="T21" s="18">
+        <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="U21" s="35">
-        <f>SUM(U22:U51)</f>
+      <c r="U21" s="18">
+        <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="V21" s="35">
-        <f>SUM(V22:V51)</f>
+      <c r="V21" s="18">
+        <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="W21" s="35">
-        <f>SUM(W22:W51)</f>
+      <c r="W21" s="18">
+        <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="X21" s="35">
-        <f t="shared" ref="R21:AZ21" si="0">SUM(X22:X51)</f>
+      <c r="X21" s="18">
+        <f t="shared" ref="X21" si="1">SUM(X22:X51)</f>
         <v>26</v>
       </c>
-      <c r="Y21" s="35"/>
-      <c r="Z21" s="35"/>
-      <c r="AA21" s="35"/>
-      <c r="AB21" s="35"/>
-      <c r="AC21" s="35"/>
-      <c r="AD21" s="35"/>
-      <c r="AE21" s="35"/>
-      <c r="AF21" s="35"/>
-      <c r="AG21" s="35"/>
-      <c r="AH21" s="35"/>
-      <c r="AI21" s="35"/>
-      <c r="AJ21" s="35"/>
-      <c r="AK21" s="35"/>
-      <c r="AL21" s="35"/>
-      <c r="AM21" s="35"/>
-      <c r="AN21" s="35"/>
-      <c r="AO21" s="35"/>
-      <c r="AP21" s="35"/>
-      <c r="AQ21" s="35"/>
-      <c r="AR21" s="35"/>
-      <c r="AS21" s="35"/>
-      <c r="AT21" s="35"/>
-      <c r="AU21" s="35"/>
-      <c r="AV21" s="35"/>
-      <c r="AW21" s="35"/>
-      <c r="AX21" s="35"/>
-      <c r="AY21" s="35"/>
-      <c r="AZ21" s="38"/>
+      <c r="Y21" s="18"/>
+      <c r="Z21" s="18"/>
+      <c r="AA21" s="18"/>
+      <c r="AB21" s="18"/>
+      <c r="AC21" s="18"/>
+      <c r="AD21" s="18"/>
+      <c r="AE21" s="18"/>
+      <c r="AF21" s="18"/>
+      <c r="AG21" s="18"/>
+      <c r="AH21" s="18"/>
+      <c r="AI21" s="18"/>
+      <c r="AJ21" s="18"/>
+      <c r="AK21" s="18"/>
+      <c r="AL21" s="18"/>
+      <c r="AM21" s="18"/>
+      <c r="AN21" s="18"/>
+      <c r="AO21" s="18"/>
+      <c r="AP21" s="18"/>
+      <c r="AQ21" s="18"/>
+      <c r="AR21" s="18"/>
+      <c r="AS21" s="18"/>
+      <c r="AT21" s="18"/>
+      <c r="AU21" s="18"/>
+      <c r="AV21" s="18"/>
+      <c r="AW21" s="18"/>
+      <c r="AX21" s="18"/>
+      <c r="AY21" s="18"/>
+      <c r="AZ21" s="21"/>
     </row>
     <row r="22" spans="1:52" ht="14" thickTop="1">
-      <c r="A22" s="39" t="s">
+      <c r="A22" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="39"/>
-      <c r="C22" s="39"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="39"/>
-      <c r="F22" s="39"/>
-      <c r="G22" s="39"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="39"/>
-      <c r="J22" s="39"/>
-      <c r="K22" s="39"/>
-      <c r="L22" s="39"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="29"/>
+      <c r="L22" s="29"/>
       <c r="M22" s="26" t="s">
         <v>1</v>
       </c>
@@ -1824,20 +1824,20 @@
       <c r="AH22" s="8"/>
     </row>
     <row r="23" spans="1:52" ht="14" thickTop="1">
-      <c r="A23" s="39" t="s">
+      <c r="A23" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="39"/>
-      <c r="C23" s="39"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="39"/>
-      <c r="F23" s="39"/>
-      <c r="G23" s="39"/>
-      <c r="H23" s="39"/>
-      <c r="I23" s="39"/>
-      <c r="J23" s="39"/>
-      <c r="K23" s="39"/>
-      <c r="L23" s="39"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="29"/>
+      <c r="K23" s="29"/>
+      <c r="L23" s="29"/>
       <c r="M23" s="26" t="s">
         <v>1</v>
       </c>
@@ -1871,20 +1871,20 @@
       <c r="AE23" s="8"/>
     </row>
     <row r="24" spans="1:52" ht="14" thickTop="1">
-      <c r="A24" s="39" t="s">
+      <c r="A24" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="39"/>
-      <c r="C24" s="39"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="39"/>
-      <c r="F24" s="39"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="39"/>
-      <c r="I24" s="39"/>
-      <c r="J24" s="39"/>
-      <c r="K24" s="39"/>
-      <c r="L24" s="39"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="29"/>
+      <c r="L24" s="29"/>
       <c r="M24" s="26" t="s">
         <v>16</v>
       </c>
@@ -1918,20 +1918,20 @@
       <c r="AE24" s="8"/>
     </row>
     <row r="25" spans="1:52" ht="14" thickTop="1">
-      <c r="A25" s="39" t="s">
+      <c r="A25" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="39"/>
-      <c r="C25" s="39"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="39"/>
-      <c r="F25" s="39"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="39"/>
-      <c r="I25" s="39"/>
-      <c r="J25" s="39"/>
-      <c r="K25" s="39"/>
-      <c r="L25" s="39"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="29"/>
+      <c r="K25" s="29"/>
+      <c r="L25" s="29"/>
       <c r="M25" s="26" t="s">
         <v>14</v>
       </c>
@@ -1959,23 +1959,26 @@
       <c r="W25" s="13">
         <v>1</v>
       </c>
+      <c r="X25" s="13">
+        <v>0</v>
+      </c>
       <c r="AE25" s="8"/>
     </row>
     <row r="26" spans="1:52" ht="14" thickTop="1">
-      <c r="A26" s="39" t="s">
+      <c r="A26" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="39"/>
-      <c r="C26" s="39"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="39"/>
-      <c r="I26" s="39"/>
-      <c r="J26" s="39"/>
-      <c r="K26" s="39"/>
-      <c r="L26" s="39"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="29"/>
+      <c r="L26" s="29"/>
       <c r="M26" s="26" t="s">
         <v>14</v>
       </c>
@@ -2003,23 +2006,26 @@
       <c r="W26" s="13">
         <v>1</v>
       </c>
+      <c r="X26" s="13">
+        <v>0</v>
+      </c>
       <c r="AE26" s="8"/>
     </row>
     <row r="27" spans="1:52" ht="14" thickTop="1">
-      <c r="A27" s="39" t="s">
+      <c r="A27" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="39"/>
-      <c r="C27" s="39"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="39"/>
-      <c r="F27" s="39"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="39"/>
-      <c r="I27" s="39"/>
-      <c r="J27" s="39"/>
-      <c r="K27" s="39"/>
-      <c r="L27" s="39"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="29"/>
+      <c r="K27" s="29"/>
+      <c r="L27" s="29"/>
       <c r="M27" s="26" t="s">
         <v>14</v>
       </c>
@@ -2047,23 +2053,26 @@
       <c r="W27" s="13">
         <v>1</v>
       </c>
+      <c r="X27" s="13">
+        <v>0</v>
+      </c>
       <c r="AE27" s="8"/>
     </row>
     <row r="28" spans="1:52">
-      <c r="A28" s="39" t="s">
+      <c r="A28" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="39"/>
-      <c r="C28" s="39"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="39"/>
-      <c r="I28" s="39"/>
-      <c r="J28" s="39"/>
-      <c r="K28" s="39"/>
-      <c r="L28" s="39"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
+      <c r="K28" s="29"/>
+      <c r="L28" s="29"/>
       <c r="M28" s="26" t="s">
         <v>15</v>
       </c>
@@ -2097,24 +2106,24 @@
       <c r="AE28" s="8"/>
     </row>
     <row r="29" spans="1:52">
-      <c r="A29" s="40" t="s">
+      <c r="A29" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="40"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="40"/>
-      <c r="F29" s="40"/>
-      <c r="G29" s="40"/>
-      <c r="H29" s="40"/>
-      <c r="I29" s="40"/>
-      <c r="J29" s="40"/>
-      <c r="K29" s="40"/>
-      <c r="L29" s="40"/>
-      <c r="M29" s="31"/>
-      <c r="N29" s="31"/>
-      <c r="O29" s="31"/>
-      <c r="P29" s="31"/>
+      <c r="B29" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
+      <c r="J29" s="27"/>
+      <c r="K29" s="27"/>
+      <c r="L29" s="27"/>
+      <c r="M29" s="28"/>
+      <c r="N29" s="28"/>
+      <c r="O29" s="28"/>
+      <c r="P29" s="28"/>
       <c r="Q29" s="13">
         <v>2</v>
       </c>
@@ -2148,20 +2157,20 @@
       <c r="AE29" s="8"/>
     </row>
     <row r="30" spans="1:52">
-      <c r="A30" s="41" t="s">
+      <c r="A30" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="41"/>
-      <c r="C30" s="41"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="41"/>
-      <c r="F30" s="41"/>
-      <c r="G30" s="41"/>
-      <c r="H30" s="41"/>
-      <c r="I30" s="41"/>
-      <c r="J30" s="41"/>
-      <c r="K30" s="41"/>
-      <c r="L30" s="41"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
+      <c r="I30" s="31"/>
+      <c r="J30" s="31"/>
+      <c r="K30" s="31"/>
+      <c r="L30" s="31"/>
       <c r="M30" s="26"/>
       <c r="N30" s="26"/>
       <c r="O30" s="26"/>
@@ -2199,20 +2208,20 @@
       <c r="AE30" s="8"/>
     </row>
     <row r="31" spans="1:52">
-      <c r="A31" s="41" t="s">
+      <c r="A31" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="41"/>
-      <c r="C31" s="41"/>
-      <c r="D31" s="41"/>
-      <c r="E31" s="41"/>
-      <c r="F31" s="41"/>
-      <c r="G31" s="41"/>
-      <c r="H31" s="41"/>
-      <c r="I31" s="41"/>
-      <c r="J31" s="41"/>
-      <c r="K31" s="41"/>
-      <c r="L31" s="41"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="31"/>
+      <c r="J31" s="31"/>
+      <c r="K31" s="31"/>
+      <c r="L31" s="31"/>
       <c r="M31" s="26"/>
       <c r="N31" s="26"/>
       <c r="O31" s="26"/>
@@ -2250,20 +2259,20 @@
       <c r="AE31" s="8"/>
     </row>
     <row r="32" spans="1:52">
-      <c r="A32" s="41" t="s">
+      <c r="A32" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="B32" s="41"/>
-      <c r="C32" s="41"/>
-      <c r="D32" s="41"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="41"/>
-      <c r="G32" s="41"/>
-      <c r="H32" s="41"/>
-      <c r="I32" s="41"/>
-      <c r="J32" s="41"/>
-      <c r="K32" s="41"/>
-      <c r="L32" s="41"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="31"/>
+      <c r="H32" s="31"/>
+      <c r="I32" s="31"/>
+      <c r="J32" s="31"/>
+      <c r="K32" s="31"/>
+      <c r="L32" s="31"/>
       <c r="M32" s="26"/>
       <c r="N32" s="26"/>
       <c r="O32" s="26"/>
@@ -2301,20 +2310,20 @@
       <c r="AE32" s="8"/>
     </row>
     <row r="33" spans="1:31">
-      <c r="A33" s="41" t="s">
+      <c r="A33" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="B33" s="41"/>
-      <c r="C33" s="41"/>
-      <c r="D33" s="41"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="41"/>
-      <c r="G33" s="41"/>
-      <c r="H33" s="41"/>
-      <c r="I33" s="41"/>
-      <c r="J33" s="41"/>
-      <c r="K33" s="41"/>
-      <c r="L33" s="41"/>
+      <c r="B33" s="31"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="31"/>
+      <c r="H33" s="31"/>
+      <c r="I33" s="31"/>
+      <c r="J33" s="31"/>
+      <c r="K33" s="31"/>
+      <c r="L33" s="31"/>
       <c r="M33" s="26"/>
       <c r="N33" s="26"/>
       <c r="O33" s="26"/>
@@ -2352,20 +2361,20 @@
       <c r="AE33" s="8"/>
     </row>
     <row r="34" spans="1:31">
-      <c r="A34" s="41" t="s">
+      <c r="A34" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="B34" s="41"/>
-      <c r="C34" s="41"/>
-      <c r="D34" s="41"/>
-      <c r="E34" s="41"/>
-      <c r="F34" s="41"/>
-      <c r="G34" s="41"/>
-      <c r="H34" s="41"/>
-      <c r="I34" s="41"/>
-      <c r="J34" s="41"/>
-      <c r="K34" s="41"/>
-      <c r="L34" s="41"/>
+      <c r="B34" s="31"/>
+      <c r="C34" s="31"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="31"/>
+      <c r="G34" s="31"/>
+      <c r="H34" s="31"/>
+      <c r="I34" s="31"/>
+      <c r="J34" s="31"/>
+      <c r="K34" s="31"/>
+      <c r="L34" s="31"/>
       <c r="M34" s="26"/>
       <c r="N34" s="26"/>
       <c r="O34" s="26"/>
@@ -2403,20 +2412,20 @@
       <c r="AE34" s="8"/>
     </row>
     <row r="35" spans="1:31">
-      <c r="A35" s="42" t="s">
+      <c r="A35" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="B35" s="42"/>
-      <c r="C35" s="42"/>
-      <c r="D35" s="42"/>
-      <c r="E35" s="42"/>
-      <c r="F35" s="42"/>
-      <c r="G35" s="42"/>
-      <c r="H35" s="42"/>
-      <c r="I35" s="42"/>
-      <c r="J35" s="42"/>
-      <c r="K35" s="42"/>
-      <c r="L35" s="42"/>
+      <c r="B35" s="30"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="30"/>
+      <c r="H35" s="30"/>
+      <c r="I35" s="30"/>
+      <c r="J35" s="30"/>
+      <c r="K35" s="30"/>
+      <c r="L35" s="30"/>
       <c r="M35" s="26"/>
       <c r="N35" s="26"/>
       <c r="O35" s="26"/>
@@ -2454,20 +2463,20 @@
       <c r="AE35" s="8"/>
     </row>
     <row r="36" spans="1:31">
-      <c r="A36" s="42" t="s">
+      <c r="A36" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B36" s="42"/>
-      <c r="C36" s="42"/>
-      <c r="D36" s="42"/>
-      <c r="E36" s="42"/>
-      <c r="F36" s="42"/>
-      <c r="G36" s="42"/>
-      <c r="H36" s="42"/>
-      <c r="I36" s="42"/>
-      <c r="J36" s="42"/>
-      <c r="K36" s="42"/>
-      <c r="L36" s="42"/>
+      <c r="B36" s="30"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="30"/>
+      <c r="F36" s="30"/>
+      <c r="G36" s="30"/>
+      <c r="H36" s="30"/>
+      <c r="I36" s="30"/>
+      <c r="J36" s="30"/>
+      <c r="K36" s="30"/>
+      <c r="L36" s="30"/>
       <c r="M36" s="26"/>
       <c r="N36" s="26"/>
       <c r="O36" s="26"/>
@@ -2505,20 +2514,20 @@
       <c r="AE36" s="8"/>
     </row>
     <row r="37" spans="1:31">
-      <c r="A37" s="42" t="s">
+      <c r="A37" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="B37" s="42"/>
-      <c r="C37" s="42"/>
-      <c r="D37" s="42"/>
-      <c r="E37" s="42"/>
-      <c r="F37" s="42"/>
-      <c r="G37" s="42"/>
-      <c r="H37" s="42"/>
-      <c r="I37" s="42"/>
-      <c r="J37" s="42"/>
-      <c r="K37" s="42"/>
-      <c r="L37" s="42"/>
+      <c r="B37" s="30"/>
+      <c r="C37" s="30"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="30"/>
+      <c r="F37" s="30"/>
+      <c r="G37" s="30"/>
+      <c r="H37" s="30"/>
+      <c r="I37" s="30"/>
+      <c r="J37" s="30"/>
+      <c r="K37" s="30"/>
+      <c r="L37" s="30"/>
       <c r="M37" s="26"/>
       <c r="N37" s="26"/>
       <c r="O37" s="26"/>
@@ -2556,18 +2565,18 @@
       <c r="AE37" s="8"/>
     </row>
     <row r="38" spans="1:31">
-      <c r="A38" s="27"/>
-      <c r="B38" s="27"/>
-      <c r="C38" s="27"/>
-      <c r="D38" s="27"/>
-      <c r="E38" s="27"/>
-      <c r="F38" s="27"/>
-      <c r="G38" s="27"/>
-      <c r="H38" s="27"/>
-      <c r="I38" s="27"/>
-      <c r="J38" s="27"/>
-      <c r="K38" s="27"/>
-      <c r="L38" s="27"/>
+      <c r="A38" s="25"/>
+      <c r="B38" s="25"/>
+      <c r="C38" s="25"/>
+      <c r="D38" s="25"/>
+      <c r="E38" s="25"/>
+      <c r="F38" s="25"/>
+      <c r="G38" s="25"/>
+      <c r="H38" s="25"/>
+      <c r="I38" s="25"/>
+      <c r="J38" s="25"/>
+      <c r="K38" s="25"/>
+      <c r="L38" s="25"/>
       <c r="M38" s="26"/>
       <c r="N38" s="26"/>
       <c r="O38" s="26"/>
@@ -2589,18 +2598,18 @@
       <c r="AE38" s="8"/>
     </row>
     <row r="39" spans="1:31">
-      <c r="A39" s="27"/>
-      <c r="B39" s="27"/>
-      <c r="C39" s="27"/>
-      <c r="D39" s="27"/>
-      <c r="E39" s="27"/>
-      <c r="F39" s="27"/>
-      <c r="G39" s="27"/>
-      <c r="H39" s="27"/>
-      <c r="I39" s="27"/>
-      <c r="J39" s="27"/>
-      <c r="K39" s="27"/>
-      <c r="L39" s="27"/>
+      <c r="A39" s="25"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="25"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="25"/>
+      <c r="F39" s="25"/>
+      <c r="G39" s="25"/>
+      <c r="H39" s="25"/>
+      <c r="I39" s="25"/>
+      <c r="J39" s="25"/>
+      <c r="K39" s="25"/>
+      <c r="L39" s="25"/>
       <c r="M39" s="26"/>
       <c r="N39" s="26"/>
       <c r="O39" s="26"/>
@@ -2622,18 +2631,18 @@
       <c r="AE39" s="8"/>
     </row>
     <row r="40" spans="1:31">
-      <c r="A40" s="27"/>
-      <c r="B40" s="27"/>
-      <c r="C40" s="27"/>
-      <c r="D40" s="27"/>
-      <c r="E40" s="27"/>
-      <c r="F40" s="27"/>
-      <c r="G40" s="27"/>
-      <c r="H40" s="27"/>
-      <c r="I40" s="27"/>
-      <c r="J40" s="27"/>
-      <c r="K40" s="27"/>
-      <c r="L40" s="27"/>
+      <c r="A40" s="25"/>
+      <c r="B40" s="25"/>
+      <c r="C40" s="25"/>
+      <c r="D40" s="25"/>
+      <c r="E40" s="25"/>
+      <c r="F40" s="25"/>
+      <c r="G40" s="25"/>
+      <c r="H40" s="25"/>
+      <c r="I40" s="25"/>
+      <c r="J40" s="25"/>
+      <c r="K40" s="25"/>
+      <c r="L40" s="25"/>
       <c r="M40" s="26"/>
       <c r="N40" s="26"/>
       <c r="O40" s="26"/>
@@ -2655,18 +2664,18 @@
       <c r="AE40" s="8"/>
     </row>
     <row r="41" spans="1:31">
-      <c r="A41" s="27"/>
-      <c r="B41" s="27"/>
-      <c r="C41" s="27"/>
-      <c r="D41" s="27"/>
-      <c r="E41" s="27"/>
-      <c r="F41" s="27"/>
-      <c r="G41" s="27"/>
-      <c r="H41" s="27"/>
-      <c r="I41" s="27"/>
-      <c r="J41" s="27"/>
-      <c r="K41" s="27"/>
-      <c r="L41" s="27"/>
+      <c r="A41" s="25"/>
+      <c r="B41" s="25"/>
+      <c r="C41" s="25"/>
+      <c r="D41" s="25"/>
+      <c r="E41" s="25"/>
+      <c r="F41" s="25"/>
+      <c r="G41" s="25"/>
+      <c r="H41" s="25"/>
+      <c r="I41" s="25"/>
+      <c r="J41" s="25"/>
+      <c r="K41" s="25"/>
+      <c r="L41" s="25"/>
       <c r="M41" s="26"/>
       <c r="N41" s="26"/>
       <c r="O41" s="26"/>
@@ -2688,18 +2697,18 @@
       <c r="AE41" s="8"/>
     </row>
     <row r="42" spans="1:31">
-      <c r="A42" s="27"/>
-      <c r="B42" s="27"/>
-      <c r="C42" s="27"/>
-      <c r="D42" s="27"/>
-      <c r="E42" s="27"/>
-      <c r="F42" s="27"/>
-      <c r="G42" s="27"/>
-      <c r="H42" s="27"/>
-      <c r="I42" s="27"/>
-      <c r="J42" s="27"/>
-      <c r="K42" s="27"/>
-      <c r="L42" s="27"/>
+      <c r="A42" s="25"/>
+      <c r="B42" s="25"/>
+      <c r="C42" s="25"/>
+      <c r="D42" s="25"/>
+      <c r="E42" s="25"/>
+      <c r="F42" s="25"/>
+      <c r="G42" s="25"/>
+      <c r="H42" s="25"/>
+      <c r="I42" s="25"/>
+      <c r="J42" s="25"/>
+      <c r="K42" s="25"/>
+      <c r="L42" s="25"/>
       <c r="M42" s="26"/>
       <c r="N42" s="26"/>
       <c r="O42" s="26"/>
@@ -2721,18 +2730,18 @@
       <c r="AE42" s="8"/>
     </row>
     <row r="43" spans="1:31">
-      <c r="A43" s="27"/>
-      <c r="B43" s="27"/>
-      <c r="C43" s="27"/>
-      <c r="D43" s="27"/>
-      <c r="E43" s="27"/>
-      <c r="F43" s="27"/>
-      <c r="G43" s="27"/>
-      <c r="H43" s="27"/>
-      <c r="I43" s="27"/>
-      <c r="J43" s="27"/>
-      <c r="K43" s="27"/>
-      <c r="L43" s="27"/>
+      <c r="A43" s="25"/>
+      <c r="B43" s="25"/>
+      <c r="C43" s="25"/>
+      <c r="D43" s="25"/>
+      <c r="E43" s="25"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="25"/>
+      <c r="H43" s="25"/>
+      <c r="I43" s="25"/>
+      <c r="J43" s="25"/>
+      <c r="K43" s="25"/>
+      <c r="L43" s="25"/>
       <c r="M43" s="26"/>
       <c r="N43" s="26"/>
       <c r="O43" s="26"/>
@@ -2754,18 +2763,18 @@
       <c r="AE43" s="8"/>
     </row>
     <row r="44" spans="1:31">
-      <c r="A44" s="27"/>
-      <c r="B44" s="27"/>
-      <c r="C44" s="27"/>
-      <c r="D44" s="27"/>
-      <c r="E44" s="27"/>
-      <c r="F44" s="27"/>
-      <c r="G44" s="27"/>
-      <c r="H44" s="27"/>
-      <c r="I44" s="27"/>
-      <c r="J44" s="27"/>
-      <c r="K44" s="27"/>
-      <c r="L44" s="27"/>
+      <c r="A44" s="25"/>
+      <c r="B44" s="25"/>
+      <c r="C44" s="25"/>
+      <c r="D44" s="25"/>
+      <c r="E44" s="25"/>
+      <c r="F44" s="25"/>
+      <c r="G44" s="25"/>
+      <c r="H44" s="25"/>
+      <c r="I44" s="25"/>
+      <c r="J44" s="25"/>
+      <c r="K44" s="25"/>
+      <c r="L44" s="25"/>
       <c r="M44" s="26"/>
       <c r="N44" s="26"/>
       <c r="O44" s="26"/>
@@ -2787,18 +2796,18 @@
       <c r="AE44" s="8"/>
     </row>
     <row r="45" spans="1:31">
-      <c r="A45" s="27"/>
-      <c r="B45" s="27"/>
-      <c r="C45" s="27"/>
-      <c r="D45" s="27"/>
-      <c r="E45" s="27"/>
-      <c r="F45" s="27"/>
-      <c r="G45" s="27"/>
-      <c r="H45" s="27"/>
-      <c r="I45" s="27"/>
-      <c r="J45" s="27"/>
-      <c r="K45" s="27"/>
-      <c r="L45" s="27"/>
+      <c r="A45" s="25"/>
+      <c r="B45" s="25"/>
+      <c r="C45" s="25"/>
+      <c r="D45" s="25"/>
+      <c r="E45" s="25"/>
+      <c r="F45" s="25"/>
+      <c r="G45" s="25"/>
+      <c r="H45" s="25"/>
+      <c r="I45" s="25"/>
+      <c r="J45" s="25"/>
+      <c r="K45" s="25"/>
+      <c r="L45" s="25"/>
       <c r="M45" s="26"/>
       <c r="N45" s="26"/>
       <c r="O45" s="26"/>
@@ -2820,18 +2829,18 @@
       <c r="AE45" s="8"/>
     </row>
     <row r="46" spans="1:31">
-      <c r="A46" s="27"/>
-      <c r="B46" s="27"/>
-      <c r="C46" s="27"/>
-      <c r="D46" s="27"/>
-      <c r="E46" s="27"/>
-      <c r="F46" s="27"/>
-      <c r="G46" s="27"/>
-      <c r="H46" s="27"/>
-      <c r="I46" s="27"/>
-      <c r="J46" s="27"/>
-      <c r="K46" s="27"/>
-      <c r="L46" s="27"/>
+      <c r="A46" s="25"/>
+      <c r="B46" s="25"/>
+      <c r="C46" s="25"/>
+      <c r="D46" s="25"/>
+      <c r="E46" s="25"/>
+      <c r="F46" s="25"/>
+      <c r="G46" s="25"/>
+      <c r="H46" s="25"/>
+      <c r="I46" s="25"/>
+      <c r="J46" s="25"/>
+      <c r="K46" s="25"/>
+      <c r="L46" s="25"/>
       <c r="M46" s="26"/>
       <c r="N46" s="26"/>
       <c r="O46" s="26"/>
@@ -2853,18 +2862,18 @@
       <c r="AE46" s="8"/>
     </row>
     <row r="47" spans="1:31">
-      <c r="A47" s="27"/>
-      <c r="B47" s="27"/>
-      <c r="C47" s="27"/>
-      <c r="D47" s="27"/>
-      <c r="E47" s="27"/>
-      <c r="F47" s="27"/>
-      <c r="G47" s="27"/>
-      <c r="H47" s="27"/>
-      <c r="I47" s="27"/>
-      <c r="J47" s="27"/>
-      <c r="K47" s="27"/>
-      <c r="L47" s="27"/>
+      <c r="A47" s="25"/>
+      <c r="B47" s="25"/>
+      <c r="C47" s="25"/>
+      <c r="D47" s="25"/>
+      <c r="E47" s="25"/>
+      <c r="F47" s="25"/>
+      <c r="G47" s="25"/>
+      <c r="H47" s="25"/>
+      <c r="I47" s="25"/>
+      <c r="J47" s="25"/>
+      <c r="K47" s="25"/>
+      <c r="L47" s="25"/>
       <c r="M47" s="26"/>
       <c r="N47" s="26"/>
       <c r="O47" s="26"/>
@@ -2886,18 +2895,18 @@
       <c r="AE47" s="8"/>
     </row>
     <row r="48" spans="1:31">
-      <c r="A48" s="27"/>
-      <c r="B48" s="27"/>
-      <c r="C48" s="27"/>
-      <c r="D48" s="27"/>
-      <c r="E48" s="27"/>
-      <c r="F48" s="27"/>
-      <c r="G48" s="27"/>
-      <c r="H48" s="27"/>
-      <c r="I48" s="27"/>
-      <c r="J48" s="27"/>
-      <c r="K48" s="27"/>
-      <c r="L48" s="27"/>
+      <c r="A48" s="25"/>
+      <c r="B48" s="25"/>
+      <c r="C48" s="25"/>
+      <c r="D48" s="25"/>
+      <c r="E48" s="25"/>
+      <c r="F48" s="25"/>
+      <c r="G48" s="25"/>
+      <c r="H48" s="25"/>
+      <c r="I48" s="25"/>
+      <c r="J48" s="25"/>
+      <c r="K48" s="25"/>
+      <c r="L48" s="25"/>
       <c r="M48" s="26"/>
       <c r="N48" s="26"/>
       <c r="O48" s="26"/>
@@ -2919,18 +2928,18 @@
       <c r="AE48" s="8"/>
     </row>
     <row r="49" spans="1:31">
-      <c r="A49" s="27"/>
-      <c r="B49" s="27"/>
-      <c r="C49" s="27"/>
-      <c r="D49" s="27"/>
-      <c r="E49" s="27"/>
-      <c r="F49" s="27"/>
-      <c r="G49" s="27"/>
-      <c r="H49" s="27"/>
-      <c r="I49" s="27"/>
-      <c r="J49" s="27"/>
-      <c r="K49" s="27"/>
-      <c r="L49" s="27"/>
+      <c r="A49" s="25"/>
+      <c r="B49" s="25"/>
+      <c r="C49" s="25"/>
+      <c r="D49" s="25"/>
+      <c r="E49" s="25"/>
+      <c r="F49" s="25"/>
+      <c r="G49" s="25"/>
+      <c r="H49" s="25"/>
+      <c r="I49" s="25"/>
+      <c r="J49" s="25"/>
+      <c r="K49" s="25"/>
+      <c r="L49" s="25"/>
       <c r="M49" s="26"/>
       <c r="N49" s="26"/>
       <c r="O49" s="26"/>
@@ -2952,18 +2961,18 @@
       <c r="AE49" s="8"/>
     </row>
     <row r="50" spans="1:31">
-      <c r="A50" s="27"/>
-      <c r="B50" s="27"/>
-      <c r="C50" s="27"/>
-      <c r="D50" s="27"/>
-      <c r="E50" s="27"/>
-      <c r="F50" s="27"/>
-      <c r="G50" s="27"/>
-      <c r="H50" s="27"/>
-      <c r="I50" s="27"/>
-      <c r="J50" s="27"/>
-      <c r="K50" s="27"/>
-      <c r="L50" s="27"/>
+      <c r="A50" s="25"/>
+      <c r="B50" s="25"/>
+      <c r="C50" s="25"/>
+      <c r="D50" s="25"/>
+      <c r="E50" s="25"/>
+      <c r="F50" s="25"/>
+      <c r="G50" s="25"/>
+      <c r="H50" s="25"/>
+      <c r="I50" s="25"/>
+      <c r="J50" s="25"/>
+      <c r="K50" s="25"/>
+      <c r="L50" s="25"/>
       <c r="M50" s="26"/>
       <c r="N50" s="26"/>
       <c r="O50" s="26"/>
@@ -2985,18 +2994,18 @@
       <c r="AE50" s="8"/>
     </row>
     <row r="51" spans="1:31">
-      <c r="A51" s="27"/>
-      <c r="B51" s="27"/>
-      <c r="C51" s="27"/>
-      <c r="D51" s="27"/>
-      <c r="E51" s="27"/>
-      <c r="F51" s="27"/>
-      <c r="G51" s="27"/>
-      <c r="H51" s="27"/>
-      <c r="I51" s="27"/>
-      <c r="J51" s="27"/>
-      <c r="K51" s="27"/>
-      <c r="L51" s="27"/>
+      <c r="A51" s="25"/>
+      <c r="B51" s="25"/>
+      <c r="C51" s="25"/>
+      <c r="D51" s="25"/>
+      <c r="E51" s="25"/>
+      <c r="F51" s="25"/>
+      <c r="G51" s="25"/>
+      <c r="H51" s="25"/>
+      <c r="I51" s="25"/>
+      <c r="J51" s="25"/>
+      <c r="K51" s="25"/>
+      <c r="L51" s="25"/>
       <c r="M51" s="26"/>
       <c r="N51" s="26"/>
       <c r="O51" s="26"/>
@@ -3019,6 +3028,55 @@
     </row>
   </sheetData>
   <mergeCells count="65">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="M19:P21"/>
+    <mergeCell ref="A19:L21"/>
+    <mergeCell ref="M22:P22"/>
+    <mergeCell ref="A22:L22"/>
+    <mergeCell ref="A26:L26"/>
+    <mergeCell ref="M26:P26"/>
+    <mergeCell ref="A27:L27"/>
+    <mergeCell ref="M27:P27"/>
+    <mergeCell ref="A23:L23"/>
+    <mergeCell ref="M23:P23"/>
+    <mergeCell ref="A24:L24"/>
+    <mergeCell ref="M24:P24"/>
+    <mergeCell ref="A28:L28"/>
+    <mergeCell ref="M28:P28"/>
+    <mergeCell ref="A30:L30"/>
+    <mergeCell ref="M30:P30"/>
+    <mergeCell ref="A31:L31"/>
+    <mergeCell ref="M31:P31"/>
+    <mergeCell ref="A32:L32"/>
+    <mergeCell ref="M32:P32"/>
+    <mergeCell ref="A33:L33"/>
+    <mergeCell ref="M33:P33"/>
+    <mergeCell ref="A34:L34"/>
+    <mergeCell ref="M34:P34"/>
+    <mergeCell ref="A35:L35"/>
+    <mergeCell ref="M35:P35"/>
+    <mergeCell ref="A36:L36"/>
+    <mergeCell ref="M36:P36"/>
+    <mergeCell ref="A37:L37"/>
+    <mergeCell ref="M37:P37"/>
+    <mergeCell ref="A38:L38"/>
+    <mergeCell ref="M38:P38"/>
+    <mergeCell ref="A39:L39"/>
+    <mergeCell ref="M39:P39"/>
+    <mergeCell ref="A40:L40"/>
+    <mergeCell ref="M40:P40"/>
+    <mergeCell ref="A41:L41"/>
+    <mergeCell ref="M41:P41"/>
+    <mergeCell ref="A42:L42"/>
+    <mergeCell ref="M42:P42"/>
+    <mergeCell ref="A43:L43"/>
+    <mergeCell ref="M43:P43"/>
+    <mergeCell ref="M44:P44"/>
+    <mergeCell ref="A45:L45"/>
+    <mergeCell ref="M45:P45"/>
+    <mergeCell ref="A46:L46"/>
+    <mergeCell ref="M46:P46"/>
     <mergeCell ref="Q19:AZ19"/>
     <mergeCell ref="A50:L50"/>
     <mergeCell ref="M50:P50"/>
@@ -3035,59 +3093,9 @@
     <mergeCell ref="A49:L49"/>
     <mergeCell ref="M49:P49"/>
     <mergeCell ref="A44:L44"/>
-    <mergeCell ref="M44:P44"/>
-    <mergeCell ref="A45:L45"/>
-    <mergeCell ref="M45:P45"/>
-    <mergeCell ref="A46:L46"/>
-    <mergeCell ref="M46:P46"/>
-    <mergeCell ref="A41:L41"/>
-    <mergeCell ref="M41:P41"/>
-    <mergeCell ref="A42:L42"/>
-    <mergeCell ref="M42:P42"/>
-    <mergeCell ref="A43:L43"/>
-    <mergeCell ref="M43:P43"/>
-    <mergeCell ref="A38:L38"/>
-    <mergeCell ref="M38:P38"/>
-    <mergeCell ref="A39:L39"/>
-    <mergeCell ref="M39:P39"/>
-    <mergeCell ref="A40:L40"/>
-    <mergeCell ref="M40:P40"/>
-    <mergeCell ref="A35:L35"/>
-    <mergeCell ref="M35:P35"/>
-    <mergeCell ref="A36:L36"/>
-    <mergeCell ref="M36:P36"/>
-    <mergeCell ref="A37:L37"/>
-    <mergeCell ref="M37:P37"/>
-    <mergeCell ref="A32:L32"/>
-    <mergeCell ref="M32:P32"/>
-    <mergeCell ref="A33:L33"/>
-    <mergeCell ref="M33:P33"/>
-    <mergeCell ref="A34:L34"/>
-    <mergeCell ref="M34:P34"/>
-    <mergeCell ref="A28:L28"/>
-    <mergeCell ref="M28:P28"/>
-    <mergeCell ref="A30:L30"/>
-    <mergeCell ref="M30:P30"/>
-    <mergeCell ref="A31:L31"/>
-    <mergeCell ref="M31:P31"/>
-    <mergeCell ref="A26:L26"/>
-    <mergeCell ref="M26:P26"/>
-    <mergeCell ref="A27:L27"/>
-    <mergeCell ref="M27:P27"/>
-    <mergeCell ref="A23:L23"/>
-    <mergeCell ref="M23:P23"/>
-    <mergeCell ref="A24:L24"/>
-    <mergeCell ref="M24:P24"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="M19:P21"/>
-    <mergeCell ref="A19:L21"/>
-    <mergeCell ref="M22:P22"/>
-    <mergeCell ref="A22:L22"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -3108,20 +3116,20 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.140625" defaultRowHeight="13"/>
   <sheetData>
     <row r="1" spans="1:32">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="18" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -3148,61 +3156,61 @@
       <c r="P2" s="1"/>
     </row>
     <row r="3" spans="1:32" ht="14" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19" t="s">
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19"/>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="28" t="s">
+      <c r="N3" s="34"/>
+      <c r="O3" s="34"/>
+      <c r="P3" s="34"/>
+      <c r="Q3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="R3" s="29"/>
-      <c r="S3" s="29"/>
-      <c r="T3" s="29"/>
-      <c r="U3" s="29"/>
-      <c r="V3" s="29"/>
-      <c r="W3" s="29"/>
-      <c r="X3" s="29"/>
-      <c r="Y3" s="29"/>
-      <c r="Z3" s="29"/>
-      <c r="AA3" s="29"/>
-      <c r="AB3" s="29"/>
-      <c r="AC3" s="29"/>
-      <c r="AD3" s="29"/>
-      <c r="AE3" s="30"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="23"/>
+      <c r="U3" s="23"/>
+      <c r="V3" s="23"/>
+      <c r="W3" s="23"/>
+      <c r="X3" s="23"/>
+      <c r="Y3" s="23"/>
+      <c r="Z3" s="23"/>
+      <c r="AA3" s="23"/>
+      <c r="AB3" s="23"/>
+      <c r="AC3" s="23"/>
+      <c r="AD3" s="23"/>
+      <c r="AE3" s="24"/>
     </row>
     <row r="4" spans="1:32">
-      <c r="A4" s="23"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="20"/>
+      <c r="A4" s="38"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
+      <c r="N4" s="35"/>
+      <c r="O4" s="35"/>
+      <c r="P4" s="35"/>
       <c r="Q4" s="3">
         <v>14</v>
       </c>
@@ -3251,22 +3259,22 @@
       <c r="AF4" s="9"/>
     </row>
     <row r="5" spans="1:32" ht="14" thickBot="1">
-      <c r="A5" s="24"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="21"/>
-      <c r="O5" s="21"/>
-      <c r="P5" s="21"/>
+      <c r="A5" s="40"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="41"/>
+      <c r="N5" s="41"/>
+      <c r="O5" s="41"/>
+      <c r="P5" s="41"/>
       <c r="Q5" s="5">
         <f>SUM(Q6:Q35)</f>
         <v>0</v>
@@ -3330,22 +3338,22 @@
       <c r="AF5" s="10"/>
     </row>
     <row r="6" spans="1:32">
-      <c r="A6" s="25"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
-      <c r="L6" s="25"/>
-      <c r="M6" s="25"/>
-      <c r="N6" s="25"/>
-      <c r="O6" s="25"/>
-      <c r="P6" s="25"/>
+      <c r="A6" s="42"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="42"/>
+      <c r="K6" s="42"/>
+      <c r="L6" s="42"/>
+      <c r="M6" s="42"/>
+      <c r="N6" s="42"/>
+      <c r="O6" s="42"/>
+      <c r="P6" s="42"/>
       <c r="Q6" s="7"/>
       <c r="R6" s="7"/>
       <c r="S6" s="7"/>
@@ -4320,61 +4328,7 @@
       <c r="AE35" s="8"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="65">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="A3:L5"/>
-    <mergeCell ref="M3:P5"/>
-    <mergeCell ref="Q3:AE3"/>
-    <mergeCell ref="A7:L7"/>
-    <mergeCell ref="M7:P7"/>
-    <mergeCell ref="A8:L8"/>
-    <mergeCell ref="M8:P8"/>
-    <mergeCell ref="A6:L6"/>
-    <mergeCell ref="M6:P6"/>
-    <mergeCell ref="A9:L9"/>
-    <mergeCell ref="M9:P9"/>
-    <mergeCell ref="A10:L10"/>
-    <mergeCell ref="M10:P10"/>
-    <mergeCell ref="A11:L11"/>
-    <mergeCell ref="M11:P11"/>
-    <mergeCell ref="A12:L12"/>
-    <mergeCell ref="M12:P12"/>
-    <mergeCell ref="A13:L13"/>
-    <mergeCell ref="M13:P13"/>
-    <mergeCell ref="A14:L14"/>
-    <mergeCell ref="M14:P14"/>
-    <mergeCell ref="A15:L15"/>
-    <mergeCell ref="M15:P15"/>
-    <mergeCell ref="A16:L16"/>
-    <mergeCell ref="M16:P16"/>
-    <mergeCell ref="A17:L17"/>
-    <mergeCell ref="M17:P17"/>
-    <mergeCell ref="A18:L18"/>
-    <mergeCell ref="M18:P18"/>
-    <mergeCell ref="A19:L19"/>
-    <mergeCell ref="M19:P19"/>
-    <mergeCell ref="A20:L20"/>
-    <mergeCell ref="M20:P20"/>
-    <mergeCell ref="A21:L21"/>
-    <mergeCell ref="M21:P21"/>
-    <mergeCell ref="A22:L22"/>
-    <mergeCell ref="M22:P22"/>
-    <mergeCell ref="A23:L23"/>
-    <mergeCell ref="M23:P23"/>
-    <mergeCell ref="A24:L24"/>
-    <mergeCell ref="M24:P24"/>
-    <mergeCell ref="A25:L25"/>
-    <mergeCell ref="M25:P25"/>
-    <mergeCell ref="A26:L26"/>
-    <mergeCell ref="M26:P26"/>
-    <mergeCell ref="A27:L27"/>
-    <mergeCell ref="M27:P27"/>
-    <mergeCell ref="A28:L28"/>
-    <mergeCell ref="M28:P28"/>
-    <mergeCell ref="A29:L29"/>
-    <mergeCell ref="M29:P29"/>
     <mergeCell ref="A30:L30"/>
     <mergeCell ref="M30:P30"/>
     <mergeCell ref="A34:L34"/>
@@ -4387,6 +4341,59 @@
     <mergeCell ref="M32:P32"/>
     <mergeCell ref="A33:L33"/>
     <mergeCell ref="M33:P33"/>
+    <mergeCell ref="A27:L27"/>
+    <mergeCell ref="M27:P27"/>
+    <mergeCell ref="A28:L28"/>
+    <mergeCell ref="M28:P28"/>
+    <mergeCell ref="A29:L29"/>
+    <mergeCell ref="M29:P29"/>
+    <mergeCell ref="A24:L24"/>
+    <mergeCell ref="M24:P24"/>
+    <mergeCell ref="A25:L25"/>
+    <mergeCell ref="M25:P25"/>
+    <mergeCell ref="A26:L26"/>
+    <mergeCell ref="M26:P26"/>
+    <mergeCell ref="A21:L21"/>
+    <mergeCell ref="M21:P21"/>
+    <mergeCell ref="A22:L22"/>
+    <mergeCell ref="M22:P22"/>
+    <mergeCell ref="A23:L23"/>
+    <mergeCell ref="M23:P23"/>
+    <mergeCell ref="A18:L18"/>
+    <mergeCell ref="M18:P18"/>
+    <mergeCell ref="A19:L19"/>
+    <mergeCell ref="M19:P19"/>
+    <mergeCell ref="A20:L20"/>
+    <mergeCell ref="M20:P20"/>
+    <mergeCell ref="A15:L15"/>
+    <mergeCell ref="M15:P15"/>
+    <mergeCell ref="A16:L16"/>
+    <mergeCell ref="M16:P16"/>
+    <mergeCell ref="A17:L17"/>
+    <mergeCell ref="M17:P17"/>
+    <mergeCell ref="A12:L12"/>
+    <mergeCell ref="M12:P12"/>
+    <mergeCell ref="A13:L13"/>
+    <mergeCell ref="M13:P13"/>
+    <mergeCell ref="A14:L14"/>
+    <mergeCell ref="M14:P14"/>
+    <mergeCell ref="A9:L9"/>
+    <mergeCell ref="M9:P9"/>
+    <mergeCell ref="A10:L10"/>
+    <mergeCell ref="M10:P10"/>
+    <mergeCell ref="A11:L11"/>
+    <mergeCell ref="M11:P11"/>
+    <mergeCell ref="A7:L7"/>
+    <mergeCell ref="M7:P7"/>
+    <mergeCell ref="A8:L8"/>
+    <mergeCell ref="M8:P8"/>
+    <mergeCell ref="A6:L6"/>
+    <mergeCell ref="M6:P6"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="A3:L5"/>
+    <mergeCell ref="M3:P5"/>
+    <mergeCell ref="Q3:AE3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4410,20 +4417,20 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.140625" defaultRowHeight="13"/>
   <sheetData>
     <row r="1" spans="1:32">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="18" t="s">
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -4450,61 +4457,61 @@
       <c r="P2" s="1"/>
     </row>
     <row r="3" spans="1:32" ht="14" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="19"/>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19" t="s">
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="N3" s="19"/>
-      <c r="O3" s="19"/>
-      <c r="P3" s="19"/>
-      <c r="Q3" s="28" t="s">
+      <c r="N3" s="34"/>
+      <c r="O3" s="34"/>
+      <c r="P3" s="34"/>
+      <c r="Q3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="R3" s="29"/>
-      <c r="S3" s="29"/>
-      <c r="T3" s="29"/>
-      <c r="U3" s="29"/>
-      <c r="V3" s="29"/>
-      <c r="W3" s="29"/>
-      <c r="X3" s="29"/>
-      <c r="Y3" s="29"/>
-      <c r="Z3" s="29"/>
-      <c r="AA3" s="29"/>
-      <c r="AB3" s="29"/>
-      <c r="AC3" s="29"/>
-      <c r="AD3" s="29"/>
-      <c r="AE3" s="30"/>
+      <c r="R3" s="23"/>
+      <c r="S3" s="23"/>
+      <c r="T3" s="23"/>
+      <c r="U3" s="23"/>
+      <c r="V3" s="23"/>
+      <c r="W3" s="23"/>
+      <c r="X3" s="23"/>
+      <c r="Y3" s="23"/>
+      <c r="Z3" s="23"/>
+      <c r="AA3" s="23"/>
+      <c r="AB3" s="23"/>
+      <c r="AC3" s="23"/>
+      <c r="AD3" s="23"/>
+      <c r="AE3" s="24"/>
     </row>
     <row r="4" spans="1:32">
-      <c r="A4" s="23"/>
-      <c r="B4" s="20"/>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="20"/>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
-      <c r="J4" s="20"/>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="20"/>
+      <c r="A4" s="38"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
+      <c r="N4" s="35"/>
+      <c r="O4" s="35"/>
+      <c r="P4" s="35"/>
       <c r="Q4" s="3">
         <v>14</v>
       </c>
@@ -4553,22 +4560,22 @@
       <c r="AF4" s="9"/>
     </row>
     <row r="5" spans="1:32" ht="14" thickBot="1">
-      <c r="A5" s="24"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="21"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="21"/>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="21"/>
-      <c r="N5" s="21"/>
-      <c r="O5" s="21"/>
-      <c r="P5" s="21"/>
+      <c r="A5" s="40"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
+      <c r="G5" s="41"/>
+      <c r="H5" s="41"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="41"/>
+      <c r="M5" s="41"/>
+      <c r="N5" s="41"/>
+      <c r="O5" s="41"/>
+      <c r="P5" s="41"/>
       <c r="Q5" s="5">
         <f>SUM(Q6:Q35)</f>
         <v>0</v>
@@ -4632,22 +4639,22 @@
       <c r="AF5" s="10"/>
     </row>
     <row r="6" spans="1:32">
-      <c r="A6" s="25"/>
-      <c r="B6" s="25"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="25"/>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25"/>
-      <c r="L6" s="25"/>
-      <c r="M6" s="25"/>
-      <c r="N6" s="25"/>
-      <c r="O6" s="25"/>
-      <c r="P6" s="25"/>
+      <c r="A6" s="42"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="42"/>
+      <c r="K6" s="42"/>
+      <c r="L6" s="42"/>
+      <c r="M6" s="42"/>
+      <c r="N6" s="42"/>
+      <c r="O6" s="42"/>
+      <c r="P6" s="42"/>
       <c r="Q6" s="7"/>
       <c r="R6" s="7"/>
       <c r="S6" s="7"/>
@@ -5622,61 +5629,7 @@
       <c r="AE35" s="8"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="65">
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="A3:L5"/>
-    <mergeCell ref="M3:P5"/>
-    <mergeCell ref="Q3:AE3"/>
-    <mergeCell ref="A7:L7"/>
-    <mergeCell ref="M7:P7"/>
-    <mergeCell ref="A8:L8"/>
-    <mergeCell ref="M8:P8"/>
-    <mergeCell ref="A6:L6"/>
-    <mergeCell ref="M6:P6"/>
-    <mergeCell ref="A9:L9"/>
-    <mergeCell ref="M9:P9"/>
-    <mergeCell ref="A10:L10"/>
-    <mergeCell ref="M10:P10"/>
-    <mergeCell ref="A11:L11"/>
-    <mergeCell ref="M11:P11"/>
-    <mergeCell ref="A12:L12"/>
-    <mergeCell ref="M12:P12"/>
-    <mergeCell ref="A13:L13"/>
-    <mergeCell ref="M13:P13"/>
-    <mergeCell ref="A14:L14"/>
-    <mergeCell ref="M14:P14"/>
-    <mergeCell ref="A15:L15"/>
-    <mergeCell ref="M15:P15"/>
-    <mergeCell ref="A16:L16"/>
-    <mergeCell ref="M16:P16"/>
-    <mergeCell ref="A17:L17"/>
-    <mergeCell ref="M17:P17"/>
-    <mergeCell ref="A18:L18"/>
-    <mergeCell ref="M18:P18"/>
-    <mergeCell ref="A19:L19"/>
-    <mergeCell ref="M19:P19"/>
-    <mergeCell ref="A20:L20"/>
-    <mergeCell ref="M20:P20"/>
-    <mergeCell ref="A21:L21"/>
-    <mergeCell ref="M21:P21"/>
-    <mergeCell ref="A22:L22"/>
-    <mergeCell ref="M22:P22"/>
-    <mergeCell ref="A23:L23"/>
-    <mergeCell ref="M23:P23"/>
-    <mergeCell ref="A24:L24"/>
-    <mergeCell ref="M24:P24"/>
-    <mergeCell ref="A25:L25"/>
-    <mergeCell ref="M25:P25"/>
-    <mergeCell ref="A26:L26"/>
-    <mergeCell ref="M26:P26"/>
-    <mergeCell ref="A27:L27"/>
-    <mergeCell ref="M27:P27"/>
-    <mergeCell ref="A28:L28"/>
-    <mergeCell ref="M28:P28"/>
-    <mergeCell ref="A29:L29"/>
-    <mergeCell ref="M29:P29"/>
     <mergeCell ref="A30:L30"/>
     <mergeCell ref="M30:P30"/>
     <mergeCell ref="A34:L34"/>
@@ -5689,6 +5642,59 @@
     <mergeCell ref="M32:P32"/>
     <mergeCell ref="A33:L33"/>
     <mergeCell ref="M33:P33"/>
+    <mergeCell ref="A27:L27"/>
+    <mergeCell ref="M27:P27"/>
+    <mergeCell ref="A28:L28"/>
+    <mergeCell ref="M28:P28"/>
+    <mergeCell ref="A29:L29"/>
+    <mergeCell ref="M29:P29"/>
+    <mergeCell ref="A24:L24"/>
+    <mergeCell ref="M24:P24"/>
+    <mergeCell ref="A25:L25"/>
+    <mergeCell ref="M25:P25"/>
+    <mergeCell ref="A26:L26"/>
+    <mergeCell ref="M26:P26"/>
+    <mergeCell ref="A21:L21"/>
+    <mergeCell ref="M21:P21"/>
+    <mergeCell ref="A22:L22"/>
+    <mergeCell ref="M22:P22"/>
+    <mergeCell ref="A23:L23"/>
+    <mergeCell ref="M23:P23"/>
+    <mergeCell ref="A18:L18"/>
+    <mergeCell ref="M18:P18"/>
+    <mergeCell ref="A19:L19"/>
+    <mergeCell ref="M19:P19"/>
+    <mergeCell ref="A20:L20"/>
+    <mergeCell ref="M20:P20"/>
+    <mergeCell ref="A15:L15"/>
+    <mergeCell ref="M15:P15"/>
+    <mergeCell ref="A16:L16"/>
+    <mergeCell ref="M16:P16"/>
+    <mergeCell ref="A17:L17"/>
+    <mergeCell ref="M17:P17"/>
+    <mergeCell ref="A12:L12"/>
+    <mergeCell ref="M12:P12"/>
+    <mergeCell ref="A13:L13"/>
+    <mergeCell ref="M13:P13"/>
+    <mergeCell ref="A14:L14"/>
+    <mergeCell ref="M14:P14"/>
+    <mergeCell ref="A9:L9"/>
+    <mergeCell ref="M9:P9"/>
+    <mergeCell ref="A10:L10"/>
+    <mergeCell ref="M10:P10"/>
+    <mergeCell ref="A11:L11"/>
+    <mergeCell ref="M11:P11"/>
+    <mergeCell ref="A7:L7"/>
+    <mergeCell ref="M7:P7"/>
+    <mergeCell ref="A8:L8"/>
+    <mergeCell ref="M8:P8"/>
+    <mergeCell ref="A6:L6"/>
+    <mergeCell ref="M6:P6"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="A3:L5"/>
+    <mergeCell ref="M3:P5"/>
+    <mergeCell ref="Q3:AE3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Updated Burn down and added content section to CSS
</commit_message>
<xml_diff>
--- a/Burn Down Chart.xlsx
+++ b/Burn Down Chart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25360" windowHeight="15320" tabRatio="500"/>
+    <workbookView xWindow="9460" yWindow="0" windowWidth="25360" windowHeight="15320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
   <si>
     <t>Job Assignment</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -126,17 +126,43 @@
     <t>Search fuctions of the database</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
+  <si>
+    <t>MJ</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Submit an App to the Database</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CH, RV</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Create App Database</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>MJ</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AS</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>CH, RV</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Create the Visual of pages</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
   <fonts count="3">
     <font>
       <sz val="10"/>
@@ -752,50 +778,50 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="36"/>
                 <c:pt idx="0">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>67.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>67.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>67.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>54.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>51.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>51.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>54.0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>51.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>38.0</c:v>
-                </c:pt>
                 <c:pt idx="6">
-                  <c:v>31.0</c:v>
+                  <c:v>47.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>26.0</c:v>
+                  <c:v>41.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="468494680"/>
-        <c:axId val="467886648"/>
+        <c:axId val="226374616"/>
+        <c:axId val="226384968"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="468494680"/>
+        <c:axId val="226374616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="467886648"/>
+        <c:crossAx val="226384968"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="467886648"/>
+        <c:axId val="226384968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -803,7 +829,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="468494680"/>
+        <c:crossAx val="226374616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1177,10 +1203,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:AZ51"/>
+  <dimension ref="A1:AZ54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X28" sqref="X28"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="AD37" sqref="AD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.140625" defaultRowHeight="13"/>
@@ -1713,36 +1739,36 @@
       <c r="O21" s="36"/>
       <c r="P21" s="36"/>
       <c r="Q21" s="17">
-        <f t="shared" ref="Q21:W21" si="0">SUM(Q22:Q51)</f>
-        <v>54</v>
+        <f t="shared" ref="Q21:W21" si="0">SUM(Q22:Q54)</f>
+        <v>70</v>
       </c>
       <c r="R21" s="18">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="S21" s="18">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="T21" s="18">
         <f t="shared" si="0"/>
-        <v>54</v>
+        <v>70</v>
       </c>
       <c r="U21" s="18">
         <f t="shared" si="0"/>
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="V21" s="18">
         <f t="shared" si="0"/>
-        <v>38</v>
+        <v>54</v>
       </c>
       <c r="W21" s="18">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="X21" s="18">
-        <f t="shared" ref="X21" si="1">SUM(X22:X51)</f>
-        <v>26</v>
+        <f t="shared" ref="X21" si="1">SUM(X22:X54)</f>
+        <v>41</v>
       </c>
       <c r="Y21" s="18"/>
       <c r="Z21" s="18"/>
@@ -1818,6 +1844,21 @@
       <c r="X22" s="13">
         <v>0</v>
       </c>
+      <c r="Y22" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="13">
+        <v>0</v>
+      </c>
+      <c r="AB22" s="13">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="13">
+        <v>0</v>
+      </c>
       <c r="AE22" s="8"/>
       <c r="AF22" s="8"/>
       <c r="AG22" s="8"/>
@@ -1868,6 +1909,21 @@
       <c r="X23" s="13">
         <v>0</v>
       </c>
+      <c r="Y23" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA23" s="13">
+        <v>0</v>
+      </c>
+      <c r="AB23" s="13">
+        <v>0</v>
+      </c>
+      <c r="AC23" s="13">
+        <v>0</v>
+      </c>
       <c r="AE23" s="8"/>
     </row>
     <row r="24" spans="1:52" ht="14" thickTop="1">
@@ -1915,6 +1971,21 @@
       <c r="X24" s="13">
         <v>0</v>
       </c>
+      <c r="Y24" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z24" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA24" s="13">
+        <v>0</v>
+      </c>
+      <c r="AB24" s="13">
+        <v>0</v>
+      </c>
+      <c r="AC24" s="13">
+        <v>0</v>
+      </c>
       <c r="AE24" s="8"/>
     </row>
     <row r="25" spans="1:52" ht="14" thickTop="1">
@@ -1962,6 +2033,21 @@
       <c r="X25" s="13">
         <v>0</v>
       </c>
+      <c r="Y25" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z25" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA25" s="13">
+        <v>0</v>
+      </c>
+      <c r="AB25" s="13">
+        <v>0</v>
+      </c>
+      <c r="AC25" s="13">
+        <v>0</v>
+      </c>
       <c r="AE25" s="8"/>
     </row>
     <row r="26" spans="1:52" ht="14" thickTop="1">
@@ -2009,6 +2095,21 @@
       <c r="X26" s="13">
         <v>0</v>
       </c>
+      <c r="Y26" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z26" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA26" s="13">
+        <v>0</v>
+      </c>
+      <c r="AB26" s="13">
+        <v>0</v>
+      </c>
+      <c r="AC26" s="13">
+        <v>0</v>
+      </c>
       <c r="AE26" s="8"/>
     </row>
     <row r="27" spans="1:52" ht="14" thickTop="1">
@@ -2056,6 +2157,21 @@
       <c r="X27" s="13">
         <v>0</v>
       </c>
+      <c r="Y27" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z27" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA27" s="13">
+        <v>0</v>
+      </c>
+      <c r="AB27" s="13">
+        <v>0</v>
+      </c>
+      <c r="AC27" s="13">
+        <v>0</v>
+      </c>
       <c r="AE27" s="8"/>
     </row>
     <row r="28" spans="1:52">
@@ -2101,7 +2217,22 @@
         <v>1</v>
       </c>
       <c r="X28" s="13">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="Y28" s="13">
+        <v>0</v>
+      </c>
+      <c r="Z28" s="13">
+        <v>0</v>
+      </c>
+      <c r="AA28" s="13">
+        <v>0</v>
+      </c>
+      <c r="AB28" s="13">
+        <v>0</v>
+      </c>
+      <c r="AC28" s="13">
+        <v>0</v>
       </c>
       <c r="AE28" s="8"/>
     </row>
@@ -2120,7 +2251,9 @@
       <c r="J29" s="27"/>
       <c r="K29" s="27"/>
       <c r="L29" s="27"/>
-      <c r="M29" s="28"/>
+      <c r="M29" s="28" t="s">
+        <v>31</v>
+      </c>
       <c r="N29" s="28"/>
       <c r="O29" s="28"/>
       <c r="P29" s="28"/>
@@ -2148,11 +2281,21 @@
       <c r="X29" s="13">
         <v>2</v>
       </c>
-      <c r="Y29" s="8"/>
-      <c r="Z29" s="8"/>
-      <c r="AA29" s="8"/>
-      <c r="AB29" s="8"/>
-      <c r="AC29" s="8"/>
+      <c r="Y29" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z29" s="13">
+        <v>2</v>
+      </c>
+      <c r="AA29" s="13">
+        <v>2</v>
+      </c>
+      <c r="AB29" s="13">
+        <v>2</v>
+      </c>
+      <c r="AC29" s="13">
+        <v>2</v>
+      </c>
       <c r="AD29" s="8"/>
       <c r="AE29" s="8"/>
     </row>
@@ -2171,7 +2314,9 @@
       <c r="J30" s="31"/>
       <c r="K30" s="31"/>
       <c r="L30" s="31"/>
-      <c r="M30" s="26"/>
+      <c r="M30" s="26" t="s">
+        <v>26</v>
+      </c>
       <c r="N30" s="26"/>
       <c r="O30" s="26"/>
       <c r="P30" s="26"/>
@@ -2199,11 +2344,21 @@
       <c r="X30" s="8">
         <v>3</v>
       </c>
-      <c r="Y30" s="8"/>
-      <c r="Z30" s="8"/>
-      <c r="AA30" s="8"/>
-      <c r="AB30" s="8"/>
-      <c r="AC30" s="8"/>
+      <c r="Y30" s="13">
+        <v>3</v>
+      </c>
+      <c r="Z30" s="13">
+        <v>3</v>
+      </c>
+      <c r="AA30" s="13">
+        <v>3</v>
+      </c>
+      <c r="AB30" s="13">
+        <v>3</v>
+      </c>
+      <c r="AC30" s="13">
+        <v>3</v>
+      </c>
       <c r="AD30" s="8"/>
       <c r="AE30" s="8"/>
     </row>
@@ -2222,7 +2377,9 @@
       <c r="J31" s="31"/>
       <c r="K31" s="31"/>
       <c r="L31" s="31"/>
-      <c r="M31" s="26"/>
+      <c r="M31" s="26" t="s">
+        <v>26</v>
+      </c>
       <c r="N31" s="26"/>
       <c r="O31" s="26"/>
       <c r="P31" s="26"/>
@@ -2250,11 +2407,21 @@
       <c r="X31" s="13">
         <v>3</v>
       </c>
-      <c r="Y31" s="8"/>
-      <c r="Z31" s="8"/>
-      <c r="AA31" s="8"/>
-      <c r="AB31" s="8"/>
-      <c r="AC31" s="8"/>
+      <c r="Y31" s="13">
+        <v>3</v>
+      </c>
+      <c r="Z31" s="13">
+        <v>3</v>
+      </c>
+      <c r="AA31" s="13">
+        <v>3</v>
+      </c>
+      <c r="AB31" s="13">
+        <v>3</v>
+      </c>
+      <c r="AC31" s="13">
+        <v>3</v>
+      </c>
       <c r="AD31" s="8"/>
       <c r="AE31" s="8"/>
     </row>
@@ -2273,7 +2440,9 @@
       <c r="J32" s="31"/>
       <c r="K32" s="31"/>
       <c r="L32" s="31"/>
-      <c r="M32" s="26"/>
+      <c r="M32" s="26" t="s">
+        <v>28</v>
+      </c>
       <c r="N32" s="26"/>
       <c r="O32" s="26"/>
       <c r="P32" s="26"/>
@@ -2301,11 +2470,21 @@
       <c r="X32" s="13">
         <v>7</v>
       </c>
-      <c r="Y32" s="8"/>
-      <c r="Z32" s="8"/>
-      <c r="AA32" s="8"/>
-      <c r="AB32" s="8"/>
-      <c r="AC32" s="8"/>
+      <c r="Y32" s="13">
+        <v>7</v>
+      </c>
+      <c r="Z32" s="13">
+        <v>7</v>
+      </c>
+      <c r="AA32" s="13">
+        <v>7</v>
+      </c>
+      <c r="AB32" s="13">
+        <v>7</v>
+      </c>
+      <c r="AC32" s="13">
+        <v>7</v>
+      </c>
       <c r="AD32" s="8"/>
       <c r="AE32" s="8"/>
     </row>
@@ -2324,7 +2503,9 @@
       <c r="J33" s="31"/>
       <c r="K33" s="31"/>
       <c r="L33" s="31"/>
-      <c r="M33" s="26"/>
+      <c r="M33" s="26" t="s">
+        <v>31</v>
+      </c>
       <c r="N33" s="26"/>
       <c r="O33" s="26"/>
       <c r="P33" s="26"/>
@@ -2352,17 +2533,27 @@
       <c r="X33" s="13">
         <v>2</v>
       </c>
-      <c r="Y33" s="8"/>
-      <c r="Z33" s="8"/>
-      <c r="AA33" s="8"/>
-      <c r="AB33" s="8"/>
-      <c r="AC33" s="8"/>
+      <c r="Y33" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z33" s="13">
+        <v>2</v>
+      </c>
+      <c r="AA33" s="13">
+        <v>2</v>
+      </c>
+      <c r="AB33" s="13">
+        <v>2</v>
+      </c>
+      <c r="AC33" s="13">
+        <v>2</v>
+      </c>
       <c r="AD33" s="8"/>
       <c r="AE33" s="8"/>
     </row>
     <row r="34" spans="1:31">
       <c r="A34" s="31" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="B34" s="31"/>
       <c r="C34" s="31"/>
@@ -2375,11 +2566,13 @@
       <c r="J34" s="31"/>
       <c r="K34" s="31"/>
       <c r="L34" s="31"/>
-      <c r="M34" s="26"/>
+      <c r="M34" s="26" t="s">
+        <v>26</v>
+      </c>
       <c r="N34" s="26"/>
       <c r="O34" s="26"/>
       <c r="P34" s="26"/>
-      <c r="Q34" s="8">
+      <c r="Q34" s="13">
         <v>1</v>
       </c>
       <c r="R34" s="13">
@@ -2403,263 +2596,393 @@
       <c r="X34" s="13">
         <v>1</v>
       </c>
-      <c r="Y34" s="8"/>
-      <c r="Z34" s="8"/>
-      <c r="AA34" s="8"/>
-      <c r="AB34" s="8"/>
-      <c r="AC34" s="8"/>
+      <c r="Y34" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z34" s="13">
+        <v>1</v>
+      </c>
+      <c r="AA34" s="13">
+        <v>1</v>
+      </c>
+      <c r="AB34" s="13">
+        <v>1</v>
+      </c>
+      <c r="AC34" s="13">
+        <v>1</v>
+      </c>
       <c r="AD34" s="8"/>
       <c r="AE34" s="8"/>
     </row>
     <row r="35" spans="1:31">
-      <c r="A35" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="B35" s="30"/>
-      <c r="C35" s="30"/>
-      <c r="D35" s="30"/>
-      <c r="E35" s="30"/>
-      <c r="F35" s="30"/>
-      <c r="G35" s="30"/>
-      <c r="H35" s="30"/>
-      <c r="I35" s="30"/>
-      <c r="J35" s="30"/>
-      <c r="K35" s="30"/>
-      <c r="L35" s="30"/>
-      <c r="M35" s="26"/>
+      <c r="A35" s="31" t="s">
+        <v>29</v>
+      </c>
+      <c r="B35" s="31"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="31"/>
+      <c r="G35" s="31"/>
+      <c r="H35" s="31"/>
+      <c r="I35" s="31"/>
+      <c r="J35" s="31"/>
+      <c r="K35" s="31"/>
+      <c r="L35" s="31"/>
+      <c r="M35" s="26" t="s">
+        <v>30</v>
+      </c>
       <c r="N35" s="26"/>
       <c r="O35" s="26"/>
       <c r="P35" s="26"/>
-      <c r="Q35" s="8">
-        <v>3</v>
+      <c r="Q35" s="13">
+        <v>5</v>
       </c>
       <c r="R35" s="13">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="S35" s="13">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="T35" s="13">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="U35" s="13">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="V35" s="13">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="W35" s="13">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="X35" s="13">
-        <v>3</v>
-      </c>
-      <c r="Y35" s="8"/>
-      <c r="Z35" s="8"/>
-      <c r="AA35" s="8"/>
-      <c r="AB35" s="8"/>
-      <c r="AC35" s="8"/>
+        <v>5</v>
+      </c>
+      <c r="Y35" s="13">
+        <v>5</v>
+      </c>
+      <c r="Z35" s="13">
+        <v>5</v>
+      </c>
+      <c r="AA35" s="13">
+        <v>5</v>
+      </c>
+      <c r="AB35" s="13">
+        <v>5</v>
+      </c>
+      <c r="AC35" s="13">
+        <v>5</v>
+      </c>
       <c r="AD35" s="8"/>
       <c r="AE35" s="8"/>
     </row>
     <row r="36" spans="1:31">
-      <c r="A36" s="30" t="s">
-        <v>24</v>
-      </c>
-      <c r="B36" s="30"/>
-      <c r="C36" s="30"/>
-      <c r="D36" s="30"/>
-      <c r="E36" s="30"/>
-      <c r="F36" s="30"/>
-      <c r="G36" s="30"/>
-      <c r="H36" s="30"/>
-      <c r="I36" s="30"/>
-      <c r="J36" s="30"/>
-      <c r="K36" s="30"/>
-      <c r="L36" s="30"/>
-      <c r="M36" s="26"/>
+      <c r="A36" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" s="31"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="31"/>
+      <c r="G36" s="31"/>
+      <c r="H36" s="31"/>
+      <c r="I36" s="31"/>
+      <c r="J36" s="31"/>
+      <c r="K36" s="31"/>
+      <c r="L36" s="31"/>
+      <c r="M36" s="26" t="s">
+        <v>31</v>
+      </c>
       <c r="N36" s="26"/>
       <c r="O36" s="26"/>
       <c r="P36" s="26"/>
       <c r="Q36" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="R36" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S36" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T36" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="U36" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V36" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W36" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X36" s="13">
-        <v>2</v>
-      </c>
-      <c r="Y36" s="8"/>
-      <c r="Z36" s="8"/>
-      <c r="AA36" s="8"/>
-      <c r="AB36" s="8"/>
-      <c r="AC36" s="8"/>
+        <v>1</v>
+      </c>
+      <c r="Y36" s="13">
+        <v>1</v>
+      </c>
+      <c r="Z36" s="13">
+        <v>1</v>
+      </c>
+      <c r="AA36" s="13">
+        <v>1</v>
+      </c>
+      <c r="AB36" s="13">
+        <v>1</v>
+      </c>
+      <c r="AC36" s="13">
+        <v>1</v>
+      </c>
       <c r="AD36" s="8"/>
       <c r="AE36" s="8"/>
     </row>
     <row r="37" spans="1:31">
-      <c r="A37" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="B37" s="30"/>
-      <c r="C37" s="30"/>
-      <c r="D37" s="30"/>
-      <c r="E37" s="30"/>
-      <c r="F37" s="30"/>
-      <c r="G37" s="30"/>
-      <c r="H37" s="30"/>
-      <c r="I37" s="30"/>
-      <c r="J37" s="30"/>
-      <c r="K37" s="30"/>
-      <c r="L37" s="30"/>
-      <c r="M37" s="26"/>
+      <c r="A37" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B37" s="31"/>
+      <c r="C37" s="31"/>
+      <c r="D37" s="31"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
+      <c r="G37" s="31"/>
+      <c r="H37" s="31"/>
+      <c r="I37" s="31"/>
+      <c r="J37" s="31"/>
+      <c r="K37" s="31"/>
+      <c r="L37" s="31"/>
+      <c r="M37" s="26" t="s">
+        <v>32</v>
+      </c>
       <c r="N37" s="26"/>
       <c r="O37" s="26"/>
       <c r="P37" s="26"/>
-      <c r="Q37" s="8">
-        <v>2</v>
+      <c r="Q37" s="13">
+        <v>10</v>
       </c>
       <c r="R37" s="13">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="S37" s="13">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="T37" s="13">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="U37" s="13">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="V37" s="13">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="W37" s="13">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="X37" s="13">
-        <v>2</v>
-      </c>
-      <c r="Y37" s="8"/>
-      <c r="Z37" s="8"/>
-      <c r="AA37" s="8"/>
-      <c r="AB37" s="8"/>
-      <c r="AC37" s="8"/>
+        <v>10</v>
+      </c>
+      <c r="Y37" s="13">
+        <v>10</v>
+      </c>
+      <c r="Z37" s="13">
+        <v>10</v>
+      </c>
+      <c r="AA37" s="13">
+        <v>10</v>
+      </c>
+      <c r="AB37" s="13">
+        <v>10</v>
+      </c>
+      <c r="AC37" s="13">
+        <v>10</v>
+      </c>
       <c r="AD37" s="8"/>
       <c r="AE37" s="8"/>
     </row>
     <row r="38" spans="1:31">
-      <c r="A38" s="25"/>
-      <c r="B38" s="25"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="25"/>
-      <c r="G38" s="25"/>
-      <c r="H38" s="25"/>
-      <c r="I38" s="25"/>
-      <c r="J38" s="25"/>
-      <c r="K38" s="25"/>
-      <c r="L38" s="25"/>
+      <c r="A38" s="30" t="s">
+        <v>23</v>
+      </c>
+      <c r="B38" s="30"/>
+      <c r="C38" s="30"/>
+      <c r="D38" s="30"/>
+      <c r="E38" s="30"/>
+      <c r="F38" s="30"/>
+      <c r="G38" s="30"/>
+      <c r="H38" s="30"/>
+      <c r="I38" s="30"/>
+      <c r="J38" s="30"/>
+      <c r="K38" s="30"/>
+      <c r="L38" s="30"/>
       <c r="M38" s="26"/>
       <c r="N38" s="26"/>
       <c r="O38" s="26"/>
       <c r="P38" s="26"/>
-      <c r="Q38" s="8"/>
-      <c r="R38" s="8"/>
-      <c r="S38" s="8"/>
-      <c r="T38" s="8"/>
-      <c r="U38" s="8"/>
-      <c r="V38" s="8"/>
-      <c r="W38" s="8"/>
-      <c r="X38" s="8"/>
-      <c r="Y38" s="8"/>
-      <c r="Z38" s="8"/>
-      <c r="AA38" s="8"/>
-      <c r="AB38" s="8"/>
-      <c r="AC38" s="8"/>
+      <c r="Q38" s="8">
+        <v>3</v>
+      </c>
+      <c r="R38" s="13">
+        <v>3</v>
+      </c>
+      <c r="S38" s="13">
+        <v>3</v>
+      </c>
+      <c r="T38" s="13">
+        <v>3</v>
+      </c>
+      <c r="U38" s="13">
+        <v>3</v>
+      </c>
+      <c r="V38" s="13">
+        <v>3</v>
+      </c>
+      <c r="W38" s="13">
+        <v>3</v>
+      </c>
+      <c r="X38" s="13">
+        <v>3</v>
+      </c>
+      <c r="Y38" s="13">
+        <v>3</v>
+      </c>
+      <c r="Z38" s="13">
+        <v>3</v>
+      </c>
+      <c r="AA38" s="13">
+        <v>3</v>
+      </c>
+      <c r="AB38" s="13">
+        <v>3</v>
+      </c>
+      <c r="AC38" s="13">
+        <v>3</v>
+      </c>
       <c r="AD38" s="8"/>
       <c r="AE38" s="8"/>
     </row>
     <row r="39" spans="1:31">
-      <c r="A39" s="25"/>
-      <c r="B39" s="25"/>
-      <c r="C39" s="25"/>
-      <c r="D39" s="25"/>
-      <c r="E39" s="25"/>
-      <c r="F39" s="25"/>
-      <c r="G39" s="25"/>
-      <c r="H39" s="25"/>
-      <c r="I39" s="25"/>
-      <c r="J39" s="25"/>
-      <c r="K39" s="25"/>
-      <c r="L39" s="25"/>
+      <c r="A39" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="B39" s="30"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="30"/>
+      <c r="E39" s="30"/>
+      <c r="F39" s="30"/>
+      <c r="G39" s="30"/>
+      <c r="H39" s="30"/>
+      <c r="I39" s="30"/>
+      <c r="J39" s="30"/>
+      <c r="K39" s="30"/>
+      <c r="L39" s="30"/>
       <c r="M39" s="26"/>
       <c r="N39" s="26"/>
       <c r="O39" s="26"/>
       <c r="P39" s="26"/>
-      <c r="Q39" s="8"/>
-      <c r="R39" s="8"/>
-      <c r="S39" s="8"/>
-      <c r="T39" s="8"/>
-      <c r="U39" s="8"/>
-      <c r="V39" s="8"/>
-      <c r="W39" s="8"/>
-      <c r="X39" s="8"/>
-      <c r="Y39" s="8"/>
-      <c r="Z39" s="8"/>
-      <c r="AA39" s="8"/>
-      <c r="AB39" s="8"/>
-      <c r="AC39" s="8"/>
+      <c r="Q39" s="8">
+        <v>2</v>
+      </c>
+      <c r="R39" s="13">
+        <v>2</v>
+      </c>
+      <c r="S39" s="13">
+        <v>2</v>
+      </c>
+      <c r="T39" s="13">
+        <v>2</v>
+      </c>
+      <c r="U39" s="13">
+        <v>2</v>
+      </c>
+      <c r="V39" s="13">
+        <v>2</v>
+      </c>
+      <c r="W39" s="13">
+        <v>2</v>
+      </c>
+      <c r="X39" s="13">
+        <v>2</v>
+      </c>
+      <c r="Y39" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z39" s="13">
+        <v>2</v>
+      </c>
+      <c r="AA39" s="13">
+        <v>2</v>
+      </c>
+      <c r="AB39" s="13">
+        <v>2</v>
+      </c>
+      <c r="AC39" s="13">
+        <v>2</v>
+      </c>
       <c r="AD39" s="8"/>
       <c r="AE39" s="8"/>
     </row>
     <row r="40" spans="1:31">
-      <c r="A40" s="25"/>
-      <c r="B40" s="25"/>
-      <c r="C40" s="25"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="25"/>
-      <c r="G40" s="25"/>
-      <c r="H40" s="25"/>
-      <c r="I40" s="25"/>
-      <c r="J40" s="25"/>
-      <c r="K40" s="25"/>
-      <c r="L40" s="25"/>
+      <c r="A40" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B40" s="30"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="30"/>
+      <c r="E40" s="30"/>
+      <c r="F40" s="30"/>
+      <c r="G40" s="30"/>
+      <c r="H40" s="30"/>
+      <c r="I40" s="30"/>
+      <c r="J40" s="30"/>
+      <c r="K40" s="30"/>
+      <c r="L40" s="30"/>
       <c r="M40" s="26"/>
       <c r="N40" s="26"/>
       <c r="O40" s="26"/>
       <c r="P40" s="26"/>
-      <c r="Q40" s="8"/>
-      <c r="R40" s="8"/>
-      <c r="S40" s="8"/>
-      <c r="T40" s="8"/>
-      <c r="U40" s="8"/>
-      <c r="V40" s="8"/>
-      <c r="W40" s="8"/>
-      <c r="X40" s="8"/>
-      <c r="Y40" s="8"/>
-      <c r="Z40" s="8"/>
-      <c r="AA40" s="8"/>
-      <c r="AB40" s="8"/>
-      <c r="AC40" s="8"/>
+      <c r="Q40" s="8">
+        <v>2</v>
+      </c>
+      <c r="R40" s="13">
+        <v>2</v>
+      </c>
+      <c r="S40" s="13">
+        <v>2</v>
+      </c>
+      <c r="T40" s="13">
+        <v>2</v>
+      </c>
+      <c r="U40" s="13">
+        <v>2</v>
+      </c>
+      <c r="V40" s="13">
+        <v>2</v>
+      </c>
+      <c r="W40" s="13">
+        <v>2</v>
+      </c>
+      <c r="X40" s="13">
+        <v>2</v>
+      </c>
+      <c r="Y40" s="13">
+        <v>2</v>
+      </c>
+      <c r="Z40" s="13">
+        <v>2</v>
+      </c>
+      <c r="AA40" s="13">
+        <v>2</v>
+      </c>
+      <c r="AB40" s="13">
+        <v>2</v>
+      </c>
+      <c r="AC40" s="13">
+        <v>2</v>
+      </c>
       <c r="AD40" s="8"/>
       <c r="AE40" s="8"/>
     </row>
@@ -3026,8 +3349,109 @@
       <c r="AD51" s="8"/>
       <c r="AE51" s="8"/>
     </row>
+    <row r="52" spans="1:31">
+      <c r="A52" s="25"/>
+      <c r="B52" s="25"/>
+      <c r="C52" s="25"/>
+      <c r="D52" s="25"/>
+      <c r="E52" s="25"/>
+      <c r="F52" s="25"/>
+      <c r="G52" s="25"/>
+      <c r="H52" s="25"/>
+      <c r="I52" s="25"/>
+      <c r="J52" s="25"/>
+      <c r="K52" s="25"/>
+      <c r="L52" s="25"/>
+      <c r="M52" s="26"/>
+      <c r="N52" s="26"/>
+      <c r="O52" s="26"/>
+      <c r="P52" s="26"/>
+      <c r="Q52" s="8"/>
+      <c r="R52" s="8"/>
+      <c r="S52" s="8"/>
+      <c r="T52" s="8"/>
+      <c r="U52" s="8"/>
+      <c r="V52" s="8"/>
+      <c r="W52" s="8"/>
+      <c r="X52" s="8"/>
+      <c r="Y52" s="8"/>
+      <c r="Z52" s="8"/>
+      <c r="AA52" s="8"/>
+      <c r="AB52" s="8"/>
+      <c r="AC52" s="8"/>
+      <c r="AD52" s="8"/>
+      <c r="AE52" s="8"/>
+    </row>
+    <row r="53" spans="1:31">
+      <c r="A53" s="25"/>
+      <c r="B53" s="25"/>
+      <c r="C53" s="25"/>
+      <c r="D53" s="25"/>
+      <c r="E53" s="25"/>
+      <c r="F53" s="25"/>
+      <c r="G53" s="25"/>
+      <c r="H53" s="25"/>
+      <c r="I53" s="25"/>
+      <c r="J53" s="25"/>
+      <c r="K53" s="25"/>
+      <c r="L53" s="25"/>
+      <c r="M53" s="26"/>
+      <c r="N53" s="26"/>
+      <c r="O53" s="26"/>
+      <c r="P53" s="26"/>
+      <c r="Q53" s="8"/>
+      <c r="R53" s="8"/>
+      <c r="S53" s="8"/>
+      <c r="T53" s="8"/>
+      <c r="U53" s="8"/>
+      <c r="V53" s="8"/>
+      <c r="W53" s="8"/>
+      <c r="X53" s="8"/>
+      <c r="Y53" s="8"/>
+      <c r="Z53" s="8"/>
+      <c r="AA53" s="8"/>
+      <c r="AB53" s="8"/>
+      <c r="AC53" s="8"/>
+      <c r="AD53" s="8"/>
+      <c r="AE53" s="8"/>
+    </row>
+    <row r="54" spans="1:31">
+      <c r="A54" s="25"/>
+      <c r="B54" s="25"/>
+      <c r="C54" s="25"/>
+      <c r="D54" s="25"/>
+      <c r="E54" s="25"/>
+      <c r="F54" s="25"/>
+      <c r="G54" s="25"/>
+      <c r="H54" s="25"/>
+      <c r="I54" s="25"/>
+      <c r="J54" s="25"/>
+      <c r="K54" s="25"/>
+      <c r="L54" s="25"/>
+      <c r="M54" s="26"/>
+      <c r="N54" s="26"/>
+      <c r="O54" s="26"/>
+      <c r="P54" s="26"/>
+      <c r="Q54" s="8"/>
+      <c r="R54" s="8"/>
+      <c r="S54" s="8"/>
+      <c r="T54" s="8"/>
+      <c r="U54" s="8"/>
+      <c r="V54" s="8"/>
+      <c r="W54" s="8"/>
+      <c r="X54" s="8"/>
+      <c r="Y54" s="8"/>
+      <c r="Z54" s="8"/>
+      <c r="AA54" s="8"/>
+      <c r="AB54" s="8"/>
+      <c r="AC54" s="8"/>
+      <c r="AD54" s="8"/>
+      <c r="AE54" s="8"/>
+    </row>
   </sheetData>
-  <mergeCells count="65">
+  <mergeCells count="71">
+    <mergeCell ref="A37:L37"/>
+    <mergeCell ref="M37:P37"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="G1:J1"/>
     <mergeCell ref="M19:P21"/>
@@ -3052,14 +3476,12 @@
     <mergeCell ref="M32:P32"/>
     <mergeCell ref="A33:L33"/>
     <mergeCell ref="M33:P33"/>
+    <mergeCell ref="A36:L36"/>
+    <mergeCell ref="M36:P36"/>
     <mergeCell ref="A34:L34"/>
     <mergeCell ref="M34:P34"/>
     <mergeCell ref="A35:L35"/>
     <mergeCell ref="M35:P35"/>
-    <mergeCell ref="A36:L36"/>
-    <mergeCell ref="M36:P36"/>
-    <mergeCell ref="A37:L37"/>
-    <mergeCell ref="M37:P37"/>
     <mergeCell ref="A38:L38"/>
     <mergeCell ref="M38:P38"/>
     <mergeCell ref="A39:L39"/>
@@ -3072,27 +3494,33 @@
     <mergeCell ref="M42:P42"/>
     <mergeCell ref="A43:L43"/>
     <mergeCell ref="M43:P43"/>
+    <mergeCell ref="A44:L44"/>
     <mergeCell ref="M44:P44"/>
     <mergeCell ref="A45:L45"/>
     <mergeCell ref="M45:P45"/>
     <mergeCell ref="A46:L46"/>
     <mergeCell ref="M46:P46"/>
-    <mergeCell ref="Q19:AZ19"/>
-    <mergeCell ref="A50:L50"/>
-    <mergeCell ref="M50:P50"/>
-    <mergeCell ref="A51:L51"/>
-    <mergeCell ref="M51:P51"/>
-    <mergeCell ref="A29:L29"/>
-    <mergeCell ref="M29:P29"/>
-    <mergeCell ref="M25:P25"/>
-    <mergeCell ref="A25:L25"/>
-    <mergeCell ref="A47:L47"/>
     <mergeCell ref="M47:P47"/>
     <mergeCell ref="A48:L48"/>
     <mergeCell ref="M48:P48"/>
     <mergeCell ref="A49:L49"/>
     <mergeCell ref="M49:P49"/>
-    <mergeCell ref="A44:L44"/>
+    <mergeCell ref="Q19:AZ19"/>
+    <mergeCell ref="A53:L53"/>
+    <mergeCell ref="M53:P53"/>
+    <mergeCell ref="A54:L54"/>
+    <mergeCell ref="M54:P54"/>
+    <mergeCell ref="A29:L29"/>
+    <mergeCell ref="M29:P29"/>
+    <mergeCell ref="M25:P25"/>
+    <mergeCell ref="A25:L25"/>
+    <mergeCell ref="A50:L50"/>
+    <mergeCell ref="M50:P50"/>
+    <mergeCell ref="A51:L51"/>
+    <mergeCell ref="M51:P51"/>
+    <mergeCell ref="A52:L52"/>
+    <mergeCell ref="M52:P52"/>
+    <mergeCell ref="A47:L47"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3109,7 +3537,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:AF35"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
+    <sheetView showRuler="0" view="pageLayout" workbookViewId="0">
       <selection activeCell="G1" sqref="G1:J1"/>
     </sheetView>
   </sheetViews>
@@ -4410,7 +4838,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:AF35"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
+    <sheetView showRuler="0" view="pageLayout" workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
App Database, Burn Down, & Agendas
I fixed the form, and the database is now up and running. I updated the
burn down chart, and created two new agendas.
</commit_message>
<xml_diff>
--- a/Burn Down Chart.xlsx
+++ b/Burn Down Chart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15960" windowHeight="15320" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20900" windowHeight="15320" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Iteration 1" sheetId="1" r:id="rId1"/>
@@ -686,33 +686,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -738,14 +716,36 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -949,27 +949,30 @@
                 <c:pt idx="18">
                   <c:v>37.0</c:v>
                 </c:pt>
+                <c:pt idx="19">
+                  <c:v>26.0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="341794968"/>
-        <c:axId val="341798072"/>
+        <c:axId val="312750216"/>
+        <c:axId val="312752920"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="341794968"/>
+        <c:axId val="312750216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="341798072"/>
+        <c:crossAx val="312752920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="341798072"/>
+        <c:axId val="312752920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -977,7 +980,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="341794968"/>
+        <c:crossAx val="312750216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1353,23 +1356,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:AZ54"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:L37"/>
+    <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
+      <selection activeCell="AO30" sqref="AO30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.140625" defaultRowHeight="13"/>
   <sheetData>
     <row r="1" spans="1:16">
-      <c r="A1" s="32"/>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
+      <c r="A1" s="24"/>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -1684,82 +1687,82 @@
       <c r="P18" s="1"/>
     </row>
     <row r="19" spans="1:52" ht="14" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A19" s="37" t="s">
+      <c r="A19" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="34"/>
-      <c r="C19" s="34"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
-      <c r="K19" s="34"/>
-      <c r="L19" s="34"/>
-      <c r="M19" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="N19" s="34"/>
-      <c r="O19" s="34"/>
-      <c r="P19" s="34"/>
-      <c r="Q19" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="R19" s="23"/>
-      <c r="S19" s="23"/>
-      <c r="T19" s="23"/>
-      <c r="U19" s="23"/>
-      <c r="V19" s="23"/>
-      <c r="W19" s="23"/>
-      <c r="X19" s="23"/>
-      <c r="Y19" s="23"/>
-      <c r="Z19" s="23"/>
-      <c r="AA19" s="23"/>
-      <c r="AB19" s="23"/>
-      <c r="AC19" s="23"/>
-      <c r="AD19" s="23"/>
-      <c r="AE19" s="23"/>
-      <c r="AF19" s="23"/>
-      <c r="AG19" s="23"/>
-      <c r="AH19" s="23"/>
-      <c r="AI19" s="23"/>
-      <c r="AJ19" s="23"/>
-      <c r="AK19" s="23"/>
-      <c r="AL19" s="23"/>
-      <c r="AM19" s="23"/>
-      <c r="AN19" s="23"/>
-      <c r="AO19" s="23"/>
-      <c r="AP19" s="23"/>
-      <c r="AQ19" s="23"/>
-      <c r="AR19" s="23"/>
-      <c r="AS19" s="23"/>
-      <c r="AT19" s="23"/>
-      <c r="AU19" s="23"/>
-      <c r="AV19" s="23"/>
-      <c r="AW19" s="23"/>
-      <c r="AX19" s="23"/>
-      <c r="AY19" s="23"/>
-      <c r="AZ19" s="24"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="26"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
+      <c r="J19" s="26"/>
+      <c r="K19" s="26"/>
+      <c r="L19" s="26"/>
+      <c r="M19" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="N19" s="26"/>
+      <c r="O19" s="26"/>
+      <c r="P19" s="26"/>
+      <c r="Q19" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="R19" s="36"/>
+      <c r="S19" s="36"/>
+      <c r="T19" s="36"/>
+      <c r="U19" s="36"/>
+      <c r="V19" s="36"/>
+      <c r="W19" s="36"/>
+      <c r="X19" s="36"/>
+      <c r="Y19" s="36"/>
+      <c r="Z19" s="36"/>
+      <c r="AA19" s="36"/>
+      <c r="AB19" s="36"/>
+      <c r="AC19" s="36"/>
+      <c r="AD19" s="36"/>
+      <c r="AE19" s="36"/>
+      <c r="AF19" s="36"/>
+      <c r="AG19" s="36"/>
+      <c r="AH19" s="36"/>
+      <c r="AI19" s="36"/>
+      <c r="AJ19" s="36"/>
+      <c r="AK19" s="36"/>
+      <c r="AL19" s="36"/>
+      <c r="AM19" s="36"/>
+      <c r="AN19" s="36"/>
+      <c r="AO19" s="36"/>
+      <c r="AP19" s="36"/>
+      <c r="AQ19" s="36"/>
+      <c r="AR19" s="36"/>
+      <c r="AS19" s="36"/>
+      <c r="AT19" s="36"/>
+      <c r="AU19" s="36"/>
+      <c r="AV19" s="36"/>
+      <c r="AW19" s="36"/>
+      <c r="AX19" s="36"/>
+      <c r="AY19" s="36"/>
+      <c r="AZ19" s="37"/>
     </row>
     <row r="20" spans="1:52">
-      <c r="A20" s="38"/>
-      <c r="B20" s="35"/>
-      <c r="C20" s="35"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="35"/>
-      <c r="F20" s="35"/>
-      <c r="G20" s="35"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="35"/>
-      <c r="J20" s="35"/>
-      <c r="K20" s="35"/>
-      <c r="L20" s="35"/>
-      <c r="M20" s="35"/>
-      <c r="N20" s="35"/>
-      <c r="O20" s="35"/>
-      <c r="P20" s="35"/>
+      <c r="A20" s="30"/>
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="27"/>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="27"/>
+      <c r="N20" s="27"/>
+      <c r="O20" s="27"/>
+      <c r="P20" s="27"/>
       <c r="Q20" s="3">
         <v>0</v>
       </c>
@@ -1870,22 +1873,22 @@
       </c>
     </row>
     <row r="21" spans="1:52" ht="14" thickBot="1">
-      <c r="A21" s="39"/>
-      <c r="B21" s="36"/>
-      <c r="C21" s="36"/>
-      <c r="D21" s="36"/>
-      <c r="E21" s="36"/>
-      <c r="F21" s="36"/>
-      <c r="G21" s="36"/>
-      <c r="H21" s="36"/>
-      <c r="I21" s="36"/>
-      <c r="J21" s="36"/>
-      <c r="K21" s="36"/>
-      <c r="L21" s="36"/>
-      <c r="M21" s="36"/>
-      <c r="N21" s="36"/>
-      <c r="O21" s="36"/>
-      <c r="P21" s="36"/>
+      <c r="A21" s="31"/>
+      <c r="B21" s="28"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="28"/>
+      <c r="M21" s="28"/>
+      <c r="N21" s="28"/>
+      <c r="O21" s="28"/>
+      <c r="P21" s="28"/>
       <c r="Q21" s="17">
         <f t="shared" ref="Q21:W21" si="0">SUM(Q22:Q54)</f>
         <v>70</v>
@@ -1915,7 +1918,7 @@
         <v>47</v>
       </c>
       <c r="X21" s="18">
-        <f t="shared" ref="X21:AI21" si="1">SUM(X22:X54)</f>
+        <f t="shared" ref="X21:AJ21" si="1">SUM(X22:X54)</f>
         <v>41</v>
       </c>
       <c r="Y21" s="18">
@@ -1962,7 +1965,10 @@
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="AJ21" s="18"/>
+      <c r="AJ21" s="18">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
       <c r="AK21" s="18"/>
       <c r="AL21" s="18"/>
       <c r="AM21" s="18"/>
@@ -1981,26 +1987,26 @@
       <c r="AZ21" s="21"/>
     </row>
     <row r="22" spans="1:52">
-      <c r="A22" s="29" t="s">
+      <c r="A22" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="29"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29"/>
-      <c r="E22" s="29"/>
-      <c r="F22" s="29"/>
-      <c r="G22" s="29"/>
-      <c r="H22" s="29"/>
-      <c r="I22" s="29"/>
-      <c r="J22" s="29"/>
-      <c r="K22" s="29"/>
-      <c r="L22" s="29"/>
-      <c r="M22" s="26" t="s">
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
+      <c r="H22" s="32"/>
+      <c r="I22" s="32"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="32"/>
+      <c r="L22" s="32"/>
+      <c r="M22" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="N22" s="26"/>
-      <c r="O22" s="26"/>
-      <c r="P22" s="26"/>
+      <c r="N22" s="23"/>
+      <c r="O22" s="23"/>
+      <c r="P22" s="23"/>
       <c r="Q22" s="8">
         <v>3</v>
       </c>
@@ -2058,28 +2064,31 @@
       <c r="AI22">
         <v>0</v>
       </c>
+      <c r="AJ22">
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:52">
-      <c r="A23" s="29" t="s">
+      <c r="A23" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="B23" s="29"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="29"/>
-      <c r="F23" s="29"/>
-      <c r="G23" s="29"/>
-      <c r="H23" s="29"/>
-      <c r="I23" s="29"/>
-      <c r="J23" s="29"/>
-      <c r="K23" s="29"/>
-      <c r="L23" s="29"/>
-      <c r="M23" s="26" t="s">
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="32"/>
+      <c r="H23" s="32"/>
+      <c r="I23" s="32"/>
+      <c r="J23" s="32"/>
+      <c r="K23" s="32"/>
+      <c r="L23" s="32"/>
+      <c r="M23" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="N23" s="26"/>
-      <c r="O23" s="26"/>
-      <c r="P23" s="26"/>
+      <c r="N23" s="23"/>
+      <c r="O23" s="23"/>
+      <c r="P23" s="23"/>
       <c r="Q23" s="8">
         <v>10</v>
       </c>
@@ -2137,28 +2146,32 @@
       <c r="AI23" s="13">
         <v>0</v>
       </c>
+      <c r="AJ23" s="13">
+        <v>0</v>
+      </c>
+      <c r="AK23" s="13"/>
     </row>
     <row r="24" spans="1:52">
-      <c r="A24" s="29" t="s">
+      <c r="A24" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B24" s="29"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
-      <c r="E24" s="29"/>
-      <c r="F24" s="29"/>
-      <c r="G24" s="29"/>
-      <c r="H24" s="29"/>
-      <c r="I24" s="29"/>
-      <c r="J24" s="29"/>
-      <c r="K24" s="29"/>
-      <c r="L24" s="29"/>
-      <c r="M24" s="26" t="s">
+      <c r="B24" s="32"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="32"/>
+      <c r="L24" s="32"/>
+      <c r="M24" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="N24" s="26"/>
-      <c r="O24" s="26"/>
-      <c r="P24" s="26"/>
+      <c r="N24" s="23"/>
+      <c r="O24" s="23"/>
+      <c r="P24" s="23"/>
       <c r="Q24" s="8">
         <v>7</v>
       </c>
@@ -2216,28 +2229,32 @@
       <c r="AI24" s="13">
         <v>0</v>
       </c>
+      <c r="AJ24" s="13">
+        <v>0</v>
+      </c>
+      <c r="AK24" s="13"/>
     </row>
     <row r="25" spans="1:52">
-      <c r="A25" s="29" t="s">
+      <c r="A25" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="29"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="29"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="29"/>
-      <c r="I25" s="29"/>
-      <c r="J25" s="29"/>
-      <c r="K25" s="29"/>
-      <c r="L25" s="29"/>
-      <c r="M25" s="26" t="s">
+      <c r="B25" s="32"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
+      <c r="H25" s="32"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="32"/>
+      <c r="L25" s="32"/>
+      <c r="M25" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="N25" s="26"/>
-      <c r="O25" s="26"/>
-      <c r="P25" s="26"/>
+      <c r="N25" s="23"/>
+      <c r="O25" s="23"/>
+      <c r="P25" s="23"/>
       <c r="Q25" s="13">
         <v>3</v>
       </c>
@@ -2295,28 +2312,32 @@
       <c r="AI25" s="13">
         <v>0</v>
       </c>
+      <c r="AJ25" s="13">
+        <v>0</v>
+      </c>
+      <c r="AK25" s="13"/>
     </row>
     <row r="26" spans="1:52">
-      <c r="A26" s="29" t="s">
+      <c r="A26" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="B26" s="29"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29"/>
-      <c r="E26" s="29"/>
-      <c r="F26" s="29"/>
-      <c r="G26" s="29"/>
-      <c r="H26" s="29"/>
-      <c r="I26" s="29"/>
-      <c r="J26" s="29"/>
-      <c r="K26" s="29"/>
-      <c r="L26" s="29"/>
-      <c r="M26" s="26" t="s">
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
+      <c r="H26" s="32"/>
+      <c r="I26" s="32"/>
+      <c r="J26" s="32"/>
+      <c r="K26" s="32"/>
+      <c r="L26" s="32"/>
+      <c r="M26" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="N26" s="26"/>
-      <c r="O26" s="26"/>
-      <c r="P26" s="26"/>
+      <c r="N26" s="23"/>
+      <c r="O26" s="23"/>
+      <c r="P26" s="23"/>
       <c r="Q26" s="13">
         <v>2</v>
       </c>
@@ -2374,28 +2395,32 @@
       <c r="AI26" s="13">
         <v>0</v>
       </c>
+      <c r="AJ26" s="13">
+        <v>0</v>
+      </c>
+      <c r="AK26" s="13"/>
     </row>
     <row r="27" spans="1:52">
-      <c r="A27" s="29" t="s">
+      <c r="A27" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="B27" s="29"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
-      <c r="E27" s="29"/>
-      <c r="F27" s="29"/>
-      <c r="G27" s="29"/>
-      <c r="H27" s="29"/>
-      <c r="I27" s="29"/>
-      <c r="J27" s="29"/>
-      <c r="K27" s="29"/>
-      <c r="L27" s="29"/>
-      <c r="M27" s="26" t="s">
+      <c r="B27" s="32"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
+      <c r="H27" s="32"/>
+      <c r="I27" s="32"/>
+      <c r="J27" s="32"/>
+      <c r="K27" s="32"/>
+      <c r="L27" s="32"/>
+      <c r="M27" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="N27" s="26"/>
-      <c r="O27" s="26"/>
-      <c r="P27" s="26"/>
+      <c r="N27" s="23"/>
+      <c r="O27" s="23"/>
+      <c r="P27" s="23"/>
       <c r="Q27" s="13">
         <v>3</v>
       </c>
@@ -2453,28 +2478,32 @@
       <c r="AI27" s="13">
         <v>0</v>
       </c>
+      <c r="AJ27" s="13">
+        <v>0</v>
+      </c>
+      <c r="AK27" s="13"/>
     </row>
     <row r="28" spans="1:52">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
-      <c r="K28" s="29"/>
-      <c r="L28" s="29"/>
-      <c r="M28" s="26" t="s">
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
+      <c r="H28" s="32"/>
+      <c r="I28" s="32"/>
+      <c r="J28" s="32"/>
+      <c r="K28" s="32"/>
+      <c r="L28" s="32"/>
+      <c r="M28" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="N28" s="26"/>
-      <c r="O28" s="26"/>
-      <c r="P28" s="26"/>
+      <c r="N28" s="23"/>
+      <c r="O28" s="23"/>
+      <c r="P28" s="23"/>
       <c r="Q28" s="13">
         <v>1</v>
       </c>
@@ -2532,28 +2561,32 @@
       <c r="AI28" s="13">
         <v>0</v>
       </c>
+      <c r="AJ28" s="13">
+        <v>0</v>
+      </c>
+      <c r="AK28" s="13"/>
     </row>
     <row r="29" spans="1:52">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B29" s="27"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
-      <c r="K29" s="27"/>
-      <c r="L29" s="27"/>
-      <c r="M29" s="28" t="s">
+      <c r="B29" s="38"/>
+      <c r="C29" s="38"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="38"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="38"/>
+      <c r="I29" s="38"/>
+      <c r="J29" s="38"/>
+      <c r="K29" s="38"/>
+      <c r="L29" s="38"/>
+      <c r="M29" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="N29" s="28"/>
-      <c r="O29" s="28"/>
-      <c r="P29" s="28"/>
+      <c r="N29" s="39"/>
+      <c r="O29" s="39"/>
+      <c r="P29" s="39"/>
       <c r="Q29" s="13">
         <v>2</v>
       </c>
@@ -2611,28 +2644,32 @@
       <c r="AI29" s="13">
         <v>1</v>
       </c>
+      <c r="AJ29" s="13">
+        <v>0</v>
+      </c>
+      <c r="AK29" s="13"/>
     </row>
     <row r="30" spans="1:52">
-      <c r="A30" s="31" t="s">
+      <c r="A30" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="31"/>
-      <c r="G30" s="31"/>
-      <c r="H30" s="31"/>
-      <c r="I30" s="31"/>
-      <c r="J30" s="31"/>
-      <c r="K30" s="31"/>
-      <c r="L30" s="31"/>
-      <c r="M30" s="26" t="s">
+      <c r="B30" s="22"/>
+      <c r="C30" s="22"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+      <c r="G30" s="22"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="22"/>
+      <c r="J30" s="22"/>
+      <c r="K30" s="22"/>
+      <c r="L30" s="22"/>
+      <c r="M30" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="N30" s="26"/>
-      <c r="O30" s="26"/>
-      <c r="P30" s="26"/>
+      <c r="N30" s="23"/>
+      <c r="O30" s="23"/>
+      <c r="P30" s="23"/>
       <c r="Q30" s="13">
         <v>3</v>
       </c>
@@ -2690,28 +2727,32 @@
       <c r="AI30" s="13">
         <v>3</v>
       </c>
+      <c r="AJ30" s="13">
+        <v>2</v>
+      </c>
+      <c r="AK30" s="13"/>
     </row>
     <row r="31" spans="1:52">
-      <c r="A31" s="31" t="s">
+      <c r="A31" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="31"/>
-      <c r="F31" s="31"/>
-      <c r="G31" s="31"/>
-      <c r="H31" s="31"/>
-      <c r="I31" s="31"/>
-      <c r="J31" s="31"/>
-      <c r="K31" s="31"/>
-      <c r="L31" s="31"/>
-      <c r="M31" s="26" t="s">
+      <c r="B31" s="22"/>
+      <c r="C31" s="22"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="22"/>
+      <c r="G31" s="22"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="22"/>
+      <c r="J31" s="22"/>
+      <c r="K31" s="22"/>
+      <c r="L31" s="22"/>
+      <c r="M31" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="N31" s="26"/>
-      <c r="O31" s="26"/>
-      <c r="P31" s="26"/>
+      <c r="N31" s="23"/>
+      <c r="O31" s="23"/>
+      <c r="P31" s="23"/>
       <c r="Q31" s="13">
         <v>3</v>
       </c>
@@ -2769,28 +2810,32 @@
       <c r="AI31" s="13">
         <v>3</v>
       </c>
+      <c r="AJ31" s="13">
+        <v>3</v>
+      </c>
+      <c r="AK31" s="13"/>
     </row>
     <row r="32" spans="1:52">
-      <c r="A32" s="31" t="s">
+      <c r="A32" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="B32" s="31"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="31"/>
-      <c r="E32" s="31"/>
-      <c r="F32" s="31"/>
-      <c r="G32" s="31"/>
-      <c r="H32" s="31"/>
-      <c r="I32" s="31"/>
-      <c r="J32" s="31"/>
-      <c r="K32" s="31"/>
-      <c r="L32" s="31"/>
-      <c r="M32" s="26" t="s">
+      <c r="B32" s="22"/>
+      <c r="C32" s="22"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22"/>
+      <c r="F32" s="22"/>
+      <c r="G32" s="22"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="22"/>
+      <c r="J32" s="22"/>
+      <c r="K32" s="22"/>
+      <c r="L32" s="22"/>
+      <c r="M32" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="N32" s="26"/>
-      <c r="O32" s="26"/>
-      <c r="P32" s="26"/>
+      <c r="N32" s="23"/>
+      <c r="O32" s="23"/>
+      <c r="P32" s="23"/>
       <c r="Q32" s="8">
         <v>7</v>
       </c>
@@ -2848,28 +2893,32 @@
       <c r="AI32" s="13">
         <v>6</v>
       </c>
-    </row>
-    <row r="33" spans="1:35">
-      <c r="A33" s="31" t="s">
+      <c r="AJ32" s="13">
+        <v>5</v>
+      </c>
+      <c r="AK32" s="13"/>
+    </row>
+    <row r="33" spans="1:36">
+      <c r="A33" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="B33" s="31"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="31"/>
-      <c r="G33" s="31"/>
-      <c r="H33" s="31"/>
-      <c r="I33" s="31"/>
-      <c r="J33" s="31"/>
-      <c r="K33" s="31"/>
-      <c r="L33" s="31"/>
-      <c r="M33" s="26" t="s">
+      <c r="B33" s="22"/>
+      <c r="C33" s="22"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22"/>
+      <c r="F33" s="22"/>
+      <c r="G33" s="22"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="22"/>
+      <c r="J33" s="22"/>
+      <c r="K33" s="22"/>
+      <c r="L33" s="22"/>
+      <c r="M33" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="N33" s="26"/>
-      <c r="O33" s="26"/>
-      <c r="P33" s="26"/>
+      <c r="N33" s="23"/>
+      <c r="O33" s="23"/>
+      <c r="P33" s="23"/>
       <c r="Q33" s="8">
         <v>2</v>
       </c>
@@ -2927,28 +2976,31 @@
       <c r="AI33" s="13">
         <v>2</v>
       </c>
-    </row>
-    <row r="34" spans="1:35">
-      <c r="A34" s="31" t="s">
+      <c r="AJ33" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:36">
+      <c r="A34" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="31"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31"/>
-      <c r="E34" s="31"/>
-      <c r="F34" s="31"/>
-      <c r="G34" s="31"/>
-      <c r="H34" s="31"/>
-      <c r="I34" s="31"/>
-      <c r="J34" s="31"/>
-      <c r="K34" s="31"/>
-      <c r="L34" s="31"/>
-      <c r="M34" s="26" t="s">
+      <c r="B34" s="22"/>
+      <c r="C34" s="22"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="22"/>
+      <c r="G34" s="22"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="22"/>
+      <c r="J34" s="22"/>
+      <c r="K34" s="22"/>
+      <c r="L34" s="22"/>
+      <c r="M34" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="N34" s="26"/>
-      <c r="O34" s="26"/>
-      <c r="P34" s="26"/>
+      <c r="N34" s="23"/>
+      <c r="O34" s="23"/>
+      <c r="P34" s="23"/>
       <c r="Q34" s="13">
         <v>1</v>
       </c>
@@ -3006,28 +3058,31 @@
       <c r="AI34" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:35">
-      <c r="A35" s="31" t="s">
+      <c r="AJ34" s="13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:36">
+      <c r="A35" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="B35" s="31"/>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="31"/>
-      <c r="G35" s="31"/>
-      <c r="H35" s="31"/>
-      <c r="I35" s="31"/>
-      <c r="J35" s="31"/>
-      <c r="K35" s="31"/>
-      <c r="L35" s="31"/>
-      <c r="M35" s="26" t="s">
+      <c r="B35" s="22"/>
+      <c r="C35" s="22"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="22"/>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="22"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="22"/>
+      <c r="L35" s="22"/>
+      <c r="M35" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="N35" s="26"/>
-      <c r="O35" s="26"/>
-      <c r="P35" s="26"/>
+      <c r="N35" s="23"/>
+      <c r="O35" s="23"/>
+      <c r="P35" s="23"/>
       <c r="Q35" s="13">
         <v>5</v>
       </c>
@@ -3085,28 +3140,31 @@
       <c r="AI35" s="13">
         <v>4</v>
       </c>
-    </row>
-    <row r="36" spans="1:35">
-      <c r="A36" s="31" t="s">
+      <c r="AJ35" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:36">
+      <c r="A36" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="B36" s="31"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="31"/>
-      <c r="F36" s="31"/>
-      <c r="G36" s="31"/>
-      <c r="H36" s="31"/>
-      <c r="I36" s="31"/>
-      <c r="J36" s="31"/>
-      <c r="K36" s="31"/>
-      <c r="L36" s="31"/>
-      <c r="M36" s="26" t="s">
+      <c r="B36" s="22"/>
+      <c r="C36" s="22"/>
+      <c r="D36" s="22"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="22"/>
+      <c r="G36" s="22"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="22"/>
+      <c r="J36" s="22"/>
+      <c r="K36" s="22"/>
+      <c r="L36" s="22"/>
+      <c r="M36" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="N36" s="26"/>
-      <c r="O36" s="26"/>
-      <c r="P36" s="26"/>
+      <c r="N36" s="23"/>
+      <c r="O36" s="23"/>
+      <c r="P36" s="23"/>
       <c r="Q36" s="8">
         <v>1</v>
       </c>
@@ -3164,28 +3222,31 @@
       <c r="AI36" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:35">
-      <c r="A37" s="31" t="s">
+      <c r="AJ36" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:36">
+      <c r="A37" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="B37" s="31"/>
-      <c r="C37" s="31"/>
-      <c r="D37" s="31"/>
-      <c r="E37" s="31"/>
-      <c r="F37" s="31"/>
-      <c r="G37" s="31"/>
-      <c r="H37" s="31"/>
-      <c r="I37" s="31"/>
-      <c r="J37" s="31"/>
-      <c r="K37" s="31"/>
-      <c r="L37" s="31"/>
-      <c r="M37" s="26" t="s">
+      <c r="B37" s="22"/>
+      <c r="C37" s="22"/>
+      <c r="D37" s="22"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="22"/>
+      <c r="G37" s="22"/>
+      <c r="H37" s="22"/>
+      <c r="I37" s="22"/>
+      <c r="J37" s="22"/>
+      <c r="K37" s="22"/>
+      <c r="L37" s="22"/>
+      <c r="M37" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="N37" s="26"/>
-      <c r="O37" s="26"/>
-      <c r="P37" s="26"/>
+      <c r="N37" s="23"/>
+      <c r="O37" s="23"/>
+      <c r="P37" s="23"/>
       <c r="Q37" s="13">
         <v>10</v>
       </c>
@@ -3243,26 +3304,29 @@
       <c r="AI37" s="13">
         <v>9</v>
       </c>
-    </row>
-    <row r="38" spans="1:35">
-      <c r="A38" s="30" t="s">
+      <c r="AJ37" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:36">
+      <c r="A38" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="B38" s="30"/>
-      <c r="C38" s="30"/>
-      <c r="D38" s="30"/>
-      <c r="E38" s="30"/>
-      <c r="F38" s="30"/>
-      <c r="G38" s="30"/>
-      <c r="H38" s="30"/>
-      <c r="I38" s="30"/>
-      <c r="J38" s="30"/>
-      <c r="K38" s="30"/>
-      <c r="L38" s="30"/>
-      <c r="M38" s="26"/>
-      <c r="N38" s="26"/>
-      <c r="O38" s="26"/>
-      <c r="P38" s="26"/>
+      <c r="B38" s="33"/>
+      <c r="C38" s="33"/>
+      <c r="D38" s="33"/>
+      <c r="E38" s="33"/>
+      <c r="F38" s="33"/>
+      <c r="G38" s="33"/>
+      <c r="H38" s="33"/>
+      <c r="I38" s="33"/>
+      <c r="J38" s="33"/>
+      <c r="K38" s="33"/>
+      <c r="L38" s="33"/>
+      <c r="M38" s="23"/>
+      <c r="N38" s="23"/>
+      <c r="O38" s="23"/>
+      <c r="P38" s="23"/>
       <c r="Q38" s="8">
         <v>3</v>
       </c>
@@ -3320,26 +3384,29 @@
       <c r="AI38" s="13">
         <v>3</v>
       </c>
-    </row>
-    <row r="39" spans="1:35">
-      <c r="A39" s="30" t="s">
+      <c r="AJ38" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="1:36">
+      <c r="A39" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="B39" s="30"/>
-      <c r="C39" s="30"/>
-      <c r="D39" s="30"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="30"/>
-      <c r="G39" s="30"/>
-      <c r="H39" s="30"/>
-      <c r="I39" s="30"/>
-      <c r="J39" s="30"/>
-      <c r="K39" s="30"/>
-      <c r="L39" s="30"/>
-      <c r="M39" s="26"/>
-      <c r="N39" s="26"/>
-      <c r="O39" s="26"/>
-      <c r="P39" s="26"/>
+      <c r="B39" s="33"/>
+      <c r="C39" s="33"/>
+      <c r="D39" s="33"/>
+      <c r="E39" s="33"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="33"/>
+      <c r="H39" s="33"/>
+      <c r="I39" s="33"/>
+      <c r="J39" s="33"/>
+      <c r="K39" s="33"/>
+      <c r="L39" s="33"/>
+      <c r="M39" s="23"/>
+      <c r="N39" s="23"/>
+      <c r="O39" s="23"/>
+      <c r="P39" s="23"/>
       <c r="Q39" s="8">
         <v>2</v>
       </c>
@@ -3397,26 +3464,29 @@
       <c r="AI39">
         <v>2</v>
       </c>
-    </row>
-    <row r="40" spans="1:35">
-      <c r="A40" s="30" t="s">
+      <c r="AJ39" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:36">
+      <c r="A40" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="B40" s="30"/>
-      <c r="C40" s="30"/>
-      <c r="D40" s="30"/>
-      <c r="E40" s="30"/>
-      <c r="F40" s="30"/>
-      <c r="G40" s="30"/>
-      <c r="H40" s="30"/>
-      <c r="I40" s="30"/>
-      <c r="J40" s="30"/>
-      <c r="K40" s="30"/>
-      <c r="L40" s="30"/>
-      <c r="M40" s="26"/>
-      <c r="N40" s="26"/>
-      <c r="O40" s="26"/>
-      <c r="P40" s="26"/>
+      <c r="B40" s="33"/>
+      <c r="C40" s="33"/>
+      <c r="D40" s="33"/>
+      <c r="E40" s="33"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="33"/>
+      <c r="H40" s="33"/>
+      <c r="I40" s="33"/>
+      <c r="J40" s="33"/>
+      <c r="K40" s="33"/>
+      <c r="L40" s="33"/>
+      <c r="M40" s="23"/>
+      <c r="N40" s="23"/>
+      <c r="O40" s="23"/>
+      <c r="P40" s="23"/>
       <c r="Q40" s="8">
         <v>2</v>
       </c>
@@ -3474,24 +3544,27 @@
       <c r="AI40" s="13">
         <v>2</v>
       </c>
-    </row>
-    <row r="41" spans="1:35">
-      <c r="A41" s="25"/>
-      <c r="B41" s="25"/>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="25"/>
-      <c r="F41" s="25"/>
-      <c r="G41" s="25"/>
-      <c r="H41" s="25"/>
-      <c r="I41" s="25"/>
-      <c r="J41" s="25"/>
-      <c r="K41" s="25"/>
-      <c r="L41" s="25"/>
-      <c r="M41" s="26"/>
-      <c r="N41" s="26"/>
-      <c r="O41" s="26"/>
-      <c r="P41" s="26"/>
+      <c r="AJ40" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:36">
+      <c r="A41" s="34"/>
+      <c r="B41" s="34"/>
+      <c r="C41" s="34"/>
+      <c r="D41" s="34"/>
+      <c r="E41" s="34"/>
+      <c r="F41" s="34"/>
+      <c r="G41" s="34"/>
+      <c r="H41" s="34"/>
+      <c r="I41" s="34"/>
+      <c r="J41" s="34"/>
+      <c r="K41" s="34"/>
+      <c r="L41" s="34"/>
+      <c r="M41" s="23"/>
+      <c r="N41" s="23"/>
+      <c r="O41" s="23"/>
+      <c r="P41" s="23"/>
       <c r="Q41" s="8"/>
       <c r="R41" s="8"/>
       <c r="S41" s="8"/>
@@ -3508,23 +3581,23 @@
       <c r="AD41" s="8"/>
       <c r="AE41" s="8"/>
     </row>
-    <row r="42" spans="1:35">
-      <c r="A42" s="25"/>
-      <c r="B42" s="25"/>
-      <c r="C42" s="25"/>
-      <c r="D42" s="25"/>
-      <c r="E42" s="25"/>
-      <c r="F42" s="25"/>
-      <c r="G42" s="25"/>
-      <c r="H42" s="25"/>
-      <c r="I42" s="25"/>
-      <c r="J42" s="25"/>
-      <c r="K42" s="25"/>
-      <c r="L42" s="25"/>
-      <c r="M42" s="26"/>
-      <c r="N42" s="26"/>
-      <c r="O42" s="26"/>
-      <c r="P42" s="26"/>
+    <row r="42" spans="1:36">
+      <c r="A42" s="34"/>
+      <c r="B42" s="34"/>
+      <c r="C42" s="34"/>
+      <c r="D42" s="34"/>
+      <c r="E42" s="34"/>
+      <c r="F42" s="34"/>
+      <c r="G42" s="34"/>
+      <c r="H42" s="34"/>
+      <c r="I42" s="34"/>
+      <c r="J42" s="34"/>
+      <c r="K42" s="34"/>
+      <c r="L42" s="34"/>
+      <c r="M42" s="23"/>
+      <c r="N42" s="23"/>
+      <c r="O42" s="23"/>
+      <c r="P42" s="23"/>
       <c r="Q42" s="8"/>
       <c r="R42" s="8"/>
       <c r="S42" s="8"/>
@@ -3541,23 +3614,23 @@
       <c r="AD42" s="8"/>
       <c r="AE42" s="8"/>
     </row>
-    <row r="43" spans="1:35">
-      <c r="A43" s="25"/>
-      <c r="B43" s="25"/>
-      <c r="C43" s="25"/>
-      <c r="D43" s="25"/>
-      <c r="E43" s="25"/>
-      <c r="F43" s="25"/>
-      <c r="G43" s="25"/>
-      <c r="H43" s="25"/>
-      <c r="I43" s="25"/>
-      <c r="J43" s="25"/>
-      <c r="K43" s="25"/>
-      <c r="L43" s="25"/>
-      <c r="M43" s="26"/>
-      <c r="N43" s="26"/>
-      <c r="O43" s="26"/>
-      <c r="P43" s="26"/>
+    <row r="43" spans="1:36">
+      <c r="A43" s="34"/>
+      <c r="B43" s="34"/>
+      <c r="C43" s="34"/>
+      <c r="D43" s="34"/>
+      <c r="E43" s="34"/>
+      <c r="F43" s="34"/>
+      <c r="G43" s="34"/>
+      <c r="H43" s="34"/>
+      <c r="I43" s="34"/>
+      <c r="J43" s="34"/>
+      <c r="K43" s="34"/>
+      <c r="L43" s="34"/>
+      <c r="M43" s="23"/>
+      <c r="N43" s="23"/>
+      <c r="O43" s="23"/>
+      <c r="P43" s="23"/>
       <c r="Q43" s="8"/>
       <c r="R43" s="8"/>
       <c r="S43" s="8"/>
@@ -3574,23 +3647,23 @@
       <c r="AD43" s="8"/>
       <c r="AE43" s="8"/>
     </row>
-    <row r="44" spans="1:35">
-      <c r="A44" s="25"/>
-      <c r="B44" s="25"/>
-      <c r="C44" s="25"/>
-      <c r="D44" s="25"/>
-      <c r="E44" s="25"/>
-      <c r="F44" s="25"/>
-      <c r="G44" s="25"/>
-      <c r="H44" s="25"/>
-      <c r="I44" s="25"/>
-      <c r="J44" s="25"/>
-      <c r="K44" s="25"/>
-      <c r="L44" s="25"/>
-      <c r="M44" s="26"/>
-      <c r="N44" s="26"/>
-      <c r="O44" s="26"/>
-      <c r="P44" s="26"/>
+    <row r="44" spans="1:36">
+      <c r="A44" s="34"/>
+      <c r="B44" s="34"/>
+      <c r="C44" s="34"/>
+      <c r="D44" s="34"/>
+      <c r="E44" s="34"/>
+      <c r="F44" s="34"/>
+      <c r="G44" s="34"/>
+      <c r="H44" s="34"/>
+      <c r="I44" s="34"/>
+      <c r="J44" s="34"/>
+      <c r="K44" s="34"/>
+      <c r="L44" s="34"/>
+      <c r="M44" s="23"/>
+      <c r="N44" s="23"/>
+      <c r="O44" s="23"/>
+      <c r="P44" s="23"/>
       <c r="Q44" s="8"/>
       <c r="R44" s="8"/>
       <c r="S44" s="8"/>
@@ -3607,23 +3680,23 @@
       <c r="AD44" s="8"/>
       <c r="AE44" s="8"/>
     </row>
-    <row r="45" spans="1:35">
-      <c r="A45" s="25"/>
-      <c r="B45" s="25"/>
-      <c r="C45" s="25"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="25"/>
-      <c r="F45" s="25"/>
-      <c r="G45" s="25"/>
-      <c r="H45" s="25"/>
-      <c r="I45" s="25"/>
-      <c r="J45" s="25"/>
-      <c r="K45" s="25"/>
-      <c r="L45" s="25"/>
-      <c r="M45" s="26"/>
-      <c r="N45" s="26"/>
-      <c r="O45" s="26"/>
-      <c r="P45" s="26"/>
+    <row r="45" spans="1:36">
+      <c r="A45" s="34"/>
+      <c r="B45" s="34"/>
+      <c r="C45" s="34"/>
+      <c r="D45" s="34"/>
+      <c r="E45" s="34"/>
+      <c r="F45" s="34"/>
+      <c r="G45" s="34"/>
+      <c r="H45" s="34"/>
+      <c r="I45" s="34"/>
+      <c r="J45" s="34"/>
+      <c r="K45" s="34"/>
+      <c r="L45" s="34"/>
+      <c r="M45" s="23"/>
+      <c r="N45" s="23"/>
+      <c r="O45" s="23"/>
+      <c r="P45" s="23"/>
       <c r="Q45" s="8"/>
       <c r="R45" s="8"/>
       <c r="S45" s="8"/>
@@ -3640,23 +3713,23 @@
       <c r="AD45" s="8"/>
       <c r="AE45" s="8"/>
     </row>
-    <row r="46" spans="1:35">
-      <c r="A46" s="25"/>
-      <c r="B46" s="25"/>
-      <c r="C46" s="25"/>
-      <c r="D46" s="25"/>
-      <c r="E46" s="25"/>
-      <c r="F46" s="25"/>
-      <c r="G46" s="25"/>
-      <c r="H46" s="25"/>
-      <c r="I46" s="25"/>
-      <c r="J46" s="25"/>
-      <c r="K46" s="25"/>
-      <c r="L46" s="25"/>
-      <c r="M46" s="26"/>
-      <c r="N46" s="26"/>
-      <c r="O46" s="26"/>
-      <c r="P46" s="26"/>
+    <row r="46" spans="1:36">
+      <c r="A46" s="34"/>
+      <c r="B46" s="34"/>
+      <c r="C46" s="34"/>
+      <c r="D46" s="34"/>
+      <c r="E46" s="34"/>
+      <c r="F46" s="34"/>
+      <c r="G46" s="34"/>
+      <c r="H46" s="34"/>
+      <c r="I46" s="34"/>
+      <c r="J46" s="34"/>
+      <c r="K46" s="34"/>
+      <c r="L46" s="34"/>
+      <c r="M46" s="23"/>
+      <c r="N46" s="23"/>
+      <c r="O46" s="23"/>
+      <c r="P46" s="23"/>
       <c r="Q46" s="8"/>
       <c r="R46" s="8"/>
       <c r="S46" s="8"/>
@@ -3673,23 +3746,23 @@
       <c r="AD46" s="8"/>
       <c r="AE46" s="8"/>
     </row>
-    <row r="47" spans="1:35">
-      <c r="A47" s="25"/>
-      <c r="B47" s="25"/>
-      <c r="C47" s="25"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
-      <c r="H47" s="25"/>
-      <c r="I47" s="25"/>
-      <c r="J47" s="25"/>
-      <c r="K47" s="25"/>
-      <c r="L47" s="25"/>
-      <c r="M47" s="26"/>
-      <c r="N47" s="26"/>
-      <c r="O47" s="26"/>
-      <c r="P47" s="26"/>
+    <row r="47" spans="1:36">
+      <c r="A47" s="34"/>
+      <c r="B47" s="34"/>
+      <c r="C47" s="34"/>
+      <c r="D47" s="34"/>
+      <c r="E47" s="34"/>
+      <c r="F47" s="34"/>
+      <c r="G47" s="34"/>
+      <c r="H47" s="34"/>
+      <c r="I47" s="34"/>
+      <c r="J47" s="34"/>
+      <c r="K47" s="34"/>
+      <c r="L47" s="34"/>
+      <c r="M47" s="23"/>
+      <c r="N47" s="23"/>
+      <c r="O47" s="23"/>
+      <c r="P47" s="23"/>
       <c r="Q47" s="8"/>
       <c r="R47" s="8"/>
       <c r="S47" s="8"/>
@@ -3706,23 +3779,23 @@
       <c r="AD47" s="8"/>
       <c r="AE47" s="8"/>
     </row>
-    <row r="48" spans="1:35">
-      <c r="A48" s="25"/>
-      <c r="B48" s="25"/>
-      <c r="C48" s="25"/>
-      <c r="D48" s="25"/>
-      <c r="E48" s="25"/>
-      <c r="F48" s="25"/>
-      <c r="G48" s="25"/>
-      <c r="H48" s="25"/>
-      <c r="I48" s="25"/>
-      <c r="J48" s="25"/>
-      <c r="K48" s="25"/>
-      <c r="L48" s="25"/>
-      <c r="M48" s="26"/>
-      <c r="N48" s="26"/>
-      <c r="O48" s="26"/>
-      <c r="P48" s="26"/>
+    <row r="48" spans="1:36">
+      <c r="A48" s="34"/>
+      <c r="B48" s="34"/>
+      <c r="C48" s="34"/>
+      <c r="D48" s="34"/>
+      <c r="E48" s="34"/>
+      <c r="F48" s="34"/>
+      <c r="G48" s="34"/>
+      <c r="H48" s="34"/>
+      <c r="I48" s="34"/>
+      <c r="J48" s="34"/>
+      <c r="K48" s="34"/>
+      <c r="L48" s="34"/>
+      <c r="M48" s="23"/>
+      <c r="N48" s="23"/>
+      <c r="O48" s="23"/>
+      <c r="P48" s="23"/>
       <c r="Q48" s="8"/>
       <c r="R48" s="8"/>
       <c r="S48" s="8"/>
@@ -3740,22 +3813,22 @@
       <c r="AE48" s="8"/>
     </row>
     <row r="49" spans="1:31">
-      <c r="A49" s="25"/>
-      <c r="B49" s="25"/>
-      <c r="C49" s="25"/>
-      <c r="D49" s="25"/>
-      <c r="E49" s="25"/>
-      <c r="F49" s="25"/>
-      <c r="G49" s="25"/>
-      <c r="H49" s="25"/>
-      <c r="I49" s="25"/>
-      <c r="J49" s="25"/>
-      <c r="K49" s="25"/>
-      <c r="L49" s="25"/>
-      <c r="M49" s="26"/>
-      <c r="N49" s="26"/>
-      <c r="O49" s="26"/>
-      <c r="P49" s="26"/>
+      <c r="A49" s="34"/>
+      <c r="B49" s="34"/>
+      <c r="C49" s="34"/>
+      <c r="D49" s="34"/>
+      <c r="E49" s="34"/>
+      <c r="F49" s="34"/>
+      <c r="G49" s="34"/>
+      <c r="H49" s="34"/>
+      <c r="I49" s="34"/>
+      <c r="J49" s="34"/>
+      <c r="K49" s="34"/>
+      <c r="L49" s="34"/>
+      <c r="M49" s="23"/>
+      <c r="N49" s="23"/>
+      <c r="O49" s="23"/>
+      <c r="P49" s="23"/>
       <c r="Q49" s="8"/>
       <c r="R49" s="8"/>
       <c r="S49" s="8"/>
@@ -3773,22 +3846,22 @@
       <c r="AE49" s="8"/>
     </row>
     <row r="50" spans="1:31">
-      <c r="A50" s="25"/>
-      <c r="B50" s="25"/>
-      <c r="C50" s="25"/>
-      <c r="D50" s="25"/>
-      <c r="E50" s="25"/>
-      <c r="F50" s="25"/>
-      <c r="G50" s="25"/>
-      <c r="H50" s="25"/>
-      <c r="I50" s="25"/>
-      <c r="J50" s="25"/>
-      <c r="K50" s="25"/>
-      <c r="L50" s="25"/>
-      <c r="M50" s="26"/>
-      <c r="N50" s="26"/>
-      <c r="O50" s="26"/>
-      <c r="P50" s="26"/>
+      <c r="A50" s="34"/>
+      <c r="B50" s="34"/>
+      <c r="C50" s="34"/>
+      <c r="D50" s="34"/>
+      <c r="E50" s="34"/>
+      <c r="F50" s="34"/>
+      <c r="G50" s="34"/>
+      <c r="H50" s="34"/>
+      <c r="I50" s="34"/>
+      <c r="J50" s="34"/>
+      <c r="K50" s="34"/>
+      <c r="L50" s="34"/>
+      <c r="M50" s="23"/>
+      <c r="N50" s="23"/>
+      <c r="O50" s="23"/>
+      <c r="P50" s="23"/>
       <c r="Q50" s="8"/>
       <c r="R50" s="8"/>
       <c r="S50" s="8"/>
@@ -3806,22 +3879,22 @@
       <c r="AE50" s="8"/>
     </row>
     <row r="51" spans="1:31">
-      <c r="A51" s="25"/>
-      <c r="B51" s="25"/>
-      <c r="C51" s="25"/>
-      <c r="D51" s="25"/>
-      <c r="E51" s="25"/>
-      <c r="F51" s="25"/>
-      <c r="G51" s="25"/>
-      <c r="H51" s="25"/>
-      <c r="I51" s="25"/>
-      <c r="J51" s="25"/>
-      <c r="K51" s="25"/>
-      <c r="L51" s="25"/>
-      <c r="M51" s="26"/>
-      <c r="N51" s="26"/>
-      <c r="O51" s="26"/>
-      <c r="P51" s="26"/>
+      <c r="A51" s="34"/>
+      <c r="B51" s="34"/>
+      <c r="C51" s="34"/>
+      <c r="D51" s="34"/>
+      <c r="E51" s="34"/>
+      <c r="F51" s="34"/>
+      <c r="G51" s="34"/>
+      <c r="H51" s="34"/>
+      <c r="I51" s="34"/>
+      <c r="J51" s="34"/>
+      <c r="K51" s="34"/>
+      <c r="L51" s="34"/>
+      <c r="M51" s="23"/>
+      <c r="N51" s="23"/>
+      <c r="O51" s="23"/>
+      <c r="P51" s="23"/>
       <c r="Q51" s="8"/>
       <c r="R51" s="8"/>
       <c r="S51" s="8"/>
@@ -3839,22 +3912,22 @@
       <c r="AE51" s="8"/>
     </row>
     <row r="52" spans="1:31">
-      <c r="A52" s="25"/>
-      <c r="B52" s="25"/>
-      <c r="C52" s="25"/>
-      <c r="D52" s="25"/>
-      <c r="E52" s="25"/>
-      <c r="F52" s="25"/>
-      <c r="G52" s="25"/>
-      <c r="H52" s="25"/>
-      <c r="I52" s="25"/>
-      <c r="J52" s="25"/>
-      <c r="K52" s="25"/>
-      <c r="L52" s="25"/>
-      <c r="M52" s="26"/>
-      <c r="N52" s="26"/>
-      <c r="O52" s="26"/>
-      <c r="P52" s="26"/>
+      <c r="A52" s="34"/>
+      <c r="B52" s="34"/>
+      <c r="C52" s="34"/>
+      <c r="D52" s="34"/>
+      <c r="E52" s="34"/>
+      <c r="F52" s="34"/>
+      <c r="G52" s="34"/>
+      <c r="H52" s="34"/>
+      <c r="I52" s="34"/>
+      <c r="J52" s="34"/>
+      <c r="K52" s="34"/>
+      <c r="L52" s="34"/>
+      <c r="M52" s="23"/>
+      <c r="N52" s="23"/>
+      <c r="O52" s="23"/>
+      <c r="P52" s="23"/>
       <c r="Q52" s="8"/>
       <c r="R52" s="8"/>
       <c r="S52" s="8"/>
@@ -3872,22 +3945,22 @@
       <c r="AE52" s="8"/>
     </row>
     <row r="53" spans="1:31">
-      <c r="A53" s="25"/>
-      <c r="B53" s="25"/>
-      <c r="C53" s="25"/>
-      <c r="D53" s="25"/>
-      <c r="E53" s="25"/>
-      <c r="F53" s="25"/>
-      <c r="G53" s="25"/>
-      <c r="H53" s="25"/>
-      <c r="I53" s="25"/>
-      <c r="J53" s="25"/>
-      <c r="K53" s="25"/>
-      <c r="L53" s="25"/>
-      <c r="M53" s="26"/>
-      <c r="N53" s="26"/>
-      <c r="O53" s="26"/>
-      <c r="P53" s="26"/>
+      <c r="A53" s="34"/>
+      <c r="B53" s="34"/>
+      <c r="C53" s="34"/>
+      <c r="D53" s="34"/>
+      <c r="E53" s="34"/>
+      <c r="F53" s="34"/>
+      <c r="G53" s="34"/>
+      <c r="H53" s="34"/>
+      <c r="I53" s="34"/>
+      <c r="J53" s="34"/>
+      <c r="K53" s="34"/>
+      <c r="L53" s="34"/>
+      <c r="M53" s="23"/>
+      <c r="N53" s="23"/>
+      <c r="O53" s="23"/>
+      <c r="P53" s="23"/>
       <c r="Q53" s="8"/>
       <c r="R53" s="8"/>
       <c r="S53" s="8"/>
@@ -3905,22 +3978,22 @@
       <c r="AE53" s="8"/>
     </row>
     <row r="54" spans="1:31">
-      <c r="A54" s="25"/>
-      <c r="B54" s="25"/>
-      <c r="C54" s="25"/>
-      <c r="D54" s="25"/>
-      <c r="E54" s="25"/>
-      <c r="F54" s="25"/>
-      <c r="G54" s="25"/>
-      <c r="H54" s="25"/>
-      <c r="I54" s="25"/>
-      <c r="J54" s="25"/>
-      <c r="K54" s="25"/>
-      <c r="L54" s="25"/>
-      <c r="M54" s="26"/>
-      <c r="N54" s="26"/>
-      <c r="O54" s="26"/>
-      <c r="P54" s="26"/>
+      <c r="A54" s="34"/>
+      <c r="B54" s="34"/>
+      <c r="C54" s="34"/>
+      <c r="D54" s="34"/>
+      <c r="E54" s="34"/>
+      <c r="F54" s="34"/>
+      <c r="G54" s="34"/>
+      <c r="H54" s="34"/>
+      <c r="I54" s="34"/>
+      <c r="J54" s="34"/>
+      <c r="K54" s="34"/>
+      <c r="L54" s="34"/>
+      <c r="M54" s="23"/>
+      <c r="N54" s="23"/>
+      <c r="O54" s="23"/>
+      <c r="P54" s="23"/>
       <c r="Q54" s="8"/>
       <c r="R54" s="8"/>
       <c r="S54" s="8"/>
@@ -3938,8 +4011,62 @@
       <c r="AE54" s="8"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="71">
+    <mergeCell ref="Q19:AZ19"/>
+    <mergeCell ref="A53:L53"/>
+    <mergeCell ref="M53:P53"/>
+    <mergeCell ref="A54:L54"/>
+    <mergeCell ref="M54:P54"/>
+    <mergeCell ref="A29:L29"/>
+    <mergeCell ref="M29:P29"/>
+    <mergeCell ref="M25:P25"/>
+    <mergeCell ref="A25:L25"/>
+    <mergeCell ref="A50:L50"/>
+    <mergeCell ref="M50:P50"/>
+    <mergeCell ref="A51:L51"/>
+    <mergeCell ref="M51:P51"/>
+    <mergeCell ref="A52:L52"/>
+    <mergeCell ref="M52:P52"/>
+    <mergeCell ref="A47:L47"/>
+    <mergeCell ref="M47:P47"/>
+    <mergeCell ref="A48:L48"/>
+    <mergeCell ref="M48:P48"/>
+    <mergeCell ref="A49:L49"/>
+    <mergeCell ref="M49:P49"/>
+    <mergeCell ref="A44:L44"/>
+    <mergeCell ref="M44:P44"/>
+    <mergeCell ref="A45:L45"/>
+    <mergeCell ref="M45:P45"/>
+    <mergeCell ref="A46:L46"/>
+    <mergeCell ref="M46:P46"/>
+    <mergeCell ref="A41:L41"/>
+    <mergeCell ref="M41:P41"/>
+    <mergeCell ref="A42:L42"/>
+    <mergeCell ref="M42:P42"/>
+    <mergeCell ref="A43:L43"/>
+    <mergeCell ref="M43:P43"/>
+    <mergeCell ref="A38:L38"/>
+    <mergeCell ref="M38:P38"/>
+    <mergeCell ref="A39:L39"/>
+    <mergeCell ref="M39:P39"/>
+    <mergeCell ref="A40:L40"/>
+    <mergeCell ref="M40:P40"/>
+    <mergeCell ref="A32:L32"/>
+    <mergeCell ref="M32:P32"/>
+    <mergeCell ref="A33:L33"/>
+    <mergeCell ref="M33:P33"/>
+    <mergeCell ref="A36:L36"/>
+    <mergeCell ref="M36:P36"/>
+    <mergeCell ref="A34:L34"/>
+    <mergeCell ref="M34:P34"/>
+    <mergeCell ref="A35:L35"/>
+    <mergeCell ref="M35:P35"/>
+    <mergeCell ref="A28:L28"/>
+    <mergeCell ref="M28:P28"/>
+    <mergeCell ref="A30:L30"/>
+    <mergeCell ref="M30:P30"/>
+    <mergeCell ref="A31:L31"/>
+    <mergeCell ref="M31:P31"/>
     <mergeCell ref="A37:L37"/>
     <mergeCell ref="M37:P37"/>
     <mergeCell ref="A1:F1"/>
@@ -3956,64 +4083,10 @@
     <mergeCell ref="M23:P23"/>
     <mergeCell ref="A24:L24"/>
     <mergeCell ref="M24:P24"/>
-    <mergeCell ref="A28:L28"/>
-    <mergeCell ref="M28:P28"/>
-    <mergeCell ref="A30:L30"/>
-    <mergeCell ref="M30:P30"/>
-    <mergeCell ref="A31:L31"/>
-    <mergeCell ref="M31:P31"/>
-    <mergeCell ref="A32:L32"/>
-    <mergeCell ref="M32:P32"/>
-    <mergeCell ref="A33:L33"/>
-    <mergeCell ref="M33:P33"/>
-    <mergeCell ref="A36:L36"/>
-    <mergeCell ref="M36:P36"/>
-    <mergeCell ref="A34:L34"/>
-    <mergeCell ref="M34:P34"/>
-    <mergeCell ref="A35:L35"/>
-    <mergeCell ref="M35:P35"/>
-    <mergeCell ref="A38:L38"/>
-    <mergeCell ref="M38:P38"/>
-    <mergeCell ref="A39:L39"/>
-    <mergeCell ref="M39:P39"/>
-    <mergeCell ref="A40:L40"/>
-    <mergeCell ref="M40:P40"/>
-    <mergeCell ref="A41:L41"/>
-    <mergeCell ref="M41:P41"/>
-    <mergeCell ref="A42:L42"/>
-    <mergeCell ref="M42:P42"/>
-    <mergeCell ref="A43:L43"/>
-    <mergeCell ref="M43:P43"/>
-    <mergeCell ref="A44:L44"/>
-    <mergeCell ref="M44:P44"/>
-    <mergeCell ref="A45:L45"/>
-    <mergeCell ref="M45:P45"/>
-    <mergeCell ref="A46:L46"/>
-    <mergeCell ref="M46:P46"/>
-    <mergeCell ref="M47:P47"/>
-    <mergeCell ref="A48:L48"/>
-    <mergeCell ref="M48:P48"/>
-    <mergeCell ref="A49:L49"/>
-    <mergeCell ref="M49:P49"/>
-    <mergeCell ref="Q19:AZ19"/>
-    <mergeCell ref="A53:L53"/>
-    <mergeCell ref="M53:P53"/>
-    <mergeCell ref="A54:L54"/>
-    <mergeCell ref="M54:P54"/>
-    <mergeCell ref="A29:L29"/>
-    <mergeCell ref="M29:P29"/>
-    <mergeCell ref="M25:P25"/>
-    <mergeCell ref="A25:L25"/>
-    <mergeCell ref="A50:L50"/>
-    <mergeCell ref="M50:P50"/>
-    <mergeCell ref="A51:L51"/>
-    <mergeCell ref="M51:P51"/>
-    <mergeCell ref="A52:L52"/>
-    <mergeCell ref="M52:P52"/>
-    <mergeCell ref="A47:L47"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
   <extLst>
@@ -4035,20 +4108,20 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.140625" defaultRowHeight="13"/>
   <sheetData>
     <row r="1" spans="1:32">
-      <c r="A1" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="33" t="s">
+      <c r="A1" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -4075,61 +4148,61 @@
       <c r="P2" s="1"/>
     </row>
     <row r="3" spans="1:32" ht="14" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="N3" s="34"/>
-      <c r="O3" s="34"/>
-      <c r="P3" s="34"/>
-      <c r="Q3" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="R3" s="23"/>
-      <c r="S3" s="23"/>
-      <c r="T3" s="23"/>
-      <c r="U3" s="23"/>
-      <c r="V3" s="23"/>
-      <c r="W3" s="23"/>
-      <c r="X3" s="23"/>
-      <c r="Y3" s="23"/>
-      <c r="Z3" s="23"/>
-      <c r="AA3" s="23"/>
-      <c r="AB3" s="23"/>
-      <c r="AC3" s="23"/>
-      <c r="AD3" s="23"/>
-      <c r="AE3" s="24"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="26"/>
+      <c r="Q3" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="R3" s="36"/>
+      <c r="S3" s="36"/>
+      <c r="T3" s="36"/>
+      <c r="U3" s="36"/>
+      <c r="V3" s="36"/>
+      <c r="W3" s="36"/>
+      <c r="X3" s="36"/>
+      <c r="Y3" s="36"/>
+      <c r="Z3" s="36"/>
+      <c r="AA3" s="36"/>
+      <c r="AB3" s="36"/>
+      <c r="AC3" s="36"/>
+      <c r="AD3" s="36"/>
+      <c r="AE3" s="37"/>
     </row>
     <row r="4" spans="1:32">
-      <c r="A4" s="38"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35"/>
-      <c r="N4" s="35"/>
-      <c r="O4" s="35"/>
-      <c r="P4" s="35"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="27"/>
+      <c r="O4" s="27"/>
+      <c r="P4" s="27"/>
       <c r="Q4" s="3">
         <v>14</v>
       </c>
@@ -4178,22 +4251,22 @@
       <c r="AF4" s="9"/>
     </row>
     <row r="5" spans="1:32" ht="14" thickBot="1">
-      <c r="A5" s="40"/>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="41"/>
-      <c r="K5" s="41"/>
-      <c r="L5" s="41"/>
-      <c r="M5" s="41"/>
-      <c r="N5" s="41"/>
-      <c r="O5" s="41"/>
-      <c r="P5" s="41"/>
+      <c r="A5" s="41"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="42"/>
+      <c r="L5" s="42"/>
+      <c r="M5" s="42"/>
+      <c r="N5" s="42"/>
+      <c r="O5" s="42"/>
+      <c r="P5" s="42"/>
       <c r="Q5" s="5">
         <f>SUM(Q6:Q35)</f>
         <v>0</v>
@@ -4257,22 +4330,22 @@
       <c r="AF5" s="10"/>
     </row>
     <row r="6" spans="1:32">
-      <c r="A6" s="42"/>
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="42"/>
-      <c r="K6" s="42"/>
-      <c r="L6" s="42"/>
-      <c r="M6" s="42"/>
-      <c r="N6" s="42"/>
-      <c r="O6" s="42"/>
-      <c r="P6" s="42"/>
+      <c r="A6" s="40"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="40"/>
+      <c r="O6" s="40"/>
+      <c r="P6" s="40"/>
       <c r="Q6" s="7"/>
       <c r="R6" s="7"/>
       <c r="S6" s="7"/>
@@ -4290,22 +4363,22 @@
       <c r="AE6" s="7"/>
     </row>
     <row r="7" spans="1:32">
-      <c r="A7" s="26"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
-      <c r="M7" s="26"/>
-      <c r="N7" s="26"/>
-      <c r="O7" s="26"/>
-      <c r="P7" s="26"/>
+      <c r="A7" s="23"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="23"/>
       <c r="Q7" s="8"/>
       <c r="R7" s="8"/>
       <c r="S7" s="8"/>
@@ -4323,22 +4396,22 @@
       <c r="AE7" s="8"/>
     </row>
     <row r="8" spans="1:32">
-      <c r="A8" s="26"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="26"/>
-      <c r="M8" s="26"/>
-      <c r="N8" s="26"/>
-      <c r="O8" s="26"/>
-      <c r="P8" s="26"/>
+      <c r="A8" s="23"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="23"/>
+      <c r="P8" s="23"/>
       <c r="Q8" s="8"/>
       <c r="R8" s="8"/>
       <c r="S8" s="8"/>
@@ -4356,22 +4429,22 @@
       <c r="AE8" s="8"/>
     </row>
     <row r="9" spans="1:32">
-      <c r="A9" s="26"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="26"/>
-      <c r="O9" s="26"/>
-      <c r="P9" s="26"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="23"/>
       <c r="Q9" s="8"/>
       <c r="R9" s="8"/>
       <c r="S9" s="8"/>
@@ -4389,22 +4462,22 @@
       <c r="AE9" s="8"/>
     </row>
     <row r="10" spans="1:32">
-      <c r="A10" s="26"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="26"/>
-      <c r="N10" s="26"/>
-      <c r="O10" s="26"/>
-      <c r="P10" s="26"/>
+      <c r="A10" s="23"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="23"/>
+      <c r="P10" s="23"/>
       <c r="Q10" s="8"/>
       <c r="R10" s="8"/>
       <c r="S10" s="8"/>
@@ -4422,22 +4495,22 @@
       <c r="AE10" s="8"/>
     </row>
     <row r="11" spans="1:32">
-      <c r="A11" s="26"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
-      <c r="N11" s="26"/>
-      <c r="O11" s="26"/>
-      <c r="P11" s="26"/>
+      <c r="A11" s="23"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="23"/>
       <c r="Q11" s="8"/>
       <c r="R11" s="8"/>
       <c r="S11" s="8"/>
@@ -4455,22 +4528,22 @@
       <c r="AE11" s="8"/>
     </row>
     <row r="12" spans="1:32">
-      <c r="A12" s="26"/>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="26"/>
-      <c r="N12" s="26"/>
-      <c r="O12" s="26"/>
-      <c r="P12" s="26"/>
+      <c r="A12" s="23"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="23"/>
       <c r="Q12" s="8"/>
       <c r="R12" s="8"/>
       <c r="S12" s="8"/>
@@ -4488,22 +4561,22 @@
       <c r="AE12" s="8"/>
     </row>
     <row r="13" spans="1:32">
-      <c r="A13" s="26"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="26"/>
-      <c r="M13" s="26"/>
-      <c r="N13" s="26"/>
-      <c r="O13" s="26"/>
-      <c r="P13" s="26"/>
+      <c r="A13" s="23"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="23"/>
+      <c r="M13" s="23"/>
+      <c r="N13" s="23"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="23"/>
       <c r="Q13" s="8"/>
       <c r="R13" s="8"/>
       <c r="S13" s="8"/>
@@ -4521,22 +4594,22 @@
       <c r="AE13" s="8"/>
     </row>
     <row r="14" spans="1:32">
-      <c r="A14" s="26"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="26"/>
-      <c r="M14" s="26"/>
-      <c r="N14" s="26"/>
-      <c r="O14" s="26"/>
-      <c r="P14" s="26"/>
+      <c r="A14" s="23"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="23"/>
+      <c r="O14" s="23"/>
+      <c r="P14" s="23"/>
       <c r="Q14" s="8"/>
       <c r="R14" s="8"/>
       <c r="S14" s="8"/>
@@ -4554,22 +4627,22 @@
       <c r="AE14" s="8"/>
     </row>
     <row r="15" spans="1:32">
-      <c r="A15" s="26"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="26"/>
-      <c r="L15" s="26"/>
-      <c r="M15" s="26"/>
-      <c r="N15" s="26"/>
-      <c r="O15" s="26"/>
-      <c r="P15" s="26"/>
+      <c r="A15" s="23"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="23"/>
+      <c r="O15" s="23"/>
+      <c r="P15" s="23"/>
       <c r="Q15" s="8"/>
       <c r="R15" s="8"/>
       <c r="S15" s="8"/>
@@ -4587,22 +4660,22 @@
       <c r="AE15" s="8"/>
     </row>
     <row r="16" spans="1:32">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
-      <c r="M16" s="26"/>
-      <c r="N16" s="26"/>
-      <c r="O16" s="26"/>
-      <c r="P16" s="26"/>
+      <c r="A16" s="23"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="23"/>
+      <c r="N16" s="23"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="23"/>
       <c r="Q16" s="8"/>
       <c r="R16" s="8"/>
       <c r="S16" s="8"/>
@@ -4620,22 +4693,22 @@
       <c r="AE16" s="8"/>
     </row>
     <row r="17" spans="1:31">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="26"/>
-      <c r="L17" s="26"/>
-      <c r="M17" s="26"/>
-      <c r="N17" s="26"/>
-      <c r="O17" s="26"/>
-      <c r="P17" s="26"/>
+      <c r="A17" s="23"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="23"/>
+      <c r="N17" s="23"/>
+      <c r="O17" s="23"/>
+      <c r="P17" s="23"/>
       <c r="Q17" s="8"/>
       <c r="R17" s="8"/>
       <c r="S17" s="8"/>
@@ -4653,22 +4726,22 @@
       <c r="AE17" s="8"/>
     </row>
     <row r="18" spans="1:31">
-      <c r="A18" s="26"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="26"/>
-      <c r="L18" s="26"/>
-      <c r="M18" s="26"/>
-      <c r="N18" s="26"/>
-      <c r="O18" s="26"/>
-      <c r="P18" s="26"/>
+      <c r="A18" s="23"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="23"/>
+      <c r="M18" s="23"/>
+      <c r="N18" s="23"/>
+      <c r="O18" s="23"/>
+      <c r="P18" s="23"/>
       <c r="Q18" s="8"/>
       <c r="R18" s="8"/>
       <c r="S18" s="8"/>
@@ -4686,22 +4759,22 @@
       <c r="AE18" s="8"/>
     </row>
     <row r="19" spans="1:31">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="26"/>
-      <c r="K19" s="26"/>
-      <c r="L19" s="26"/>
-      <c r="M19" s="26"/>
-      <c r="N19" s="26"/>
-      <c r="O19" s="26"/>
-      <c r="P19" s="26"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="23"/>
+      <c r="P19" s="23"/>
       <c r="Q19" s="8"/>
       <c r="R19" s="8"/>
       <c r="S19" s="8"/>
@@ -4719,22 +4792,22 @@
       <c r="AE19" s="8"/>
     </row>
     <row r="20" spans="1:31">
-      <c r="A20" s="26"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
-      <c r="K20" s="26"/>
-      <c r="L20" s="26"/>
-      <c r="M20" s="26"/>
-      <c r="N20" s="26"/>
-      <c r="O20" s="26"/>
-      <c r="P20" s="26"/>
+      <c r="A20" s="23"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="23"/>
+      <c r="N20" s="23"/>
+      <c r="O20" s="23"/>
+      <c r="P20" s="23"/>
       <c r="Q20" s="8"/>
       <c r="R20" s="8"/>
       <c r="S20" s="8"/>
@@ -4752,22 +4825,22 @@
       <c r="AE20" s="8"/>
     </row>
     <row r="21" spans="1:31">
-      <c r="A21" s="26"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="26"/>
-      <c r="K21" s="26"/>
-      <c r="L21" s="26"/>
-      <c r="M21" s="26"/>
-      <c r="N21" s="26"/>
-      <c r="O21" s="26"/>
-      <c r="P21" s="26"/>
+      <c r="A21" s="23"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="23"/>
+      <c r="M21" s="23"/>
+      <c r="N21" s="23"/>
+      <c r="O21" s="23"/>
+      <c r="P21" s="23"/>
       <c r="Q21" s="8"/>
       <c r="R21" s="8"/>
       <c r="S21" s="8"/>
@@ -4785,22 +4858,22 @@
       <c r="AE21" s="8"/>
     </row>
     <row r="22" spans="1:31">
-      <c r="A22" s="26"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="26"/>
-      <c r="K22" s="26"/>
-      <c r="L22" s="26"/>
-      <c r="M22" s="26"/>
-      <c r="N22" s="26"/>
-      <c r="O22" s="26"/>
-      <c r="P22" s="26"/>
+      <c r="A22" s="23"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="23"/>
+      <c r="M22" s="23"/>
+      <c r="N22" s="23"/>
+      <c r="O22" s="23"/>
+      <c r="P22" s="23"/>
       <c r="Q22" s="8"/>
       <c r="R22" s="8"/>
       <c r="S22" s="8"/>
@@ -4818,22 +4891,22 @@
       <c r="AE22" s="8"/>
     </row>
     <row r="23" spans="1:31">
-      <c r="A23" s="26"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="26"/>
-      <c r="K23" s="26"/>
-      <c r="L23" s="26"/>
-      <c r="M23" s="26"/>
-      <c r="N23" s="26"/>
-      <c r="O23" s="26"/>
-      <c r="P23" s="26"/>
+      <c r="A23" s="23"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="23"/>
+      <c r="N23" s="23"/>
+      <c r="O23" s="23"/>
+      <c r="P23" s="23"/>
       <c r="Q23" s="8"/>
       <c r="R23" s="8"/>
       <c r="S23" s="8"/>
@@ -4851,22 +4924,22 @@
       <c r="AE23" s="8"/>
     </row>
     <row r="24" spans="1:31">
-      <c r="A24" s="26"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="26"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="26"/>
-      <c r="M24" s="26"/>
-      <c r="N24" s="26"/>
-      <c r="O24" s="26"/>
-      <c r="P24" s="26"/>
+      <c r="A24" s="23"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="23"/>
+      <c r="L24" s="23"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="23"/>
+      <c r="O24" s="23"/>
+      <c r="P24" s="23"/>
       <c r="Q24" s="8"/>
       <c r="R24" s="8"/>
       <c r="S24" s="8"/>
@@ -4884,22 +4957,22 @@
       <c r="AE24" s="8"/>
     </row>
     <row r="25" spans="1:31">
-      <c r="A25" s="26"/>
-      <c r="B25" s="26"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="26"/>
-      <c r="K25" s="26"/>
-      <c r="L25" s="26"/>
-      <c r="M25" s="26"/>
-      <c r="N25" s="26"/>
-      <c r="O25" s="26"/>
-      <c r="P25" s="26"/>
+      <c r="A25" s="23"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="23"/>
+      <c r="L25" s="23"/>
+      <c r="M25" s="23"/>
+      <c r="N25" s="23"/>
+      <c r="O25" s="23"/>
+      <c r="P25" s="23"/>
       <c r="Q25" s="8"/>
       <c r="R25" s="8"/>
       <c r="S25" s="8"/>
@@ -4917,22 +4990,22 @@
       <c r="AE25" s="8"/>
     </row>
     <row r="26" spans="1:31">
-      <c r="A26" s="26"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="26"/>
-      <c r="J26" s="26"/>
-      <c r="K26" s="26"/>
-      <c r="L26" s="26"/>
-      <c r="M26" s="26"/>
-      <c r="N26" s="26"/>
-      <c r="O26" s="26"/>
-      <c r="P26" s="26"/>
+      <c r="A26" s="23"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="23"/>
+      <c r="K26" s="23"/>
+      <c r="L26" s="23"/>
+      <c r="M26" s="23"/>
+      <c r="N26" s="23"/>
+      <c r="O26" s="23"/>
+      <c r="P26" s="23"/>
       <c r="Q26" s="8"/>
       <c r="R26" s="8"/>
       <c r="S26" s="8"/>
@@ -4950,22 +5023,22 @@
       <c r="AE26" s="8"/>
     </row>
     <row r="27" spans="1:31">
-      <c r="A27" s="26"/>
-      <c r="B27" s="26"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="26"/>
-      <c r="J27" s="26"/>
-      <c r="K27" s="26"/>
-      <c r="L27" s="26"/>
-      <c r="M27" s="26"/>
-      <c r="N27" s="26"/>
-      <c r="O27" s="26"/>
-      <c r="P27" s="26"/>
+      <c r="A27" s="23"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="23"/>
+      <c r="K27" s="23"/>
+      <c r="L27" s="23"/>
+      <c r="M27" s="23"/>
+      <c r="N27" s="23"/>
+      <c r="O27" s="23"/>
+      <c r="P27" s="23"/>
       <c r="Q27" s="8"/>
       <c r="R27" s="8"/>
       <c r="S27" s="8"/>
@@ -4983,22 +5056,22 @@
       <c r="AE27" s="8"/>
     </row>
     <row r="28" spans="1:31">
-      <c r="A28" s="26"/>
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="26"/>
-      <c r="J28" s="26"/>
-      <c r="K28" s="26"/>
-      <c r="L28" s="26"/>
-      <c r="M28" s="26"/>
-      <c r="N28" s="26"/>
-      <c r="O28" s="26"/>
-      <c r="P28" s="26"/>
+      <c r="A28" s="23"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
+      <c r="K28" s="23"/>
+      <c r="L28" s="23"/>
+      <c r="M28" s="23"/>
+      <c r="N28" s="23"/>
+      <c r="O28" s="23"/>
+      <c r="P28" s="23"/>
       <c r="Q28" s="8"/>
       <c r="R28" s="8"/>
       <c r="S28" s="8"/>
@@ -5016,22 +5089,22 @@
       <c r="AE28" s="8"/>
     </row>
     <row r="29" spans="1:31">
-      <c r="A29" s="26"/>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
-      <c r="K29" s="26"/>
-      <c r="L29" s="26"/>
-      <c r="M29" s="26"/>
-      <c r="N29" s="26"/>
-      <c r="O29" s="26"/>
-      <c r="P29" s="26"/>
+      <c r="A29" s="23"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="23"/>
+      <c r="K29" s="23"/>
+      <c r="L29" s="23"/>
+      <c r="M29" s="23"/>
+      <c r="N29" s="23"/>
+      <c r="O29" s="23"/>
+      <c r="P29" s="23"/>
       <c r="Q29" s="8"/>
       <c r="R29" s="8"/>
       <c r="S29" s="8"/>
@@ -5049,22 +5122,22 @@
       <c r="AE29" s="8"/>
     </row>
     <row r="30" spans="1:31">
-      <c r="A30" s="26"/>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="26"/>
-      <c r="K30" s="26"/>
-      <c r="L30" s="26"/>
-      <c r="M30" s="26"/>
-      <c r="N30" s="26"/>
-      <c r="O30" s="26"/>
-      <c r="P30" s="26"/>
+      <c r="A30" s="23"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="23"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="23"/>
+      <c r="K30" s="23"/>
+      <c r="L30" s="23"/>
+      <c r="M30" s="23"/>
+      <c r="N30" s="23"/>
+      <c r="O30" s="23"/>
+      <c r="P30" s="23"/>
       <c r="Q30" s="8"/>
       <c r="R30" s="8"/>
       <c r="S30" s="8"/>
@@ -5082,22 +5155,22 @@
       <c r="AE30" s="8"/>
     </row>
     <row r="31" spans="1:31">
-      <c r="A31" s="26"/>
-      <c r="B31" s="26"/>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="26"/>
-      <c r="J31" s="26"/>
-      <c r="K31" s="26"/>
-      <c r="L31" s="26"/>
-      <c r="M31" s="26"/>
-      <c r="N31" s="26"/>
-      <c r="O31" s="26"/>
-      <c r="P31" s="26"/>
+      <c r="A31" s="23"/>
+      <c r="B31" s="23"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="23"/>
+      <c r="H31" s="23"/>
+      <c r="I31" s="23"/>
+      <c r="J31" s="23"/>
+      <c r="K31" s="23"/>
+      <c r="L31" s="23"/>
+      <c r="M31" s="23"/>
+      <c r="N31" s="23"/>
+      <c r="O31" s="23"/>
+      <c r="P31" s="23"/>
       <c r="Q31" s="8"/>
       <c r="R31" s="8"/>
       <c r="S31" s="8"/>
@@ -5115,22 +5188,22 @@
       <c r="AE31" s="8"/>
     </row>
     <row r="32" spans="1:31">
-      <c r="A32" s="26"/>
-      <c r="B32" s="26"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="26"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="26"/>
-      <c r="H32" s="26"/>
-      <c r="I32" s="26"/>
-      <c r="J32" s="26"/>
-      <c r="K32" s="26"/>
-      <c r="L32" s="26"/>
-      <c r="M32" s="26"/>
-      <c r="N32" s="26"/>
-      <c r="O32" s="26"/>
-      <c r="P32" s="26"/>
+      <c r="A32" s="23"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="23"/>
+      <c r="K32" s="23"/>
+      <c r="L32" s="23"/>
+      <c r="M32" s="23"/>
+      <c r="N32" s="23"/>
+      <c r="O32" s="23"/>
+      <c r="P32" s="23"/>
       <c r="Q32" s="8"/>
       <c r="R32" s="8"/>
       <c r="S32" s="8"/>
@@ -5148,22 +5221,22 @@
       <c r="AE32" s="8"/>
     </row>
     <row r="33" spans="1:31">
-      <c r="A33" s="26"/>
-      <c r="B33" s="26"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="26"/>
-      <c r="G33" s="26"/>
-      <c r="H33" s="26"/>
-      <c r="I33" s="26"/>
-      <c r="J33" s="26"/>
-      <c r="K33" s="26"/>
-      <c r="L33" s="26"/>
-      <c r="M33" s="26"/>
-      <c r="N33" s="26"/>
-      <c r="O33" s="26"/>
-      <c r="P33" s="26"/>
+      <c r="A33" s="23"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="23"/>
+      <c r="I33" s="23"/>
+      <c r="J33" s="23"/>
+      <c r="K33" s="23"/>
+      <c r="L33" s="23"/>
+      <c r="M33" s="23"/>
+      <c r="N33" s="23"/>
+      <c r="O33" s="23"/>
+      <c r="P33" s="23"/>
       <c r="Q33" s="8"/>
       <c r="R33" s="8"/>
       <c r="S33" s="8"/>
@@ -5181,22 +5254,22 @@
       <c r="AE33" s="8"/>
     </row>
     <row r="34" spans="1:31">
-      <c r="A34" s="26"/>
-      <c r="B34" s="26"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
-      <c r="G34" s="26"/>
-      <c r="H34" s="26"/>
-      <c r="I34" s="26"/>
-      <c r="J34" s="26"/>
-      <c r="K34" s="26"/>
-      <c r="L34" s="26"/>
-      <c r="M34" s="26"/>
-      <c r="N34" s="26"/>
-      <c r="O34" s="26"/>
-      <c r="P34" s="26"/>
+      <c r="A34" s="23"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="23"/>
+      <c r="K34" s="23"/>
+      <c r="L34" s="23"/>
+      <c r="M34" s="23"/>
+      <c r="N34" s="23"/>
+      <c r="O34" s="23"/>
+      <c r="P34" s="23"/>
       <c r="Q34" s="8"/>
       <c r="R34" s="8"/>
       <c r="S34" s="8"/>
@@ -5214,22 +5287,22 @@
       <c r="AE34" s="8"/>
     </row>
     <row r="35" spans="1:31">
-      <c r="A35" s="26"/>
-      <c r="B35" s="26"/>
-      <c r="C35" s="26"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="26"/>
-      <c r="F35" s="26"/>
-      <c r="G35" s="26"/>
-      <c r="H35" s="26"/>
-      <c r="I35" s="26"/>
-      <c r="J35" s="26"/>
-      <c r="K35" s="26"/>
-      <c r="L35" s="26"/>
-      <c r="M35" s="26"/>
-      <c r="N35" s="26"/>
-      <c r="O35" s="26"/>
-      <c r="P35" s="26"/>
+      <c r="A35" s="23"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="23"/>
+      <c r="I35" s="23"/>
+      <c r="J35" s="23"/>
+      <c r="K35" s="23"/>
+      <c r="L35" s="23"/>
+      <c r="M35" s="23"/>
+      <c r="N35" s="23"/>
+      <c r="O35" s="23"/>
+      <c r="P35" s="23"/>
       <c r="Q35" s="8"/>
       <c r="R35" s="8"/>
       <c r="S35" s="8"/>
@@ -5247,8 +5320,60 @@
       <c r="AE35" s="8"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="65">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="A3:L5"/>
+    <mergeCell ref="M3:P5"/>
+    <mergeCell ref="Q3:AE3"/>
+    <mergeCell ref="A7:L7"/>
+    <mergeCell ref="M7:P7"/>
+    <mergeCell ref="A8:L8"/>
+    <mergeCell ref="M8:P8"/>
+    <mergeCell ref="A6:L6"/>
+    <mergeCell ref="M6:P6"/>
+    <mergeCell ref="A9:L9"/>
+    <mergeCell ref="M9:P9"/>
+    <mergeCell ref="A10:L10"/>
+    <mergeCell ref="M10:P10"/>
+    <mergeCell ref="A11:L11"/>
+    <mergeCell ref="M11:P11"/>
+    <mergeCell ref="A12:L12"/>
+    <mergeCell ref="M12:P12"/>
+    <mergeCell ref="A13:L13"/>
+    <mergeCell ref="M13:P13"/>
+    <mergeCell ref="A14:L14"/>
+    <mergeCell ref="M14:P14"/>
+    <mergeCell ref="A15:L15"/>
+    <mergeCell ref="M15:P15"/>
+    <mergeCell ref="A16:L16"/>
+    <mergeCell ref="M16:P16"/>
+    <mergeCell ref="A17:L17"/>
+    <mergeCell ref="M17:P17"/>
+    <mergeCell ref="A18:L18"/>
+    <mergeCell ref="M18:P18"/>
+    <mergeCell ref="A19:L19"/>
+    <mergeCell ref="M19:P19"/>
+    <mergeCell ref="A20:L20"/>
+    <mergeCell ref="M20:P20"/>
+    <mergeCell ref="A21:L21"/>
+    <mergeCell ref="M21:P21"/>
+    <mergeCell ref="A22:L22"/>
+    <mergeCell ref="M22:P22"/>
+    <mergeCell ref="A23:L23"/>
+    <mergeCell ref="M23:P23"/>
+    <mergeCell ref="A24:L24"/>
+    <mergeCell ref="M24:P24"/>
+    <mergeCell ref="A25:L25"/>
+    <mergeCell ref="M25:P25"/>
+    <mergeCell ref="A26:L26"/>
+    <mergeCell ref="M26:P26"/>
+    <mergeCell ref="A27:L27"/>
+    <mergeCell ref="M27:P27"/>
+    <mergeCell ref="A28:L28"/>
+    <mergeCell ref="M28:P28"/>
+    <mergeCell ref="A29:L29"/>
+    <mergeCell ref="M29:P29"/>
     <mergeCell ref="A30:L30"/>
     <mergeCell ref="M30:P30"/>
     <mergeCell ref="A34:L34"/>
@@ -5261,59 +5386,6 @@
     <mergeCell ref="M32:P32"/>
     <mergeCell ref="A33:L33"/>
     <mergeCell ref="M33:P33"/>
-    <mergeCell ref="A27:L27"/>
-    <mergeCell ref="M27:P27"/>
-    <mergeCell ref="A28:L28"/>
-    <mergeCell ref="M28:P28"/>
-    <mergeCell ref="A29:L29"/>
-    <mergeCell ref="M29:P29"/>
-    <mergeCell ref="A24:L24"/>
-    <mergeCell ref="M24:P24"/>
-    <mergeCell ref="A25:L25"/>
-    <mergeCell ref="M25:P25"/>
-    <mergeCell ref="A26:L26"/>
-    <mergeCell ref="M26:P26"/>
-    <mergeCell ref="A21:L21"/>
-    <mergeCell ref="M21:P21"/>
-    <mergeCell ref="A22:L22"/>
-    <mergeCell ref="M22:P22"/>
-    <mergeCell ref="A23:L23"/>
-    <mergeCell ref="M23:P23"/>
-    <mergeCell ref="A18:L18"/>
-    <mergeCell ref="M18:P18"/>
-    <mergeCell ref="A19:L19"/>
-    <mergeCell ref="M19:P19"/>
-    <mergeCell ref="A20:L20"/>
-    <mergeCell ref="M20:P20"/>
-    <mergeCell ref="A15:L15"/>
-    <mergeCell ref="M15:P15"/>
-    <mergeCell ref="A16:L16"/>
-    <mergeCell ref="M16:P16"/>
-    <mergeCell ref="A17:L17"/>
-    <mergeCell ref="M17:P17"/>
-    <mergeCell ref="A12:L12"/>
-    <mergeCell ref="M12:P12"/>
-    <mergeCell ref="A13:L13"/>
-    <mergeCell ref="M13:P13"/>
-    <mergeCell ref="A14:L14"/>
-    <mergeCell ref="M14:P14"/>
-    <mergeCell ref="A9:L9"/>
-    <mergeCell ref="M9:P9"/>
-    <mergeCell ref="A10:L10"/>
-    <mergeCell ref="M10:P10"/>
-    <mergeCell ref="A11:L11"/>
-    <mergeCell ref="M11:P11"/>
-    <mergeCell ref="A7:L7"/>
-    <mergeCell ref="M7:P7"/>
-    <mergeCell ref="A8:L8"/>
-    <mergeCell ref="M8:P8"/>
-    <mergeCell ref="A6:L6"/>
-    <mergeCell ref="M6:P6"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="A3:L5"/>
-    <mergeCell ref="M3:P5"/>
-    <mergeCell ref="Q3:AE3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -5337,20 +5409,20 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.140625" defaultRowHeight="13"/>
   <sheetData>
     <row r="1" spans="1:32">
-      <c r="A1" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="33" t="s">
+      <c r="A1" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
@@ -5377,61 +5449,61 @@
       <c r="P2" s="1"/>
     </row>
     <row r="3" spans="1:32" ht="14" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
-      <c r="G3" s="34"/>
-      <c r="H3" s="34"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="34"/>
-      <c r="K3" s="34"/>
-      <c r="L3" s="34"/>
-      <c r="M3" s="34" t="s">
-        <v>0</v>
-      </c>
-      <c r="N3" s="34"/>
-      <c r="O3" s="34"/>
-      <c r="P3" s="34"/>
-      <c r="Q3" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="R3" s="23"/>
-      <c r="S3" s="23"/>
-      <c r="T3" s="23"/>
-      <c r="U3" s="23"/>
-      <c r="V3" s="23"/>
-      <c r="W3" s="23"/>
-      <c r="X3" s="23"/>
-      <c r="Y3" s="23"/>
-      <c r="Z3" s="23"/>
-      <c r="AA3" s="23"/>
-      <c r="AB3" s="23"/>
-      <c r="AC3" s="23"/>
-      <c r="AD3" s="23"/>
-      <c r="AE3" s="24"/>
+      <c r="B3" s="26"/>
+      <c r="C3" s="26"/>
+      <c r="D3" s="26"/>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
+      <c r="J3" s="26"/>
+      <c r="K3" s="26"/>
+      <c r="L3" s="26"/>
+      <c r="M3" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="N3" s="26"/>
+      <c r="O3" s="26"/>
+      <c r="P3" s="26"/>
+      <c r="Q3" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="R3" s="36"/>
+      <c r="S3" s="36"/>
+      <c r="T3" s="36"/>
+      <c r="U3" s="36"/>
+      <c r="V3" s="36"/>
+      <c r="W3" s="36"/>
+      <c r="X3" s="36"/>
+      <c r="Y3" s="36"/>
+      <c r="Z3" s="36"/>
+      <c r="AA3" s="36"/>
+      <c r="AB3" s="36"/>
+      <c r="AC3" s="36"/>
+      <c r="AD3" s="36"/>
+      <c r="AE3" s="37"/>
     </row>
     <row r="4" spans="1:32">
-      <c r="A4" s="38"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="35"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="35"/>
-      <c r="J4" s="35"/>
-      <c r="K4" s="35"/>
-      <c r="L4" s="35"/>
-      <c r="M4" s="35"/>
-      <c r="N4" s="35"/>
-      <c r="O4" s="35"/>
-      <c r="P4" s="35"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="27"/>
+      <c r="C4" s="27"/>
+      <c r="D4" s="27"/>
+      <c r="E4" s="27"/>
+      <c r="F4" s="27"/>
+      <c r="G4" s="27"/>
+      <c r="H4" s="27"/>
+      <c r="I4" s="27"/>
+      <c r="J4" s="27"/>
+      <c r="K4" s="27"/>
+      <c r="L4" s="27"/>
+      <c r="M4" s="27"/>
+      <c r="N4" s="27"/>
+      <c r="O4" s="27"/>
+      <c r="P4" s="27"/>
       <c r="Q4" s="3">
         <v>14</v>
       </c>
@@ -5480,22 +5552,22 @@
       <c r="AF4" s="9"/>
     </row>
     <row r="5" spans="1:32" ht="14" thickBot="1">
-      <c r="A5" s="40"/>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="41"/>
-      <c r="K5" s="41"/>
-      <c r="L5" s="41"/>
-      <c r="M5" s="41"/>
-      <c r="N5" s="41"/>
-      <c r="O5" s="41"/>
-      <c r="P5" s="41"/>
+      <c r="A5" s="41"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="42"/>
+      <c r="I5" s="42"/>
+      <c r="J5" s="42"/>
+      <c r="K5" s="42"/>
+      <c r="L5" s="42"/>
+      <c r="M5" s="42"/>
+      <c r="N5" s="42"/>
+      <c r="O5" s="42"/>
+      <c r="P5" s="42"/>
       <c r="Q5" s="5">
         <f>SUM(Q6:Q35)</f>
         <v>0</v>
@@ -5559,22 +5631,22 @@
       <c r="AF5" s="10"/>
     </row>
     <row r="6" spans="1:32">
-      <c r="A6" s="42"/>
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="42"/>
-      <c r="K6" s="42"/>
-      <c r="L6" s="42"/>
-      <c r="M6" s="42"/>
-      <c r="N6" s="42"/>
-      <c r="O6" s="42"/>
-      <c r="P6" s="42"/>
+      <c r="A6" s="40"/>
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
+      <c r="K6" s="40"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="40"/>
+      <c r="N6" s="40"/>
+      <c r="O6" s="40"/>
+      <c r="P6" s="40"/>
       <c r="Q6" s="7"/>
       <c r="R6" s="7"/>
       <c r="S6" s="7"/>
@@ -5592,22 +5664,22 @@
       <c r="AE6" s="7"/>
     </row>
     <row r="7" spans="1:32">
-      <c r="A7" s="26"/>
-      <c r="B7" s="26"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
-      <c r="M7" s="26"/>
-      <c r="N7" s="26"/>
-      <c r="O7" s="26"/>
-      <c r="P7" s="26"/>
+      <c r="A7" s="23"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="23"/>
       <c r="Q7" s="8"/>
       <c r="R7" s="8"/>
       <c r="S7" s="8"/>
@@ -5625,22 +5697,22 @@
       <c r="AE7" s="8"/>
     </row>
     <row r="8" spans="1:32">
-      <c r="A8" s="26"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="26"/>
-      <c r="G8" s="26"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="26"/>
-      <c r="J8" s="26"/>
-      <c r="K8" s="26"/>
-      <c r="L8" s="26"/>
-      <c r="M8" s="26"/>
-      <c r="N8" s="26"/>
-      <c r="O8" s="26"/>
-      <c r="P8" s="26"/>
+      <c r="A8" s="23"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="23"/>
+      <c r="M8" s="23"/>
+      <c r="N8" s="23"/>
+      <c r="O8" s="23"/>
+      <c r="P8" s="23"/>
       <c r="Q8" s="8"/>
       <c r="R8" s="8"/>
       <c r="S8" s="8"/>
@@ -5658,22 +5730,22 @@
       <c r="AE8" s="8"/>
     </row>
     <row r="9" spans="1:32">
-      <c r="A9" s="26"/>
-      <c r="B9" s="26"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="26"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="26"/>
-      <c r="G9" s="26"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="26"/>
-      <c r="K9" s="26"/>
-      <c r="L9" s="26"/>
-      <c r="M9" s="26"/>
-      <c r="N9" s="26"/>
-      <c r="O9" s="26"/>
-      <c r="P9" s="26"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="E9" s="23"/>
+      <c r="F9" s="23"/>
+      <c r="G9" s="23"/>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23"/>
+      <c r="K9" s="23"/>
+      <c r="L9" s="23"/>
+      <c r="M9" s="23"/>
+      <c r="N9" s="23"/>
+      <c r="O9" s="23"/>
+      <c r="P9" s="23"/>
       <c r="Q9" s="8"/>
       <c r="R9" s="8"/>
       <c r="S9" s="8"/>
@@ -5691,22 +5763,22 @@
       <c r="AE9" s="8"/>
     </row>
     <row r="10" spans="1:32">
-      <c r="A10" s="26"/>
-      <c r="B10" s="26"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="26"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="26"/>
-      <c r="G10" s="26"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="26"/>
-      <c r="N10" s="26"/>
-      <c r="O10" s="26"/>
-      <c r="P10" s="26"/>
+      <c r="A10" s="23"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="23"/>
+      <c r="E10" s="23"/>
+      <c r="F10" s="23"/>
+      <c r="G10" s="23"/>
+      <c r="H10" s="23"/>
+      <c r="I10" s="23"/>
+      <c r="J10" s="23"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="23"/>
+      <c r="O10" s="23"/>
+      <c r="P10" s="23"/>
       <c r="Q10" s="8"/>
       <c r="R10" s="8"/>
       <c r="S10" s="8"/>
@@ -5724,22 +5796,22 @@
       <c r="AE10" s="8"/>
     </row>
     <row r="11" spans="1:32">
-      <c r="A11" s="26"/>
-      <c r="B11" s="26"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="26"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
-      <c r="N11" s="26"/>
-      <c r="O11" s="26"/>
-      <c r="P11" s="26"/>
+      <c r="A11" s="23"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="23"/>
+      <c r="D11" s="23"/>
+      <c r="E11" s="23"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
+      <c r="K11" s="23"/>
+      <c r="L11" s="23"/>
+      <c r="M11" s="23"/>
+      <c r="N11" s="23"/>
+      <c r="O11" s="23"/>
+      <c r="P11" s="23"/>
       <c r="Q11" s="8"/>
       <c r="R11" s="8"/>
       <c r="S11" s="8"/>
@@ -5757,22 +5829,22 @@
       <c r="AE11" s="8"/>
     </row>
     <row r="12" spans="1:32">
-      <c r="A12" s="26"/>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="26"/>
-      <c r="N12" s="26"/>
-      <c r="O12" s="26"/>
-      <c r="P12" s="26"/>
+      <c r="A12" s="23"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23"/>
+      <c r="F12" s="23"/>
+      <c r="G12" s="23"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23"/>
+      <c r="M12" s="23"/>
+      <c r="N12" s="23"/>
+      <c r="O12" s="23"/>
+      <c r="P12" s="23"/>
       <c r="Q12" s="8"/>
       <c r="R12" s="8"/>
       <c r="S12" s="8"/>
@@ -5790,22 +5862,22 @@
       <c r="AE12" s="8"/>
     </row>
     <row r="13" spans="1:32">
-      <c r="A13" s="26"/>
-      <c r="B13" s="26"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="26"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
-      <c r="J13" s="26"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="26"/>
-      <c r="M13" s="26"/>
-      <c r="N13" s="26"/>
-      <c r="O13" s="26"/>
-      <c r="P13" s="26"/>
+      <c r="A13" s="23"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="23"/>
+      <c r="E13" s="23"/>
+      <c r="F13" s="23"/>
+      <c r="G13" s="23"/>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23"/>
+      <c r="K13" s="23"/>
+      <c r="L13" s="23"/>
+      <c r="M13" s="23"/>
+      <c r="N13" s="23"/>
+      <c r="O13" s="23"/>
+      <c r="P13" s="23"/>
       <c r="Q13" s="8"/>
       <c r="R13" s="8"/>
       <c r="S13" s="8"/>
@@ -5823,22 +5895,22 @@
       <c r="AE13" s="8"/>
     </row>
     <row r="14" spans="1:32">
-      <c r="A14" s="26"/>
-      <c r="B14" s="26"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="26"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="26"/>
-      <c r="G14" s="26"/>
-      <c r="H14" s="26"/>
-      <c r="I14" s="26"/>
-      <c r="J14" s="26"/>
-      <c r="K14" s="26"/>
-      <c r="L14" s="26"/>
-      <c r="M14" s="26"/>
-      <c r="N14" s="26"/>
-      <c r="O14" s="26"/>
-      <c r="P14" s="26"/>
+      <c r="A14" s="23"/>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="G14" s="23"/>
+      <c r="H14" s="23"/>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23"/>
+      <c r="L14" s="23"/>
+      <c r="M14" s="23"/>
+      <c r="N14" s="23"/>
+      <c r="O14" s="23"/>
+      <c r="P14" s="23"/>
       <c r="Q14" s="8"/>
       <c r="R14" s="8"/>
       <c r="S14" s="8"/>
@@ -5856,22 +5928,22 @@
       <c r="AE14" s="8"/>
     </row>
     <row r="15" spans="1:32">
-      <c r="A15" s="26"/>
-      <c r="B15" s="26"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="26"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="26"/>
-      <c r="G15" s="26"/>
-      <c r="H15" s="26"/>
-      <c r="I15" s="26"/>
-      <c r="J15" s="26"/>
-      <c r="K15" s="26"/>
-      <c r="L15" s="26"/>
-      <c r="M15" s="26"/>
-      <c r="N15" s="26"/>
-      <c r="O15" s="26"/>
-      <c r="P15" s="26"/>
+      <c r="A15" s="23"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
+      <c r="F15" s="23"/>
+      <c r="G15" s="23"/>
+      <c r="H15" s="23"/>
+      <c r="I15" s="23"/>
+      <c r="J15" s="23"/>
+      <c r="K15" s="23"/>
+      <c r="L15" s="23"/>
+      <c r="M15" s="23"/>
+      <c r="N15" s="23"/>
+      <c r="O15" s="23"/>
+      <c r="P15" s="23"/>
       <c r="Q15" s="8"/>
       <c r="R15" s="8"/>
       <c r="S15" s="8"/>
@@ -5889,22 +5961,22 @@
       <c r="AE15" s="8"/>
     </row>
     <row r="16" spans="1:32">
-      <c r="A16" s="26"/>
-      <c r="B16" s="26"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="26"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="26"/>
-      <c r="H16" s="26"/>
-      <c r="I16" s="26"/>
-      <c r="J16" s="26"/>
-      <c r="K16" s="26"/>
-      <c r="L16" s="26"/>
-      <c r="M16" s="26"/>
-      <c r="N16" s="26"/>
-      <c r="O16" s="26"/>
-      <c r="P16" s="26"/>
+      <c r="A16" s="23"/>
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="23"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="23"/>
+      <c r="I16" s="23"/>
+      <c r="J16" s="23"/>
+      <c r="K16" s="23"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="23"/>
+      <c r="N16" s="23"/>
+      <c r="O16" s="23"/>
+      <c r="P16" s="23"/>
       <c r="Q16" s="8"/>
       <c r="R16" s="8"/>
       <c r="S16" s="8"/>
@@ -5922,22 +5994,22 @@
       <c r="AE16" s="8"/>
     </row>
     <row r="17" spans="1:31">
-      <c r="A17" s="26"/>
-      <c r="B17" s="26"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="26"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="26"/>
-      <c r="G17" s="26"/>
-      <c r="H17" s="26"/>
-      <c r="I17" s="26"/>
-      <c r="J17" s="26"/>
-      <c r="K17" s="26"/>
-      <c r="L17" s="26"/>
-      <c r="M17" s="26"/>
-      <c r="N17" s="26"/>
-      <c r="O17" s="26"/>
-      <c r="P17" s="26"/>
+      <c r="A17" s="23"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="23"/>
+      <c r="N17" s="23"/>
+      <c r="O17" s="23"/>
+      <c r="P17" s="23"/>
       <c r="Q17" s="8"/>
       <c r="R17" s="8"/>
       <c r="S17" s="8"/>
@@ -5955,22 +6027,22 @@
       <c r="AE17" s="8"/>
     </row>
     <row r="18" spans="1:31">
-      <c r="A18" s="26"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
-      <c r="G18" s="26"/>
-      <c r="H18" s="26"/>
-      <c r="I18" s="26"/>
-      <c r="J18" s="26"/>
-      <c r="K18" s="26"/>
-      <c r="L18" s="26"/>
-      <c r="M18" s="26"/>
-      <c r="N18" s="26"/>
-      <c r="O18" s="26"/>
-      <c r="P18" s="26"/>
+      <c r="A18" s="23"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="23"/>
+      <c r="G18" s="23"/>
+      <c r="H18" s="23"/>
+      <c r="I18" s="23"/>
+      <c r="J18" s="23"/>
+      <c r="K18" s="23"/>
+      <c r="L18" s="23"/>
+      <c r="M18" s="23"/>
+      <c r="N18" s="23"/>
+      <c r="O18" s="23"/>
+      <c r="P18" s="23"/>
       <c r="Q18" s="8"/>
       <c r="R18" s="8"/>
       <c r="S18" s="8"/>
@@ -5988,22 +6060,22 @@
       <c r="AE18" s="8"/>
     </row>
     <row r="19" spans="1:31">
-      <c r="A19" s="26"/>
-      <c r="B19" s="26"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="26"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="26"/>
-      <c r="G19" s="26"/>
-      <c r="H19" s="26"/>
-      <c r="I19" s="26"/>
-      <c r="J19" s="26"/>
-      <c r="K19" s="26"/>
-      <c r="L19" s="26"/>
-      <c r="M19" s="26"/>
-      <c r="N19" s="26"/>
-      <c r="O19" s="26"/>
-      <c r="P19" s="26"/>
+      <c r="A19" s="23"/>
+      <c r="B19" s="23"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="M19" s="23"/>
+      <c r="N19" s="23"/>
+      <c r="O19" s="23"/>
+      <c r="P19" s="23"/>
       <c r="Q19" s="8"/>
       <c r="R19" s="8"/>
       <c r="S19" s="8"/>
@@ -6021,22 +6093,22 @@
       <c r="AE19" s="8"/>
     </row>
     <row r="20" spans="1:31">
-      <c r="A20" s="26"/>
-      <c r="B20" s="26"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="26"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="26"/>
-      <c r="G20" s="26"/>
-      <c r="H20" s="26"/>
-      <c r="I20" s="26"/>
-      <c r="J20" s="26"/>
-      <c r="K20" s="26"/>
-      <c r="L20" s="26"/>
-      <c r="M20" s="26"/>
-      <c r="N20" s="26"/>
-      <c r="O20" s="26"/>
-      <c r="P20" s="26"/>
+      <c r="A20" s="23"/>
+      <c r="B20" s="23"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
+      <c r="F20" s="23"/>
+      <c r="G20" s="23"/>
+      <c r="H20" s="23"/>
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
+      <c r="K20" s="23"/>
+      <c r="L20" s="23"/>
+      <c r="M20" s="23"/>
+      <c r="N20" s="23"/>
+      <c r="O20" s="23"/>
+      <c r="P20" s="23"/>
       <c r="Q20" s="8"/>
       <c r="R20" s="8"/>
       <c r="S20" s="8"/>
@@ -6054,22 +6126,22 @@
       <c r="AE20" s="8"/>
     </row>
     <row r="21" spans="1:31">
-      <c r="A21" s="26"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="26"/>
-      <c r="K21" s="26"/>
-      <c r="L21" s="26"/>
-      <c r="M21" s="26"/>
-      <c r="N21" s="26"/>
-      <c r="O21" s="26"/>
-      <c r="P21" s="26"/>
+      <c r="A21" s="23"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="G21" s="23"/>
+      <c r="H21" s="23"/>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23"/>
+      <c r="K21" s="23"/>
+      <c r="L21" s="23"/>
+      <c r="M21" s="23"/>
+      <c r="N21" s="23"/>
+      <c r="O21" s="23"/>
+      <c r="P21" s="23"/>
       <c r="Q21" s="8"/>
       <c r="R21" s="8"/>
       <c r="S21" s="8"/>
@@ -6087,22 +6159,22 @@
       <c r="AE21" s="8"/>
     </row>
     <row r="22" spans="1:31">
-      <c r="A22" s="26"/>
-      <c r="B22" s="26"/>
-      <c r="C22" s="26"/>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="26"/>
-      <c r="G22" s="26"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="26"/>
-      <c r="K22" s="26"/>
-      <c r="L22" s="26"/>
-      <c r="M22" s="26"/>
-      <c r="N22" s="26"/>
-      <c r="O22" s="26"/>
-      <c r="P22" s="26"/>
+      <c r="A22" s="23"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="23"/>
+      <c r="J22" s="23"/>
+      <c r="K22" s="23"/>
+      <c r="L22" s="23"/>
+      <c r="M22" s="23"/>
+      <c r="N22" s="23"/>
+      <c r="O22" s="23"/>
+      <c r="P22" s="23"/>
       <c r="Q22" s="8"/>
       <c r="R22" s="8"/>
       <c r="S22" s="8"/>
@@ -6120,22 +6192,22 @@
       <c r="AE22" s="8"/>
     </row>
     <row r="23" spans="1:31">
-      <c r="A23" s="26"/>
-      <c r="B23" s="26"/>
-      <c r="C23" s="26"/>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="26"/>
-      <c r="G23" s="26"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="26"/>
-      <c r="K23" s="26"/>
-      <c r="L23" s="26"/>
-      <c r="M23" s="26"/>
-      <c r="N23" s="26"/>
-      <c r="O23" s="26"/>
-      <c r="P23" s="26"/>
+      <c r="A23" s="23"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="23"/>
+      <c r="N23" s="23"/>
+      <c r="O23" s="23"/>
+      <c r="P23" s="23"/>
       <c r="Q23" s="8"/>
       <c r="R23" s="8"/>
       <c r="S23" s="8"/>
@@ -6153,22 +6225,22 @@
       <c r="AE23" s="8"/>
     </row>
     <row r="24" spans="1:31">
-      <c r="A24" s="26"/>
-      <c r="B24" s="26"/>
-      <c r="C24" s="26"/>
-      <c r="D24" s="26"/>
-      <c r="E24" s="26"/>
-      <c r="F24" s="26"/>
-      <c r="G24" s="26"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="26"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="26"/>
-      <c r="M24" s="26"/>
-      <c r="N24" s="26"/>
-      <c r="O24" s="26"/>
-      <c r="P24" s="26"/>
+      <c r="A24" s="23"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
+      <c r="E24" s="23"/>
+      <c r="F24" s="23"/>
+      <c r="G24" s="23"/>
+      <c r="H24" s="23"/>
+      <c r="I24" s="23"/>
+      <c r="J24" s="23"/>
+      <c r="K24" s="23"/>
+      <c r="L24" s="23"/>
+      <c r="M24" s="23"/>
+      <c r="N24" s="23"/>
+      <c r="O24" s="23"/>
+      <c r="P24" s="23"/>
       <c r="Q24" s="8"/>
       <c r="R24" s="8"/>
       <c r="S24" s="8"/>
@@ -6186,22 +6258,22 @@
       <c r="AE24" s="8"/>
     </row>
     <row r="25" spans="1:31">
-      <c r="A25" s="26"/>
-      <c r="B25" s="26"/>
-      <c r="C25" s="26"/>
-      <c r="D25" s="26"/>
-      <c r="E25" s="26"/>
-      <c r="F25" s="26"/>
-      <c r="G25" s="26"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="26"/>
-      <c r="K25" s="26"/>
-      <c r="L25" s="26"/>
-      <c r="M25" s="26"/>
-      <c r="N25" s="26"/>
-      <c r="O25" s="26"/>
-      <c r="P25" s="26"/>
+      <c r="A25" s="23"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="23"/>
+      <c r="F25" s="23"/>
+      <c r="G25" s="23"/>
+      <c r="H25" s="23"/>
+      <c r="I25" s="23"/>
+      <c r="J25" s="23"/>
+      <c r="K25" s="23"/>
+      <c r="L25" s="23"/>
+      <c r="M25" s="23"/>
+      <c r="N25" s="23"/>
+      <c r="O25" s="23"/>
+      <c r="P25" s="23"/>
       <c r="Q25" s="8"/>
       <c r="R25" s="8"/>
       <c r="S25" s="8"/>
@@ -6219,22 +6291,22 @@
       <c r="AE25" s="8"/>
     </row>
     <row r="26" spans="1:31">
-      <c r="A26" s="26"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="26"/>
-      <c r="D26" s="26"/>
-      <c r="E26" s="26"/>
-      <c r="F26" s="26"/>
-      <c r="G26" s="26"/>
-      <c r="H26" s="26"/>
-      <c r="I26" s="26"/>
-      <c r="J26" s="26"/>
-      <c r="K26" s="26"/>
-      <c r="L26" s="26"/>
-      <c r="M26" s="26"/>
-      <c r="N26" s="26"/>
-      <c r="O26" s="26"/>
-      <c r="P26" s="26"/>
+      <c r="A26" s="23"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23"/>
+      <c r="F26" s="23"/>
+      <c r="G26" s="23"/>
+      <c r="H26" s="23"/>
+      <c r="I26" s="23"/>
+      <c r="J26" s="23"/>
+      <c r="K26" s="23"/>
+      <c r="L26" s="23"/>
+      <c r="M26" s="23"/>
+      <c r="N26" s="23"/>
+      <c r="O26" s="23"/>
+      <c r="P26" s="23"/>
       <c r="Q26" s="8"/>
       <c r="R26" s="8"/>
       <c r="S26" s="8"/>
@@ -6252,22 +6324,22 @@
       <c r="AE26" s="8"/>
     </row>
     <row r="27" spans="1:31">
-      <c r="A27" s="26"/>
-      <c r="B27" s="26"/>
-      <c r="C27" s="26"/>
-      <c r="D27" s="26"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="26"/>
-      <c r="G27" s="26"/>
-      <c r="H27" s="26"/>
-      <c r="I27" s="26"/>
-      <c r="J27" s="26"/>
-      <c r="K27" s="26"/>
-      <c r="L27" s="26"/>
-      <c r="M27" s="26"/>
-      <c r="N27" s="26"/>
-      <c r="O27" s="26"/>
-      <c r="P27" s="26"/>
+      <c r="A27" s="23"/>
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="E27" s="23"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="23"/>
+      <c r="J27" s="23"/>
+      <c r="K27" s="23"/>
+      <c r="L27" s="23"/>
+      <c r="M27" s="23"/>
+      <c r="N27" s="23"/>
+      <c r="O27" s="23"/>
+      <c r="P27" s="23"/>
       <c r="Q27" s="8"/>
       <c r="R27" s="8"/>
       <c r="S27" s="8"/>
@@ -6285,22 +6357,22 @@
       <c r="AE27" s="8"/>
     </row>
     <row r="28" spans="1:31">
-      <c r="A28" s="26"/>
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="26"/>
-      <c r="F28" s="26"/>
-      <c r="G28" s="26"/>
-      <c r="H28" s="26"/>
-      <c r="I28" s="26"/>
-      <c r="J28" s="26"/>
-      <c r="K28" s="26"/>
-      <c r="L28" s="26"/>
-      <c r="M28" s="26"/>
-      <c r="N28" s="26"/>
-      <c r="O28" s="26"/>
-      <c r="P28" s="26"/>
+      <c r="A28" s="23"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="23"/>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
+      <c r="K28" s="23"/>
+      <c r="L28" s="23"/>
+      <c r="M28" s="23"/>
+      <c r="N28" s="23"/>
+      <c r="O28" s="23"/>
+      <c r="P28" s="23"/>
       <c r="Q28" s="8"/>
       <c r="R28" s="8"/>
       <c r="S28" s="8"/>
@@ -6318,22 +6390,22 @@
       <c r="AE28" s="8"/>
     </row>
     <row r="29" spans="1:31">
-      <c r="A29" s="26"/>
-      <c r="B29" s="26"/>
-      <c r="C29" s="26"/>
-      <c r="D29" s="26"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="26"/>
-      <c r="G29" s="26"/>
-      <c r="H29" s="26"/>
-      <c r="I29" s="26"/>
-      <c r="J29" s="26"/>
-      <c r="K29" s="26"/>
-      <c r="L29" s="26"/>
-      <c r="M29" s="26"/>
-      <c r="N29" s="26"/>
-      <c r="O29" s="26"/>
-      <c r="P29" s="26"/>
+      <c r="A29" s="23"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
+      <c r="J29" s="23"/>
+      <c r="K29" s="23"/>
+      <c r="L29" s="23"/>
+      <c r="M29" s="23"/>
+      <c r="N29" s="23"/>
+      <c r="O29" s="23"/>
+      <c r="P29" s="23"/>
       <c r="Q29" s="8"/>
       <c r="R29" s="8"/>
       <c r="S29" s="8"/>
@@ -6351,22 +6423,22 @@
       <c r="AE29" s="8"/>
     </row>
     <row r="30" spans="1:31">
-      <c r="A30" s="26"/>
-      <c r="B30" s="26"/>
-      <c r="C30" s="26"/>
-      <c r="D30" s="26"/>
-      <c r="E30" s="26"/>
-      <c r="F30" s="26"/>
-      <c r="G30" s="26"/>
-      <c r="H30" s="26"/>
-      <c r="I30" s="26"/>
-      <c r="J30" s="26"/>
-      <c r="K30" s="26"/>
-      <c r="L30" s="26"/>
-      <c r="M30" s="26"/>
-      <c r="N30" s="26"/>
-      <c r="O30" s="26"/>
-      <c r="P30" s="26"/>
+      <c r="A30" s="23"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="23"/>
+      <c r="G30" s="23"/>
+      <c r="H30" s="23"/>
+      <c r="I30" s="23"/>
+      <c r="J30" s="23"/>
+      <c r="K30" s="23"/>
+      <c r="L30" s="23"/>
+      <c r="M30" s="23"/>
+      <c r="N30" s="23"/>
+      <c r="O30" s="23"/>
+      <c r="P30" s="23"/>
       <c r="Q30" s="8"/>
       <c r="R30" s="8"/>
       <c r="S30" s="8"/>
@@ -6384,22 +6456,22 @@
       <c r="AE30" s="8"/>
     </row>
     <row r="31" spans="1:31">
-      <c r="A31" s="26"/>
-      <c r="B31" s="26"/>
-      <c r="C31" s="26"/>
-      <c r="D31" s="26"/>
-      <c r="E31" s="26"/>
-      <c r="F31" s="26"/>
-      <c r="G31" s="26"/>
-      <c r="H31" s="26"/>
-      <c r="I31" s="26"/>
-      <c r="J31" s="26"/>
-      <c r="K31" s="26"/>
-      <c r="L31" s="26"/>
-      <c r="M31" s="26"/>
-      <c r="N31" s="26"/>
-      <c r="O31" s="26"/>
-      <c r="P31" s="26"/>
+      <c r="A31" s="23"/>
+      <c r="B31" s="23"/>
+      <c r="C31" s="23"/>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="23"/>
+      <c r="G31" s="23"/>
+      <c r="H31" s="23"/>
+      <c r="I31" s="23"/>
+      <c r="J31" s="23"/>
+      <c r="K31" s="23"/>
+      <c r="L31" s="23"/>
+      <c r="M31" s="23"/>
+      <c r="N31" s="23"/>
+      <c r="O31" s="23"/>
+      <c r="P31" s="23"/>
       <c r="Q31" s="8"/>
       <c r="R31" s="8"/>
       <c r="S31" s="8"/>
@@ -6417,22 +6489,22 @@
       <c r="AE31" s="8"/>
     </row>
     <row r="32" spans="1:31">
-      <c r="A32" s="26"/>
-      <c r="B32" s="26"/>
-      <c r="C32" s="26"/>
-      <c r="D32" s="26"/>
-      <c r="E32" s="26"/>
-      <c r="F32" s="26"/>
-      <c r="G32" s="26"/>
-      <c r="H32" s="26"/>
-      <c r="I32" s="26"/>
-      <c r="J32" s="26"/>
-      <c r="K32" s="26"/>
-      <c r="L32" s="26"/>
-      <c r="M32" s="26"/>
-      <c r="N32" s="26"/>
-      <c r="O32" s="26"/>
-      <c r="P32" s="26"/>
+      <c r="A32" s="23"/>
+      <c r="B32" s="23"/>
+      <c r="C32" s="23"/>
+      <c r="D32" s="23"/>
+      <c r="E32" s="23"/>
+      <c r="F32" s="23"/>
+      <c r="G32" s="23"/>
+      <c r="H32" s="23"/>
+      <c r="I32" s="23"/>
+      <c r="J32" s="23"/>
+      <c r="K32" s="23"/>
+      <c r="L32" s="23"/>
+      <c r="M32" s="23"/>
+      <c r="N32" s="23"/>
+      <c r="O32" s="23"/>
+      <c r="P32" s="23"/>
       <c r="Q32" s="8"/>
       <c r="R32" s="8"/>
       <c r="S32" s="8"/>
@@ -6450,22 +6522,22 @@
       <c r="AE32" s="8"/>
     </row>
     <row r="33" spans="1:31">
-      <c r="A33" s="26"/>
-      <c r="B33" s="26"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="26"/>
-      <c r="G33" s="26"/>
-      <c r="H33" s="26"/>
-      <c r="I33" s="26"/>
-      <c r="J33" s="26"/>
-      <c r="K33" s="26"/>
-      <c r="L33" s="26"/>
-      <c r="M33" s="26"/>
-      <c r="N33" s="26"/>
-      <c r="O33" s="26"/>
-      <c r="P33" s="26"/>
+      <c r="A33" s="23"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="23"/>
+      <c r="D33" s="23"/>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="G33" s="23"/>
+      <c r="H33" s="23"/>
+      <c r="I33" s="23"/>
+      <c r="J33" s="23"/>
+      <c r="K33" s="23"/>
+      <c r="L33" s="23"/>
+      <c r="M33" s="23"/>
+      <c r="N33" s="23"/>
+      <c r="O33" s="23"/>
+      <c r="P33" s="23"/>
       <c r="Q33" s="8"/>
       <c r="R33" s="8"/>
       <c r="S33" s="8"/>
@@ -6483,22 +6555,22 @@
       <c r="AE33" s="8"/>
     </row>
     <row r="34" spans="1:31">
-      <c r="A34" s="26"/>
-      <c r="B34" s="26"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
-      <c r="G34" s="26"/>
-      <c r="H34" s="26"/>
-      <c r="I34" s="26"/>
-      <c r="J34" s="26"/>
-      <c r="K34" s="26"/>
-      <c r="L34" s="26"/>
-      <c r="M34" s="26"/>
-      <c r="N34" s="26"/>
-      <c r="O34" s="26"/>
-      <c r="P34" s="26"/>
+      <c r="A34" s="23"/>
+      <c r="B34" s="23"/>
+      <c r="C34" s="23"/>
+      <c r="D34" s="23"/>
+      <c r="E34" s="23"/>
+      <c r="F34" s="23"/>
+      <c r="G34" s="23"/>
+      <c r="H34" s="23"/>
+      <c r="I34" s="23"/>
+      <c r="J34" s="23"/>
+      <c r="K34" s="23"/>
+      <c r="L34" s="23"/>
+      <c r="M34" s="23"/>
+      <c r="N34" s="23"/>
+      <c r="O34" s="23"/>
+      <c r="P34" s="23"/>
       <c r="Q34" s="8"/>
       <c r="R34" s="8"/>
       <c r="S34" s="8"/>
@@ -6516,22 +6588,22 @@
       <c r="AE34" s="8"/>
     </row>
     <row r="35" spans="1:31">
-      <c r="A35" s="26"/>
-      <c r="B35" s="26"/>
-      <c r="C35" s="26"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="26"/>
-      <c r="F35" s="26"/>
-      <c r="G35" s="26"/>
-      <c r="H35" s="26"/>
-      <c r="I35" s="26"/>
-      <c r="J35" s="26"/>
-      <c r="K35" s="26"/>
-      <c r="L35" s="26"/>
-      <c r="M35" s="26"/>
-      <c r="N35" s="26"/>
-      <c r="O35" s="26"/>
-      <c r="P35" s="26"/>
+      <c r="A35" s="23"/>
+      <c r="B35" s="23"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="23"/>
+      <c r="I35" s="23"/>
+      <c r="J35" s="23"/>
+      <c r="K35" s="23"/>
+      <c r="L35" s="23"/>
+      <c r="M35" s="23"/>
+      <c r="N35" s="23"/>
+      <c r="O35" s="23"/>
+      <c r="P35" s="23"/>
       <c r="Q35" s="8"/>
       <c r="R35" s="8"/>
       <c r="S35" s="8"/>
@@ -6549,8 +6621,60 @@
       <c r="AE35" s="8"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="65">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="A3:L5"/>
+    <mergeCell ref="M3:P5"/>
+    <mergeCell ref="Q3:AE3"/>
+    <mergeCell ref="A7:L7"/>
+    <mergeCell ref="M7:P7"/>
+    <mergeCell ref="A8:L8"/>
+    <mergeCell ref="M8:P8"/>
+    <mergeCell ref="A6:L6"/>
+    <mergeCell ref="M6:P6"/>
+    <mergeCell ref="A9:L9"/>
+    <mergeCell ref="M9:P9"/>
+    <mergeCell ref="A10:L10"/>
+    <mergeCell ref="M10:P10"/>
+    <mergeCell ref="A11:L11"/>
+    <mergeCell ref="M11:P11"/>
+    <mergeCell ref="A12:L12"/>
+    <mergeCell ref="M12:P12"/>
+    <mergeCell ref="A13:L13"/>
+    <mergeCell ref="M13:P13"/>
+    <mergeCell ref="A14:L14"/>
+    <mergeCell ref="M14:P14"/>
+    <mergeCell ref="A15:L15"/>
+    <mergeCell ref="M15:P15"/>
+    <mergeCell ref="A16:L16"/>
+    <mergeCell ref="M16:P16"/>
+    <mergeCell ref="A17:L17"/>
+    <mergeCell ref="M17:P17"/>
+    <mergeCell ref="A18:L18"/>
+    <mergeCell ref="M18:P18"/>
+    <mergeCell ref="A19:L19"/>
+    <mergeCell ref="M19:P19"/>
+    <mergeCell ref="A20:L20"/>
+    <mergeCell ref="M20:P20"/>
+    <mergeCell ref="A21:L21"/>
+    <mergeCell ref="M21:P21"/>
+    <mergeCell ref="A22:L22"/>
+    <mergeCell ref="M22:P22"/>
+    <mergeCell ref="A23:L23"/>
+    <mergeCell ref="M23:P23"/>
+    <mergeCell ref="A24:L24"/>
+    <mergeCell ref="M24:P24"/>
+    <mergeCell ref="A25:L25"/>
+    <mergeCell ref="M25:P25"/>
+    <mergeCell ref="A26:L26"/>
+    <mergeCell ref="M26:P26"/>
+    <mergeCell ref="A27:L27"/>
+    <mergeCell ref="M27:P27"/>
+    <mergeCell ref="A28:L28"/>
+    <mergeCell ref="M28:P28"/>
+    <mergeCell ref="A29:L29"/>
+    <mergeCell ref="M29:P29"/>
     <mergeCell ref="A30:L30"/>
     <mergeCell ref="M30:P30"/>
     <mergeCell ref="A34:L34"/>
@@ -6563,59 +6687,6 @@
     <mergeCell ref="M32:P32"/>
     <mergeCell ref="A33:L33"/>
     <mergeCell ref="M33:P33"/>
-    <mergeCell ref="A27:L27"/>
-    <mergeCell ref="M27:P27"/>
-    <mergeCell ref="A28:L28"/>
-    <mergeCell ref="M28:P28"/>
-    <mergeCell ref="A29:L29"/>
-    <mergeCell ref="M29:P29"/>
-    <mergeCell ref="A24:L24"/>
-    <mergeCell ref="M24:P24"/>
-    <mergeCell ref="A25:L25"/>
-    <mergeCell ref="M25:P25"/>
-    <mergeCell ref="A26:L26"/>
-    <mergeCell ref="M26:P26"/>
-    <mergeCell ref="A21:L21"/>
-    <mergeCell ref="M21:P21"/>
-    <mergeCell ref="A22:L22"/>
-    <mergeCell ref="M22:P22"/>
-    <mergeCell ref="A23:L23"/>
-    <mergeCell ref="M23:P23"/>
-    <mergeCell ref="A18:L18"/>
-    <mergeCell ref="M18:P18"/>
-    <mergeCell ref="A19:L19"/>
-    <mergeCell ref="M19:P19"/>
-    <mergeCell ref="A20:L20"/>
-    <mergeCell ref="M20:P20"/>
-    <mergeCell ref="A15:L15"/>
-    <mergeCell ref="M15:P15"/>
-    <mergeCell ref="A16:L16"/>
-    <mergeCell ref="M16:P16"/>
-    <mergeCell ref="A17:L17"/>
-    <mergeCell ref="M17:P17"/>
-    <mergeCell ref="A12:L12"/>
-    <mergeCell ref="M12:P12"/>
-    <mergeCell ref="A13:L13"/>
-    <mergeCell ref="M13:P13"/>
-    <mergeCell ref="A14:L14"/>
-    <mergeCell ref="M14:P14"/>
-    <mergeCell ref="A9:L9"/>
-    <mergeCell ref="M9:P9"/>
-    <mergeCell ref="A10:L10"/>
-    <mergeCell ref="M10:P10"/>
-    <mergeCell ref="A11:L11"/>
-    <mergeCell ref="M11:P11"/>
-    <mergeCell ref="A7:L7"/>
-    <mergeCell ref="M7:P7"/>
-    <mergeCell ref="A8:L8"/>
-    <mergeCell ref="M8:P8"/>
-    <mergeCell ref="A6:L6"/>
-    <mergeCell ref="M6:P6"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="A3:L5"/>
-    <mergeCell ref="M3:P5"/>
-    <mergeCell ref="Q3:AE3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>